<commit_message>
Add direct NOU forecasting fallback when drivers unavailable (v2.4.0)
</commit_message>
<xml_diff>
--- a/inputs_forecasting.xlsx
+++ b/inputs_forecasting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnachbar\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCD423D-F801-46DE-A804-3A4495F046DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50FC55B-3997-4248-9A71-3AD1D9E07F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{998CAE49-F45B-4B7A-AD02-07A41134BC5C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{998CAE49-F45B-4B7A-AD02-07A41134BC5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Actuals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="229">
   <si>
     <t>Net Ordered Units</t>
   </si>
@@ -719,6 +719,18 @@
   <si>
     <t>Wk19</t>
   </si>
+  <si>
+    <t>8.5MM</t>
+  </si>
+  <si>
+    <t>Pre Update</t>
+  </si>
+  <si>
+    <t>Post Update 20/01/2026</t>
+  </si>
+  <si>
+    <t>7.1MM</t>
+  </si>
 </sst>
 </file>
 
@@ -1226,6 +1238,174 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="7" formatCode="#,##0.00;\-#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="8"/>
         <color theme="1"/>
         <name val="Aptos Narrow"/>
@@ -1900,13 +2080,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
@@ -1941,6 +2114,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2614,342 +2794,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="7" formatCode="#,##0.00;\-#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="7" formatCode="#,##0.00;\-#,##0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF212121"/>
-        <name val="Amazon Ember"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6F6F6"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <sz val="12"/>
         <color rgb="FF212121"/>
         <name val="Amazon Ember"/>
@@ -14435,19 +14279,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -14475,19 +14321,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -14515,19 +14363,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -14555,19 +14405,63 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -17918,6 +17812,48 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -19966,19 +19902,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -20006,19 +19944,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -20046,19 +19986,21 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -20086,19 +20028,63 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="7" formatCode="#,##0.00;\-#,##0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -20727,6 +20713,48 @@
         </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF212121"/>
+        <name val="Amazon Ember"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="5" formatCode="#,##0;\-#,##0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6F6F6"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -24276,66 +24304,66 @@
     <tableColumn id="32" xr3:uid="{91D1815A-3773-4FF3-89DE-B4258A5BFB5F}" name="Wk49 2025" dataDxfId="690"/>
     <tableColumn id="33" xr3:uid="{15CBE303-07BA-4752-A521-E2E4A9065CD7}" name="Wk50 2025" dataDxfId="689"/>
     <tableColumn id="34" xr3:uid="{9B9D648B-C484-48EF-B26D-71801904B26C}" name="Wk51 2025" dataDxfId="688"/>
-    <tableColumn id="35" xr3:uid="{4D1A5032-D184-40E5-9F1C-EDCB20D37C14}" name="Wk52 2025" dataDxfId="74"/>
-    <tableColumn id="36" xr3:uid="{39369CDF-3E8C-4713-8379-436D93E94096}" name="Wk 1 2026" dataDxfId="73"/>
-    <tableColumn id="37" xr3:uid="{99BC60EE-4C69-4919-9429-1FFB73B77CEC}" name="Wk 2 2026" dataDxfId="687"/>
-    <tableColumn id="38" xr3:uid="{38873EAD-C962-4CB7-9E7A-9A9D7C5F765F}" name="Wk 3 2026" dataDxfId="686"/>
-    <tableColumn id="39" xr3:uid="{3D441407-9AA3-417E-9053-10E282CD544C}" name="Wk 4 2026" dataDxfId="685"/>
-    <tableColumn id="40" xr3:uid="{0AC4A2ED-1B2A-46E2-A4CA-FE992578B097}" name="Wk 5 2026" dataDxfId="684"/>
-    <tableColumn id="41" xr3:uid="{CA32406E-AF27-4701-8E98-915FA995785F}" name="Wk 6 2026" dataDxfId="683"/>
-    <tableColumn id="42" xr3:uid="{332C9F85-C82F-49EB-8637-45B6B35C48D1}" name="Wk 7 2026" dataDxfId="682"/>
-    <tableColumn id="43" xr3:uid="{213D3273-48AA-462B-B93F-8D5D2CCC8302}" name="Wk 8 2026" dataDxfId="681"/>
-    <tableColumn id="44" xr3:uid="{3744F9A8-BC1C-43D7-8836-870125445DF7}" name="Wk 9 2026" dataDxfId="680"/>
-    <tableColumn id="45" xr3:uid="{2FFF9FF6-2A3E-44C4-8206-8939F6E78C83}" name="Wk 10 2026" dataDxfId="679"/>
-    <tableColumn id="46" xr3:uid="{0F820EF9-3F16-4474-8408-AE6885369B78}" name="Wk 11 2026" dataDxfId="678"/>
-    <tableColumn id="47" xr3:uid="{AF581808-7A9C-40B9-AFDD-1DA62E93B9DB}" name="Wk 12 2026" dataDxfId="677"/>
-    <tableColumn id="48" xr3:uid="{D39FE1D5-C625-4940-8FFA-89B8871569FC}" name="Wk 13 2026" dataDxfId="676"/>
-    <tableColumn id="49" xr3:uid="{0FF1C889-AC30-4178-A21D-C4583DF67E8D}" name="Wk 14 2026" dataDxfId="675"/>
-    <tableColumn id="50" xr3:uid="{2C355573-FA56-4677-9FDD-E77F4B45A87B}" name="Wk 15 2026" dataDxfId="674"/>
-    <tableColumn id="51" xr3:uid="{77BB5FD6-D0A1-45D5-9A65-30D55F4DE54B}" name="Wk 16 2026" dataDxfId="673"/>
-    <tableColumn id="52" xr3:uid="{1B3951B2-C32F-463B-A647-96F9C4CF5562}" name="Wk 17 2026" dataDxfId="672"/>
-    <tableColumn id="53" xr3:uid="{5BE76B65-7E64-4D9D-9E69-C38477404C4E}" name="Wk 18 2026" dataDxfId="671"/>
-    <tableColumn id="54" xr3:uid="{085429E7-BCEC-4DD4-99A2-3F12A20AD9A2}" name="Wk 19 2026" dataDxfId="670"/>
-    <tableColumn id="55" xr3:uid="{1F704376-277E-46E8-A7B1-51C5E7014BC9}" name="Wk 20 2026" dataDxfId="669"/>
-    <tableColumn id="56" xr3:uid="{3D07B564-E4B3-473B-9EDC-B2354D0367D7}" name="Wk 21 2026" dataDxfId="668"/>
-    <tableColumn id="57" xr3:uid="{6F902361-5171-429A-9ADC-E51613527CC0}" name="Wk 22 2026" dataDxfId="667"/>
-    <tableColumn id="58" xr3:uid="{F15A3C2B-1E39-4838-8C84-89A02705600C}" name="Wk 23 2026" dataDxfId="666"/>
-    <tableColumn id="59" xr3:uid="{796B7618-0FB2-4F1A-A9F9-9BD396DC1666}" name="Wk 24 2026" dataDxfId="665"/>
-    <tableColumn id="60" xr3:uid="{168CCEF6-2F5F-424E-B7B3-D6FBA38A27ED}" name="Wk 25 2026" dataDxfId="664"/>
-    <tableColumn id="61" xr3:uid="{9AB9BC13-2C00-4514-8629-23D9D1CCBEBA}" name="Wk 26 2026" dataDxfId="663"/>
-    <tableColumn id="62" xr3:uid="{EB0BCF33-C994-4014-B7C8-0FFEAAAFAD0D}" name="Wk 27 2026" dataDxfId="662"/>
-    <tableColumn id="63" xr3:uid="{6042F14B-19E7-4326-A922-DF2CF2808630}" name="Wk 28 2026" dataDxfId="661"/>
-    <tableColumn id="64" xr3:uid="{CFAFE7FE-2B0F-46E5-A57D-96BC7350BCD2}" name="Wk 29 2026" dataDxfId="660"/>
-    <tableColumn id="65" xr3:uid="{7110FF7A-F9F1-4C80-9370-E0B2395BB5F4}" name="Wk 30 2026" dataDxfId="659"/>
-    <tableColumn id="66" xr3:uid="{9F64292D-E031-458D-887D-634E87E60EBE}" name="Wk 31 2026" dataDxfId="658"/>
-    <tableColumn id="67" xr3:uid="{BD51B877-32A3-485C-A75B-B9B7C38A0CC3}" name="Wk 32 2026" dataDxfId="657"/>
-    <tableColumn id="68" xr3:uid="{AFE97B97-BFE5-42C8-A71F-8CAB8662EC05}" name="Wk 33 2026" dataDxfId="656"/>
-    <tableColumn id="69" xr3:uid="{E66D79C7-AAF0-44AE-9C32-B3CA12508524}" name="Wk 34 2026" dataDxfId="655"/>
-    <tableColumn id="70" xr3:uid="{12AB30C4-1B7B-405C-92E6-301372E9C5C1}" name="Wk 35 2026" dataDxfId="654"/>
-    <tableColumn id="71" xr3:uid="{794C630B-BF54-4E29-9074-3E1EEDB80B16}" name="Wk 36 2026" dataDxfId="653"/>
-    <tableColumn id="72" xr3:uid="{20043D72-03E6-40C7-A1B8-0C8C2764FAA4}" name="Wk 37 2026" dataDxfId="652"/>
-    <tableColumn id="73" xr3:uid="{C05051C0-DC03-4CAA-B31C-105EE4736B34}" name="Wk 38 2026" dataDxfId="651"/>
-    <tableColumn id="74" xr3:uid="{A60CC0EC-2C84-4830-98D0-2BF9274FB02D}" name="Wk 39 2026" dataDxfId="650"/>
-    <tableColumn id="75" xr3:uid="{3670D0DC-9CEB-4E08-BC6B-B36559ED86DD}" name="Wk 40 2026" dataDxfId="649"/>
-    <tableColumn id="76" xr3:uid="{1C8869A9-BDB7-4C7A-A4EA-B78A877AC9C5}" name="Wk 41 2026" dataDxfId="648"/>
-    <tableColumn id="77" xr3:uid="{EB373CDE-40AA-46AD-B2D3-F1204A0D3E73}" name="Wk 42 2026" dataDxfId="647"/>
-    <tableColumn id="78" xr3:uid="{75C8AE7C-6871-475F-AEE0-5E515905A257}" name="Wk 43 2026" dataDxfId="646"/>
-    <tableColumn id="79" xr3:uid="{4874C6D8-199C-41D0-BBFD-A348B935E4AD}" name="Wk 44 2026" dataDxfId="645"/>
-    <tableColumn id="80" xr3:uid="{C003F127-10EE-4777-A03B-23EDF79989C0}" name="Wk 45 2026" dataDxfId="644"/>
-    <tableColumn id="81" xr3:uid="{BACD9D11-A9DE-467E-9BF3-8CA8207B8993}" name="Wk 46 2026" dataDxfId="643"/>
-    <tableColumn id="82" xr3:uid="{BFF349F6-BA1C-482C-8A88-4E5F662BF0FD}" name="Wk 47 2026" dataDxfId="642"/>
-    <tableColumn id="83" xr3:uid="{095D7966-D93A-460E-92F4-1BB9A892A198}" name="Wk 48 2026" dataDxfId="641"/>
-    <tableColumn id="84" xr3:uid="{98717447-9B93-4D62-8E60-49AF4B204795}" name="Wk 49 2026" dataDxfId="640"/>
-    <tableColumn id="85" xr3:uid="{F3BC61BC-00FB-4FAD-B795-0579D6E3B9E9}" name="Wk 50 2026" dataDxfId="639"/>
-    <tableColumn id="86" xr3:uid="{14DA971D-7FB8-4423-B6D7-F547DC785CA5}" name="Wk 51 2026" dataDxfId="638"/>
-    <tableColumn id="87" xr3:uid="{4C7541F1-6DF0-4936-BCFE-94877B51417C}" name="Wk 52 2026" dataDxfId="637"/>
+    <tableColumn id="35" xr3:uid="{4D1A5032-D184-40E5-9F1C-EDCB20D37C14}" name="Wk52 2025" dataDxfId="687"/>
+    <tableColumn id="36" xr3:uid="{39369CDF-3E8C-4713-8379-436D93E94096}" name="Wk 1 2026" dataDxfId="686"/>
+    <tableColumn id="37" xr3:uid="{99BC60EE-4C69-4919-9429-1FFB73B77CEC}" name="Wk 2 2026" dataDxfId="685"/>
+    <tableColumn id="38" xr3:uid="{38873EAD-C962-4CB7-9E7A-9A9D7C5F765F}" name="Wk 3 2026" dataDxfId="684"/>
+    <tableColumn id="39" xr3:uid="{3D441407-9AA3-417E-9053-10E282CD544C}" name="Wk 4 2026" dataDxfId="683"/>
+    <tableColumn id="40" xr3:uid="{0AC4A2ED-1B2A-46E2-A4CA-FE992578B097}" name="Wk 5 2026" dataDxfId="3"/>
+    <tableColumn id="41" xr3:uid="{CA32406E-AF27-4701-8E98-915FA995785F}" name="Wk 6 2026" dataDxfId="682"/>
+    <tableColumn id="42" xr3:uid="{332C9F85-C82F-49EB-8637-45B6B35C48D1}" name="Wk 7 2026" dataDxfId="681"/>
+    <tableColumn id="43" xr3:uid="{213D3273-48AA-462B-B93F-8D5D2CCC8302}" name="Wk 8 2026" dataDxfId="680"/>
+    <tableColumn id="44" xr3:uid="{3744F9A8-BC1C-43D7-8836-870125445DF7}" name="Wk 9 2026" dataDxfId="679"/>
+    <tableColumn id="45" xr3:uid="{2FFF9FF6-2A3E-44C4-8206-8939F6E78C83}" name="Wk 10 2026" dataDxfId="678"/>
+    <tableColumn id="46" xr3:uid="{0F820EF9-3F16-4474-8408-AE6885369B78}" name="Wk 11 2026" dataDxfId="677"/>
+    <tableColumn id="47" xr3:uid="{AF581808-7A9C-40B9-AFDD-1DA62E93B9DB}" name="Wk 12 2026" dataDxfId="676"/>
+    <tableColumn id="48" xr3:uid="{D39FE1D5-C625-4940-8FFA-89B8871569FC}" name="Wk 13 2026" dataDxfId="675"/>
+    <tableColumn id="49" xr3:uid="{0FF1C889-AC30-4178-A21D-C4583DF67E8D}" name="Wk 14 2026" dataDxfId="674"/>
+    <tableColumn id="50" xr3:uid="{2C355573-FA56-4677-9FDD-E77F4B45A87B}" name="Wk 15 2026" dataDxfId="673"/>
+    <tableColumn id="51" xr3:uid="{77BB5FD6-D0A1-45D5-9A65-30D55F4DE54B}" name="Wk 16 2026" dataDxfId="672"/>
+    <tableColumn id="52" xr3:uid="{1B3951B2-C32F-463B-A647-96F9C4CF5562}" name="Wk 17 2026" dataDxfId="671"/>
+    <tableColumn id="53" xr3:uid="{5BE76B65-7E64-4D9D-9E69-C38477404C4E}" name="Wk 18 2026" dataDxfId="670"/>
+    <tableColumn id="54" xr3:uid="{085429E7-BCEC-4DD4-99A2-3F12A20AD9A2}" name="Wk 19 2026" dataDxfId="669"/>
+    <tableColumn id="55" xr3:uid="{1F704376-277E-46E8-A7B1-51C5E7014BC9}" name="Wk 20 2026" dataDxfId="668"/>
+    <tableColumn id="56" xr3:uid="{3D07B564-E4B3-473B-9EDC-B2354D0367D7}" name="Wk 21 2026" dataDxfId="667"/>
+    <tableColumn id="57" xr3:uid="{6F902361-5171-429A-9ADC-E51613527CC0}" name="Wk 22 2026" dataDxfId="666"/>
+    <tableColumn id="58" xr3:uid="{F15A3C2B-1E39-4838-8C84-89A02705600C}" name="Wk 23 2026" dataDxfId="665"/>
+    <tableColumn id="59" xr3:uid="{796B7618-0FB2-4F1A-A9F9-9BD396DC1666}" name="Wk 24 2026" dataDxfId="664"/>
+    <tableColumn id="60" xr3:uid="{168CCEF6-2F5F-424E-B7B3-D6FBA38A27ED}" name="Wk 25 2026" dataDxfId="663"/>
+    <tableColumn id="61" xr3:uid="{9AB9BC13-2C00-4514-8629-23D9D1CCBEBA}" name="Wk 26 2026" dataDxfId="662"/>
+    <tableColumn id="62" xr3:uid="{EB0BCF33-C994-4014-B7C8-0FFEAAAFAD0D}" name="Wk 27 2026" dataDxfId="661"/>
+    <tableColumn id="63" xr3:uid="{6042F14B-19E7-4326-A922-DF2CF2808630}" name="Wk 28 2026" dataDxfId="660"/>
+    <tableColumn id="64" xr3:uid="{CFAFE7FE-2B0F-46E5-A57D-96BC7350BCD2}" name="Wk 29 2026" dataDxfId="659"/>
+    <tableColumn id="65" xr3:uid="{7110FF7A-F9F1-4C80-9370-E0B2395BB5F4}" name="Wk 30 2026" dataDxfId="658"/>
+    <tableColumn id="66" xr3:uid="{9F64292D-E031-458D-887D-634E87E60EBE}" name="Wk 31 2026" dataDxfId="657"/>
+    <tableColumn id="67" xr3:uid="{BD51B877-32A3-485C-A75B-B9B7C38A0CC3}" name="Wk 32 2026" dataDxfId="656"/>
+    <tableColumn id="68" xr3:uid="{AFE97B97-BFE5-42C8-A71F-8CAB8662EC05}" name="Wk 33 2026" dataDxfId="655"/>
+    <tableColumn id="69" xr3:uid="{E66D79C7-AAF0-44AE-9C32-B3CA12508524}" name="Wk 34 2026" dataDxfId="654"/>
+    <tableColumn id="70" xr3:uid="{12AB30C4-1B7B-405C-92E6-301372E9C5C1}" name="Wk 35 2026" dataDxfId="653"/>
+    <tableColumn id="71" xr3:uid="{794C630B-BF54-4E29-9074-3E1EEDB80B16}" name="Wk 36 2026" dataDxfId="652"/>
+    <tableColumn id="72" xr3:uid="{20043D72-03E6-40C7-A1B8-0C8C2764FAA4}" name="Wk 37 2026" dataDxfId="651"/>
+    <tableColumn id="73" xr3:uid="{C05051C0-DC03-4CAA-B31C-105EE4736B34}" name="Wk 38 2026" dataDxfId="650"/>
+    <tableColumn id="74" xr3:uid="{A60CC0EC-2C84-4830-98D0-2BF9274FB02D}" name="Wk 39 2026" dataDxfId="649"/>
+    <tableColumn id="75" xr3:uid="{3670D0DC-9CEB-4E08-BC6B-B36559ED86DD}" name="Wk 40 2026" dataDxfId="648"/>
+    <tableColumn id="76" xr3:uid="{1C8869A9-BDB7-4C7A-A4EA-B78A877AC9C5}" name="Wk 41 2026" dataDxfId="647"/>
+    <tableColumn id="77" xr3:uid="{EB373CDE-40AA-46AD-B2D3-F1204A0D3E73}" name="Wk 42 2026" dataDxfId="646"/>
+    <tableColumn id="78" xr3:uid="{75C8AE7C-6871-475F-AEE0-5E515905A257}" name="Wk 43 2026" dataDxfId="645"/>
+    <tableColumn id="79" xr3:uid="{4874C6D8-199C-41D0-BBFD-A348B935E4AD}" name="Wk 44 2026" dataDxfId="644"/>
+    <tableColumn id="80" xr3:uid="{C003F127-10EE-4777-A03B-23EDF79989C0}" name="Wk 45 2026" dataDxfId="643"/>
+    <tableColumn id="81" xr3:uid="{BACD9D11-A9DE-467E-9BF3-8CA8207B8993}" name="Wk 46 2026" dataDxfId="642"/>
+    <tableColumn id="82" xr3:uid="{BFF349F6-BA1C-482C-8A88-4E5F662BF0FD}" name="Wk 47 2026" dataDxfId="641"/>
+    <tableColumn id="83" xr3:uid="{095D7966-D93A-460E-92F4-1BB9A892A198}" name="Wk 48 2026" dataDxfId="640"/>
+    <tableColumn id="84" xr3:uid="{98717447-9B93-4D62-8E60-49AF4B204795}" name="Wk 49 2026" dataDxfId="639"/>
+    <tableColumn id="85" xr3:uid="{F3BC61BC-00FB-4FAD-B795-0579D6E3B9E9}" name="Wk 50 2026" dataDxfId="638"/>
+    <tableColumn id="86" xr3:uid="{14DA971D-7FB8-4423-B6D7-F547DC785CA5}" name="Wk 51 2026" dataDxfId="637"/>
+    <tableColumn id="87" xr3:uid="{4C7541F1-6DF0-4936-BCFE-94877B51417C}" name="Wk 52 2026" dataDxfId="636"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{280500AC-8287-40F9-99B8-C34FA90C2943}" name="Table1921" displayName="Table1921" ref="B11:AP16" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{280500AC-8287-40F9-99B8-C34FA90C2943}" name="Table1921" displayName="Table1921" ref="B11:AP16" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
   <autoFilter ref="B11:AP16" xr:uid="{1BD251F5-8623-4198-AAA7-C32AAE2AA806}"/>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{28877711-7FD6-46F6-8CBB-301B6FAA434E}" name="WK"/>
@@ -24360,25 +24388,25 @@
     <tableColumn id="20" xr3:uid="{189E1433-768F-4EEA-A41F-0534AFCAC358}" name="37"/>
     <tableColumn id="21" xr3:uid="{937FCC2E-87EF-4463-BB3B-1A51D4AC71E1}" name="38"/>
     <tableColumn id="22" xr3:uid="{0F8CEBF1-21F2-41EE-BE63-4DEB07F874FF}" name="39"/>
-    <tableColumn id="23" xr3:uid="{E792172F-C74A-4B21-B2E1-CE0C380D961A}" name="40" dataDxfId="18"/>
-    <tableColumn id="24" xr3:uid="{607EAB0B-0BBA-458C-AEF0-AC68D3968611}" name="41" dataDxfId="17"/>
-    <tableColumn id="25" xr3:uid="{1656626F-90A9-4CE2-A10E-B170D48B45EC}" name="42" dataDxfId="16"/>
-    <tableColumn id="26" xr3:uid="{0318A981-37F6-4449-B3A0-3AB5624AABDB}" name="43" dataDxfId="15"/>
-    <tableColumn id="27" xr3:uid="{B834AE61-9100-4459-8593-C6B72DC25E5A}" name="44" dataDxfId="14"/>
-    <tableColumn id="28" xr3:uid="{AAE27087-FE27-4261-B3AD-928F1045310E}" name="45" dataDxfId="13"/>
-    <tableColumn id="29" xr3:uid="{A0503AA2-F304-4050-AC77-E400C799F4E4}" name="46" dataDxfId="12"/>
-    <tableColumn id="30" xr3:uid="{7799DDB3-9D34-41CD-B0CB-E4E55C954FA9}" name="47" dataDxfId="11"/>
-    <tableColumn id="31" xr3:uid="{897038A7-829C-4E1C-A1F2-F9606D65951C}" name="48" dataDxfId="10"/>
-    <tableColumn id="32" xr3:uid="{F1FB296C-1D03-40AC-99CB-E90A259CEF76}" name="49" dataDxfId="9"/>
-    <tableColumn id="33" xr3:uid="{2543D89E-1357-48EB-AD66-34155DB50737}" name="50" dataDxfId="8"/>
-    <tableColumn id="34" xr3:uid="{E026D650-F7CB-41CE-BB07-549F3F000119}" name="51" dataDxfId="7"/>
-    <tableColumn id="35" xr3:uid="{D495A235-5DC4-42BC-B3E8-3F60C6C31431}" name="52" dataDxfId="6"/>
-    <tableColumn id="36" xr3:uid="{653DA1B9-1FE2-4D5C-89A9-476004BF553C}" name="1" dataDxfId="5"/>
-    <tableColumn id="37" xr3:uid="{A11409CF-D2F4-4F93-9EAC-9FD06BC01D2E}" name="2" dataDxfId="4"/>
-    <tableColumn id="38" xr3:uid="{D6748703-2A69-4DFE-8B00-9A3A3FD0B3D7}" name="3" dataDxfId="3"/>
-    <tableColumn id="39" xr3:uid="{DC9987F7-3761-4800-84D1-AEDAD159CCA0}" name="56" dataDxfId="2"/>
-    <tableColumn id="40" xr3:uid="{7297D95A-3C32-490A-B524-27A2D06B683B}" name="57" dataDxfId="1"/>
-    <tableColumn id="41" xr3:uid="{0AE2052C-FF22-45AE-AAAD-E7CC0AE6777E}" name="58" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{E792172F-C74A-4B21-B2E1-CE0C380D961A}" name="40" dataDxfId="22"/>
+    <tableColumn id="24" xr3:uid="{607EAB0B-0BBA-458C-AEF0-AC68D3968611}" name="41" dataDxfId="21"/>
+    <tableColumn id="25" xr3:uid="{1656626F-90A9-4CE2-A10E-B170D48B45EC}" name="42" dataDxfId="20"/>
+    <tableColumn id="26" xr3:uid="{0318A981-37F6-4449-B3A0-3AB5624AABDB}" name="43" dataDxfId="19"/>
+    <tableColumn id="27" xr3:uid="{B834AE61-9100-4459-8593-C6B72DC25E5A}" name="44" dataDxfId="18"/>
+    <tableColumn id="28" xr3:uid="{AAE27087-FE27-4261-B3AD-928F1045310E}" name="45" dataDxfId="17"/>
+    <tableColumn id="29" xr3:uid="{A0503AA2-F304-4050-AC77-E400C799F4E4}" name="46" dataDxfId="16"/>
+    <tableColumn id="30" xr3:uid="{7799DDB3-9D34-41CD-B0CB-E4E55C954FA9}" name="47" dataDxfId="15"/>
+    <tableColumn id="31" xr3:uid="{897038A7-829C-4E1C-A1F2-F9606D65951C}" name="48" dataDxfId="14"/>
+    <tableColumn id="32" xr3:uid="{F1FB296C-1D03-40AC-99CB-E90A259CEF76}" name="49" dataDxfId="13"/>
+    <tableColumn id="33" xr3:uid="{2543D89E-1357-48EB-AD66-34155DB50737}" name="50" dataDxfId="12"/>
+    <tableColumn id="34" xr3:uid="{E026D650-F7CB-41CE-BB07-549F3F000119}" name="51" dataDxfId="11"/>
+    <tableColumn id="35" xr3:uid="{D495A235-5DC4-42BC-B3E8-3F60C6C31431}" name="52" dataDxfId="10"/>
+    <tableColumn id="36" xr3:uid="{653DA1B9-1FE2-4D5C-89A9-476004BF553C}" name="1" dataDxfId="9"/>
+    <tableColumn id="37" xr3:uid="{A11409CF-D2F4-4F93-9EAC-9FD06BC01D2E}" name="2" dataDxfId="8"/>
+    <tableColumn id="38" xr3:uid="{D6748703-2A69-4DFE-8B00-9A3A3FD0B3D7}" name="3" dataDxfId="7"/>
+    <tableColumn id="39" xr3:uid="{DC9987F7-3761-4800-84D1-AEDAD159CCA0}" name="56" dataDxfId="6"/>
+    <tableColumn id="40" xr3:uid="{7297D95A-3C32-490A-B524-27A2D06B683B}" name="57" dataDxfId="5"/>
+    <tableColumn id="41" xr3:uid="{0AE2052C-FF22-45AE-AAAD-E7CC0AE6777E}" name="58" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24388,12 +24416,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCB9719C-E9A5-476C-A8B2-16DBE2BE55E6}" name="tblActualsUPO" displayName="tblActualsUPO" ref="B31:CJ37" totalsRowShown="0">
   <autoFilter ref="B31:CJ37" xr:uid="{DCB9719C-E9A5-476C-A8B2-16DBE2BE55E6}"/>
   <tableColumns count="87">
-    <tableColumn id="1" xr3:uid="{FF5E1F4C-B7F8-47C5-BB8B-86B31578F303}" name="MP" dataDxfId="636"/>
-    <tableColumn id="2" xr3:uid="{4F472AEB-857D-4C0B-9856-F73FF5174282}" name="Wk19 2025" dataDxfId="635"/>
-    <tableColumn id="3" xr3:uid="{6C36287B-5588-4F2D-BD12-BF5023D934F2}" name="Wk20 2025" dataDxfId="634"/>
-    <tableColumn id="4" xr3:uid="{01EE9C39-8977-4EEE-81E1-8826EE50047C}" name="Wk21 2025" dataDxfId="633"/>
-    <tableColumn id="5" xr3:uid="{4B23CD96-D4E0-4EB6-AF0B-5E03B0AF2D19}" name="Wk22 2025" dataDxfId="632"/>
-    <tableColumn id="6" xr3:uid="{C5CF90B9-2677-4016-8AAF-D01EE9DC1FA1}" name="Wk23 2025" dataDxfId="631"/>
+    <tableColumn id="1" xr3:uid="{FF5E1F4C-B7F8-47C5-BB8B-86B31578F303}" name="MP" dataDxfId="635"/>
+    <tableColumn id="2" xr3:uid="{4F472AEB-857D-4C0B-9856-F73FF5174282}" name="Wk19 2025" dataDxfId="634"/>
+    <tableColumn id="3" xr3:uid="{6C36287B-5588-4F2D-BD12-BF5023D934F2}" name="Wk20 2025" dataDxfId="633"/>
+    <tableColumn id="4" xr3:uid="{01EE9C39-8977-4EEE-81E1-8826EE50047C}" name="Wk21 2025" dataDxfId="632"/>
+    <tableColumn id="5" xr3:uid="{4B23CD96-D4E0-4EB6-AF0B-5E03B0AF2D19}" name="Wk22 2025" dataDxfId="631"/>
+    <tableColumn id="6" xr3:uid="{C5CF90B9-2677-4016-8AAF-D01EE9DC1FA1}" name="Wk23 2025" dataDxfId="630"/>
     <tableColumn id="7" xr3:uid="{64367572-7EAE-4264-A73B-B37563FEFDC0}" name="Wk24 2025"/>
     <tableColumn id="8" xr3:uid="{24219946-26D7-4713-800C-8A55F706C073}" name="Wk25 2025"/>
     <tableColumn id="9" xr3:uid="{1622252A-4FF9-432D-914F-489274CEC7C0}" name="Wk26 2025"/>
@@ -24409,76 +24437,76 @@
     <tableColumn id="19" xr3:uid="{D7C7A4F2-3A93-4516-ABED-6AE5E9CCE555}" name="Wk36 2025"/>
     <tableColumn id="20" xr3:uid="{E612321C-F9E7-42A8-AA7D-503CF5CE3003}" name="Wk37 2025"/>
     <tableColumn id="21" xr3:uid="{4D84044A-01AA-4DAF-9C30-6369D7769118}" name="Wk38 2025"/>
-    <tableColumn id="22" xr3:uid="{C575DE89-C32F-4C99-BEC1-65B6EDD3FB9E}" name="Wk39 2025" dataDxfId="630"/>
-    <tableColumn id="23" xr3:uid="{1B07D814-ED19-480B-BCF5-911ADD551C2E}" name="Wk40 2025" dataDxfId="629"/>
-    <tableColumn id="24" xr3:uid="{73BBCA00-89AF-4E98-8B54-56D3D273BC7D}" name="Wk41 2025" dataDxfId="628"/>
-    <tableColumn id="25" xr3:uid="{EFBAF190-93B0-4DBA-B029-746AF2A4F0CE}" name="Wk42 2025" dataDxfId="627"/>
-    <tableColumn id="26" xr3:uid="{CF028B4D-CA2E-4D85-A7DE-4F3C087025DF}" name="Wk43 2025" dataDxfId="626"/>
-    <tableColumn id="27" xr3:uid="{6B89BD83-6622-49D1-B0FE-E022771397A1}" name="Wk44 2025" dataDxfId="625"/>
-    <tableColumn id="28" xr3:uid="{A0D36DCA-3536-4368-A837-2F481787E4EC}" name="Wk45 2025" dataDxfId="624"/>
-    <tableColumn id="29" xr3:uid="{AE09007D-55DC-4C9B-AE1D-54FFEB62EEA8}" name="Wk46 2025" dataDxfId="623"/>
-    <tableColumn id="30" xr3:uid="{202B3FBC-4012-4B29-AF7F-0BCCD3531978}" name="Wk47 2025" dataDxfId="622">
+    <tableColumn id="22" xr3:uid="{C575DE89-C32F-4C99-BEC1-65B6EDD3FB9E}" name="Wk39 2025" dataDxfId="629"/>
+    <tableColumn id="23" xr3:uid="{1B07D814-ED19-480B-BCF5-911ADD551C2E}" name="Wk40 2025" dataDxfId="628"/>
+    <tableColumn id="24" xr3:uid="{73BBCA00-89AF-4E98-8B54-56D3D273BC7D}" name="Wk41 2025" dataDxfId="627"/>
+    <tableColumn id="25" xr3:uid="{EFBAF190-93B0-4DBA-B029-746AF2A4F0CE}" name="Wk42 2025" dataDxfId="626"/>
+    <tableColumn id="26" xr3:uid="{CF028B4D-CA2E-4D85-A7DE-4F3C087025DF}" name="Wk43 2025" dataDxfId="625"/>
+    <tableColumn id="27" xr3:uid="{6B89BD83-6622-49D1-B0FE-E022771397A1}" name="Wk44 2025" dataDxfId="624"/>
+    <tableColumn id="28" xr3:uid="{A0D36DCA-3536-4368-A837-2F481787E4EC}" name="Wk45 2025" dataDxfId="623"/>
+    <tableColumn id="29" xr3:uid="{AE09007D-55DC-4C9B-AE1D-54FFEB62EEA8}" name="Wk46 2025" dataDxfId="622"/>
+    <tableColumn id="30" xr3:uid="{202B3FBC-4012-4B29-AF7F-0BCCD3531978}" name="Wk47 2025" dataDxfId="621">
       <calculatedColumnFormula>AE3/(AE13*AE22)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{56F75F79-F9C0-497D-9020-C9FB0026AEB5}" name="Wk48 2025" dataDxfId="621"/>
-    <tableColumn id="32" xr3:uid="{76830D05-4C1D-4BDC-965E-AC93F1E7F0BB}" name="Wk49 2025" dataDxfId="620"/>
-    <tableColumn id="33" xr3:uid="{8F3BFDF1-7BD4-42E8-95B0-30C9B3EC8EB4}" name="Wk50 2025" dataDxfId="619">
+    <tableColumn id="31" xr3:uid="{56F75F79-F9C0-497D-9020-C9FB0026AEB5}" name="Wk48 2025" dataDxfId="620"/>
+    <tableColumn id="32" xr3:uid="{76830D05-4C1D-4BDC-965E-AC93F1E7F0BB}" name="Wk49 2025" dataDxfId="619"/>
+    <tableColumn id="33" xr3:uid="{8F3BFDF1-7BD4-42E8-95B0-30C9B3EC8EB4}" name="Wk50 2025" dataDxfId="618">
       <calculatedColumnFormula>AH3/(AH13*AH22)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{774785ED-8276-49C5-AD41-6A28486BF53E}" name="Wk51 2025" dataDxfId="618"/>
-    <tableColumn id="35" xr3:uid="{BD3E70B8-EF41-4D46-9CC3-6F40B3099B99}" name="Wk52 2025" dataDxfId="68"/>
-    <tableColumn id="36" xr3:uid="{167CF893-BA54-4B40-BC61-486C043E894F}" name="Wk 1 2026" dataDxfId="67"/>
-    <tableColumn id="37" xr3:uid="{FF999AEB-49A8-450C-A6FF-9FA78911CAB4}" name="Wk 2 2026" dataDxfId="617"/>
-    <tableColumn id="38" xr3:uid="{6FCD178F-467D-4D56-99E7-D09F0CB8DEBA}" name="Wk 3 2026" dataDxfId="616"/>
-    <tableColumn id="39" xr3:uid="{6DEAC9EA-1E3B-4E94-936A-66C0D0C5D383}" name="Wk 4 2026" dataDxfId="615"/>
-    <tableColumn id="40" xr3:uid="{428990F6-E2C6-4D56-8CE4-93D99AF0DFBE}" name="Wk 5 2026" dataDxfId="614"/>
-    <tableColumn id="41" xr3:uid="{08EB2A31-D296-462F-A62D-BC5780568B10}" name="Wk 6 2026" dataDxfId="613"/>
-    <tableColumn id="42" xr3:uid="{82F95084-04E9-4564-852F-392779661E26}" name="Wk 7 2026" dataDxfId="612"/>
-    <tableColumn id="43" xr3:uid="{FA8A8216-7F1B-4286-8B28-4A1A76A0591C}" name="Wk 8 2026" dataDxfId="611"/>
-    <tableColumn id="44" xr3:uid="{0AC662FD-A750-4B07-9FA1-C0A56834D63C}" name="Wk 9 2026" dataDxfId="610"/>
-    <tableColumn id="45" xr3:uid="{D356147E-91B3-4FE6-8902-80DE5E506356}" name="Wk 10 2026" dataDxfId="609"/>
-    <tableColumn id="46" xr3:uid="{20F85B83-DD6D-4BD3-B9C5-6719520A2EE0}" name="Wk 11 2026" dataDxfId="608"/>
-    <tableColumn id="47" xr3:uid="{A2E896C3-648A-46D8-A60D-2F61164AE4D4}" name="Wk 12 2026" dataDxfId="607"/>
-    <tableColumn id="48" xr3:uid="{D2EE3864-47AF-47B8-A5B9-60043814D83B}" name="Wk 13 2026" dataDxfId="606"/>
-    <tableColumn id="49" xr3:uid="{3167537E-6E32-4EB2-886C-DF7B752427AD}" name="Wk 14 2026" dataDxfId="605"/>
-    <tableColumn id="50" xr3:uid="{FC861F37-0681-4883-BB56-051E14737063}" name="Wk 15 2026" dataDxfId="604"/>
-    <tableColumn id="51" xr3:uid="{71CE2DF8-303C-45BD-AA22-D1D58C5280AB}" name="Wk 16 2026" dataDxfId="603"/>
-    <tableColumn id="52" xr3:uid="{43D7A940-505E-4C88-A628-6E0EA042D0E3}" name="Wk 17 2026" dataDxfId="602"/>
-    <tableColumn id="53" xr3:uid="{8D7359CD-16CB-4005-AE4E-2F17127175BF}" name="Wk 18 2026" dataDxfId="601"/>
-    <tableColumn id="54" xr3:uid="{C2DF5A20-F9A8-4F4D-9E99-4D01760D21C4}" name="Wk 19 2026" dataDxfId="600"/>
-    <tableColumn id="55" xr3:uid="{96CA90C3-2763-4B8E-B42D-89C55FE5B616}" name="Wk 20 2026" dataDxfId="599"/>
-    <tableColumn id="56" xr3:uid="{F8362AE6-018F-4A08-B091-8B83805F4BB2}" name="Wk 21 2026" dataDxfId="598"/>
-    <tableColumn id="57" xr3:uid="{45992418-70A6-4DCD-A32C-1D63AA49A4D8}" name="Wk 22 2026" dataDxfId="597"/>
-    <tableColumn id="58" xr3:uid="{1B7D0E7A-E049-479A-9080-9FDFB57FC0CA}" name="Wk 23 2026" dataDxfId="596"/>
-    <tableColumn id="59" xr3:uid="{E95BFF68-C21B-49FD-B2DA-15EE93B58EAA}" name="Wk 24 2026" dataDxfId="595"/>
-    <tableColumn id="60" xr3:uid="{ECF0F9BF-7920-419B-B2CF-F09E730FF878}" name="Wk 25 2026" dataDxfId="594"/>
-    <tableColumn id="61" xr3:uid="{5DA71C02-37E7-4396-A1B7-FF70D24CDE19}" name="Wk 26 2026" dataDxfId="593"/>
-    <tableColumn id="62" xr3:uid="{F9A5F33B-D2C0-455B-A34B-8EFDFD6C8C53}" name="Wk 27 2026" dataDxfId="592"/>
-    <tableColumn id="63" xr3:uid="{D4CD628A-4312-4FB1-995A-60E50CBDC427}" name="Wk 28 2026" dataDxfId="591"/>
-    <tableColumn id="64" xr3:uid="{CB6C362B-F773-41B2-A29C-FE9E91160619}" name="Wk 29 2026" dataDxfId="590"/>
-    <tableColumn id="65" xr3:uid="{056BC328-B98D-4D28-958C-77D46F881CB2}" name="Wk 30 2026" dataDxfId="589"/>
-    <tableColumn id="66" xr3:uid="{017E8A3B-C1CB-4DBE-B7CF-6205BE4DCDB2}" name="Wk 31 2026" dataDxfId="588"/>
-    <tableColumn id="67" xr3:uid="{1CE38079-6A49-4EDC-9CC9-30C350F40A7A}" name="Wk 32 2026" dataDxfId="587"/>
-    <tableColumn id="68" xr3:uid="{D267527A-B4F7-4FD7-A909-D77BFB9C4BFE}" name="Wk 33 2026" dataDxfId="586"/>
-    <tableColumn id="69" xr3:uid="{FBC52664-8D0E-40AC-8DE4-AEA565D8FAAD}" name="Wk 34 2026" dataDxfId="585"/>
-    <tableColumn id="70" xr3:uid="{BEEBB6E6-7DF6-4419-8EDA-37A3969DB9C0}" name="Wk 35 2026" dataDxfId="584"/>
-    <tableColumn id="71" xr3:uid="{7F513271-0C3A-441B-A2BF-AEFC48D33362}" name="Wk 36 2026" dataDxfId="583"/>
-    <tableColumn id="72" xr3:uid="{4A3C3440-7ED7-4C43-92CA-BA6E7289B8BF}" name="Wk 37 2026" dataDxfId="582"/>
-    <tableColumn id="73" xr3:uid="{1F1D81D8-3E1D-48E7-A4D7-F1354773D8FD}" name="Wk 38 2026" dataDxfId="581"/>
-    <tableColumn id="74" xr3:uid="{E238D3F0-F210-44E2-A00F-BC7CB7A3023B}" name="Wk 39 2026" dataDxfId="580"/>
-    <tableColumn id="75" xr3:uid="{F723C8D0-D8C1-42E1-BD33-E046191D32FC}" name="Wk 40 2026" dataDxfId="579"/>
-    <tableColumn id="76" xr3:uid="{6B5AD89D-E0AB-4AAE-A980-119A8B92E3B6}" name="Wk 41 2026" dataDxfId="578"/>
-    <tableColumn id="77" xr3:uid="{B3DFB992-C284-480B-A932-68F1E3BAA1F1}" name="Wk 42 2026" dataDxfId="577"/>
-    <tableColumn id="78" xr3:uid="{AF8D3D15-C719-41F6-A7B3-49DC7942AEBA}" name="Wk 43 2026" dataDxfId="576"/>
-    <tableColumn id="79" xr3:uid="{53F8DB87-1D36-4550-8E4A-254AFAFA3339}" name="Wk 44 2026" dataDxfId="575"/>
-    <tableColumn id="80" xr3:uid="{43B071E7-D7BF-4B02-8D7B-C324F1E62544}" name="Wk 45 2026" dataDxfId="574"/>
-    <tableColumn id="81" xr3:uid="{6D73DCF7-69D1-44D6-BE42-2644FC05A976}" name="Wk 46 2026" dataDxfId="573"/>
-    <tableColumn id="82" xr3:uid="{407A00F3-B635-4B5C-B192-07496436E40B}" name="Wk 47 2026" dataDxfId="572"/>
-    <tableColumn id="83" xr3:uid="{A84AA1C8-5D88-4E2D-95CE-9E3A10456C9C}" name="Wk 48 2026" dataDxfId="571"/>
-    <tableColumn id="84" xr3:uid="{23F810B7-D1C3-4A18-9C25-1C19D01CF258}" name="Wk 49 2026" dataDxfId="570"/>
-    <tableColumn id="85" xr3:uid="{5C2AB52B-D93A-4447-81C5-CBA70222893C}" name="Wk 50 2026" dataDxfId="569"/>
-    <tableColumn id="86" xr3:uid="{22AFCD3C-D466-4832-828D-19411BAA244C}" name="Wk 51 2026" dataDxfId="568"/>
-    <tableColumn id="87" xr3:uid="{0261B616-7060-407D-8580-0BF44181D661}" name="Wk 52 2026" dataDxfId="567"/>
+    <tableColumn id="34" xr3:uid="{774785ED-8276-49C5-AD41-6A28486BF53E}" name="Wk51 2025" dataDxfId="617"/>
+    <tableColumn id="35" xr3:uid="{BD3E70B8-EF41-4D46-9CC3-6F40B3099B99}" name="Wk52 2025" dataDxfId="616"/>
+    <tableColumn id="36" xr3:uid="{167CF893-BA54-4B40-BC61-486C043E894F}" name="Wk 1 2026" dataDxfId="615"/>
+    <tableColumn id="37" xr3:uid="{FF999AEB-49A8-450C-A6FF-9FA78911CAB4}" name="Wk 2 2026" dataDxfId="614"/>
+    <tableColumn id="38" xr3:uid="{6FCD178F-467D-4D56-99E7-D09F0CB8DEBA}" name="Wk 3 2026" dataDxfId="613"/>
+    <tableColumn id="39" xr3:uid="{6DEAC9EA-1E3B-4E94-936A-66C0D0C5D383}" name="Wk 4 2026" dataDxfId="612"/>
+    <tableColumn id="40" xr3:uid="{428990F6-E2C6-4D56-8CE4-93D99AF0DFBE}" name="Wk 5 2026" dataDxfId="0"/>
+    <tableColumn id="41" xr3:uid="{08EB2A31-D296-462F-A62D-BC5780568B10}" name="Wk 6 2026" dataDxfId="611"/>
+    <tableColumn id="42" xr3:uid="{82F95084-04E9-4564-852F-392779661E26}" name="Wk 7 2026" dataDxfId="610"/>
+    <tableColumn id="43" xr3:uid="{FA8A8216-7F1B-4286-8B28-4A1A76A0591C}" name="Wk 8 2026" dataDxfId="609"/>
+    <tableColumn id="44" xr3:uid="{0AC662FD-A750-4B07-9FA1-C0A56834D63C}" name="Wk 9 2026" dataDxfId="608"/>
+    <tableColumn id="45" xr3:uid="{D356147E-91B3-4FE6-8902-80DE5E506356}" name="Wk 10 2026" dataDxfId="607"/>
+    <tableColumn id="46" xr3:uid="{20F85B83-DD6D-4BD3-B9C5-6719520A2EE0}" name="Wk 11 2026" dataDxfId="606"/>
+    <tableColumn id="47" xr3:uid="{A2E896C3-648A-46D8-A60D-2F61164AE4D4}" name="Wk 12 2026" dataDxfId="605"/>
+    <tableColumn id="48" xr3:uid="{D2EE3864-47AF-47B8-A5B9-60043814D83B}" name="Wk 13 2026" dataDxfId="604"/>
+    <tableColumn id="49" xr3:uid="{3167537E-6E32-4EB2-886C-DF7B752427AD}" name="Wk 14 2026" dataDxfId="603"/>
+    <tableColumn id="50" xr3:uid="{FC861F37-0681-4883-BB56-051E14737063}" name="Wk 15 2026" dataDxfId="602"/>
+    <tableColumn id="51" xr3:uid="{71CE2DF8-303C-45BD-AA22-D1D58C5280AB}" name="Wk 16 2026" dataDxfId="601"/>
+    <tableColumn id="52" xr3:uid="{43D7A940-505E-4C88-A628-6E0EA042D0E3}" name="Wk 17 2026" dataDxfId="600"/>
+    <tableColumn id="53" xr3:uid="{8D7359CD-16CB-4005-AE4E-2F17127175BF}" name="Wk 18 2026" dataDxfId="599"/>
+    <tableColumn id="54" xr3:uid="{C2DF5A20-F9A8-4F4D-9E99-4D01760D21C4}" name="Wk 19 2026" dataDxfId="598"/>
+    <tableColumn id="55" xr3:uid="{96CA90C3-2763-4B8E-B42D-89C55FE5B616}" name="Wk 20 2026" dataDxfId="597"/>
+    <tableColumn id="56" xr3:uid="{F8362AE6-018F-4A08-B091-8B83805F4BB2}" name="Wk 21 2026" dataDxfId="596"/>
+    <tableColumn id="57" xr3:uid="{45992418-70A6-4DCD-A32C-1D63AA49A4D8}" name="Wk 22 2026" dataDxfId="595"/>
+    <tableColumn id="58" xr3:uid="{1B7D0E7A-E049-479A-9080-9FDFB57FC0CA}" name="Wk 23 2026" dataDxfId="594"/>
+    <tableColumn id="59" xr3:uid="{E95BFF68-C21B-49FD-B2DA-15EE93B58EAA}" name="Wk 24 2026" dataDxfId="593"/>
+    <tableColumn id="60" xr3:uid="{ECF0F9BF-7920-419B-B2CF-F09E730FF878}" name="Wk 25 2026" dataDxfId="592"/>
+    <tableColumn id="61" xr3:uid="{5DA71C02-37E7-4396-A1B7-FF70D24CDE19}" name="Wk 26 2026" dataDxfId="591"/>
+    <tableColumn id="62" xr3:uid="{F9A5F33B-D2C0-455B-A34B-8EFDFD6C8C53}" name="Wk 27 2026" dataDxfId="590"/>
+    <tableColumn id="63" xr3:uid="{D4CD628A-4312-4FB1-995A-60E50CBDC427}" name="Wk 28 2026" dataDxfId="589"/>
+    <tableColumn id="64" xr3:uid="{CB6C362B-F773-41B2-A29C-FE9E91160619}" name="Wk 29 2026" dataDxfId="588"/>
+    <tableColumn id="65" xr3:uid="{056BC328-B98D-4D28-958C-77D46F881CB2}" name="Wk 30 2026" dataDxfId="587"/>
+    <tableColumn id="66" xr3:uid="{017E8A3B-C1CB-4DBE-B7CF-6205BE4DCDB2}" name="Wk 31 2026" dataDxfId="586"/>
+    <tableColumn id="67" xr3:uid="{1CE38079-6A49-4EDC-9CC9-30C350F40A7A}" name="Wk 32 2026" dataDxfId="585"/>
+    <tableColumn id="68" xr3:uid="{D267527A-B4F7-4FD7-A909-D77BFB9C4BFE}" name="Wk 33 2026" dataDxfId="584"/>
+    <tableColumn id="69" xr3:uid="{FBC52664-8D0E-40AC-8DE4-AEA565D8FAAD}" name="Wk 34 2026" dataDxfId="583"/>
+    <tableColumn id="70" xr3:uid="{BEEBB6E6-7DF6-4419-8EDA-37A3969DB9C0}" name="Wk 35 2026" dataDxfId="582"/>
+    <tableColumn id="71" xr3:uid="{7F513271-0C3A-441B-A2BF-AEFC48D33362}" name="Wk 36 2026" dataDxfId="581"/>
+    <tableColumn id="72" xr3:uid="{4A3C3440-7ED7-4C43-92CA-BA6E7289B8BF}" name="Wk 37 2026" dataDxfId="580"/>
+    <tableColumn id="73" xr3:uid="{1F1D81D8-3E1D-48E7-A4D7-F1354773D8FD}" name="Wk 38 2026" dataDxfId="579"/>
+    <tableColumn id="74" xr3:uid="{E238D3F0-F210-44E2-A00F-BC7CB7A3023B}" name="Wk 39 2026" dataDxfId="578"/>
+    <tableColumn id="75" xr3:uid="{F723C8D0-D8C1-42E1-BD33-E046191D32FC}" name="Wk 40 2026" dataDxfId="577"/>
+    <tableColumn id="76" xr3:uid="{6B5AD89D-E0AB-4AAE-A980-119A8B92E3B6}" name="Wk 41 2026" dataDxfId="576"/>
+    <tableColumn id="77" xr3:uid="{B3DFB992-C284-480B-A932-68F1E3BAA1F1}" name="Wk 42 2026" dataDxfId="575"/>
+    <tableColumn id="78" xr3:uid="{AF8D3D15-C719-41F6-A7B3-49DC7942AEBA}" name="Wk 43 2026" dataDxfId="574"/>
+    <tableColumn id="79" xr3:uid="{53F8DB87-1D36-4550-8E4A-254AFAFA3339}" name="Wk 44 2026" dataDxfId="573"/>
+    <tableColumn id="80" xr3:uid="{43B071E7-D7BF-4B02-8D7B-C324F1E62544}" name="Wk 45 2026" dataDxfId="572"/>
+    <tableColumn id="81" xr3:uid="{6D73DCF7-69D1-44D6-BE42-2644FC05A976}" name="Wk 46 2026" dataDxfId="571"/>
+    <tableColumn id="82" xr3:uid="{407A00F3-B635-4B5C-B192-07496436E40B}" name="Wk 47 2026" dataDxfId="570"/>
+    <tableColumn id="83" xr3:uid="{A84AA1C8-5D88-4E2D-95CE-9E3A10456C9C}" name="Wk 48 2026" dataDxfId="569"/>
+    <tableColumn id="84" xr3:uid="{23F810B7-D1C3-4A18-9C25-1C19D01CF258}" name="Wk 49 2026" dataDxfId="568"/>
+    <tableColumn id="85" xr3:uid="{5C2AB52B-D93A-4447-81C5-CBA70222893C}" name="Wk 50 2026" dataDxfId="567"/>
+    <tableColumn id="86" xr3:uid="{22AFCD3C-D466-4832-828D-19411BAA244C}" name="Wk 51 2026" dataDxfId="566"/>
+    <tableColumn id="87" xr3:uid="{0261B616-7060-407D-8580-0BF44181D661}" name="Wk 52 2026" dataDxfId="565"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24488,12 +24516,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AF2F6AA2-3B85-49C0-93EF-6D62990D7D3D}" name="tblActualsTransits" displayName="tblActualsTransits" ref="B12:CJ18" totalsRowShown="0">
   <autoFilter ref="B12:CJ18" xr:uid="{AF2F6AA2-3B85-49C0-93EF-6D62990D7D3D}"/>
   <tableColumns count="87">
-    <tableColumn id="1" xr3:uid="{E3DA8C1F-9109-4FE4-8F24-679F193AB1C7}" name="MP" dataDxfId="566"/>
-    <tableColumn id="2" xr3:uid="{E026F489-918C-4CC7-A266-2BF2D84F6B52}" name="Wk19 2025" dataDxfId="565"/>
-    <tableColumn id="3" xr3:uid="{18E7FAA1-EF17-4B30-9AA5-A04B3BF2276D}" name="Wk20 2025" dataDxfId="564"/>
-    <tableColumn id="4" xr3:uid="{877B0054-B084-422D-AFAA-630A6454561F}" name="Wk21 2025" dataDxfId="563"/>
-    <tableColumn id="5" xr3:uid="{CA37F9BC-A31E-4EE3-ABC7-670299FF0E9C}" name="Wk22 2025" dataDxfId="562"/>
-    <tableColumn id="6" xr3:uid="{546BD560-251E-4C36-A8FD-D89903CB07B7}" name="Wk23 2025" dataDxfId="561"/>
+    <tableColumn id="1" xr3:uid="{E3DA8C1F-9109-4FE4-8F24-679F193AB1C7}" name="MP" dataDxfId="564"/>
+    <tableColumn id="2" xr3:uid="{E026F489-918C-4CC7-A266-2BF2D84F6B52}" name="Wk19 2025" dataDxfId="563"/>
+    <tableColumn id="3" xr3:uid="{18E7FAA1-EF17-4B30-9AA5-A04B3BF2276D}" name="Wk20 2025" dataDxfId="562"/>
+    <tableColumn id="4" xr3:uid="{877B0054-B084-422D-AFAA-630A6454561F}" name="Wk21 2025" dataDxfId="561"/>
+    <tableColumn id="5" xr3:uid="{CA37F9BC-A31E-4EE3-ABC7-670299FF0E9C}" name="Wk22 2025" dataDxfId="560"/>
+    <tableColumn id="6" xr3:uid="{546BD560-251E-4C36-A8FD-D89903CB07B7}" name="Wk23 2025" dataDxfId="559"/>
     <tableColumn id="7" xr3:uid="{73F9F261-C5C5-4E3F-9792-DF464514CACF}" name="Wk24 2025"/>
     <tableColumn id="8" xr3:uid="{D81B9DC7-A9EC-42C5-AF83-E3C59E37DA58}" name="Wk25 2025"/>
     <tableColumn id="9" xr3:uid="{02EB5DE8-213C-493A-B9E2-BE9CC91D979D}" name="Wk26 2025"/>
@@ -24510,167 +24538,167 @@
     <tableColumn id="20" xr3:uid="{BF9640D8-903A-4F95-8D38-4513A65B7054}" name="Wk37 2025"/>
     <tableColumn id="21" xr3:uid="{D443E079-1A8D-4B36-BCA5-69455AD64B53}" name="Wk38 2025"/>
     <tableColumn id="22" xr3:uid="{F77B4DED-7860-46DF-8C68-2A7CC8852EBC}" name="Wk39 2025"/>
-    <tableColumn id="23" xr3:uid="{B26205EF-14E9-4DD1-9C3A-C94A1ED3A259}" name="Wk40 2025" dataDxfId="560"/>
-    <tableColumn id="24" xr3:uid="{4E8B04B3-5B41-4D68-9275-B413B0485146}" name="Wk41 2025" dataDxfId="559"/>
-    <tableColumn id="25" xr3:uid="{62CF15B3-EAFE-4A97-844E-A4065946591D}" name="Wk42 2025" dataDxfId="558"/>
-    <tableColumn id="26" xr3:uid="{D4B6DD7F-CC54-48FE-AC7E-89776AB8C5FE}" name="Wk43 2025" dataDxfId="557"/>
-    <tableColumn id="27" xr3:uid="{10941D27-8F64-4156-BDFD-C56CE3FC2163}" name="Wk44 2025" dataDxfId="556"/>
-    <tableColumn id="28" xr3:uid="{F64445E6-4172-4FAA-9E8F-FC3137C4832F}" name="Wk45 2025" dataDxfId="555"/>
-    <tableColumn id="29" xr3:uid="{8151F958-E7EA-4B9D-863B-C57080849EC2}" name="Wk46 2025" dataDxfId="554"/>
-    <tableColumn id="30" xr3:uid="{6C4DCFBC-E342-48F3-B774-80A0DCFAAEE1}" name="Wk47 2025" dataDxfId="553"/>
-    <tableColumn id="31" xr3:uid="{49227077-12C2-4DAB-8607-6A807925F88B}" name="Wk48 2025" dataDxfId="552"/>
-    <tableColumn id="32" xr3:uid="{B4B9AAEB-CC82-4FD1-B714-8BCB374A521A}" name="Wk49 2025" dataDxfId="551"/>
-    <tableColumn id="33" xr3:uid="{5A90B961-E796-4C65-BA99-43EDB17D4EDA}" name="Wk50 2025" dataDxfId="550"/>
-    <tableColumn id="34" xr3:uid="{D4AFF83E-AD4D-4FDA-AF87-34821AEAD64D}" name="Wk51 2025" dataDxfId="549"/>
-    <tableColumn id="35" xr3:uid="{14FD9D8B-7FB6-494F-A6B3-D6B972357258}" name="Wk52 2025" dataDxfId="72"/>
-    <tableColumn id="36" xr3:uid="{442148C4-4271-4EED-ABAD-A34D33D9926F}" name="Wk 1 2026" dataDxfId="71"/>
-    <tableColumn id="37" xr3:uid="{11B60504-DD63-4937-94FB-2D4A06DEF060}" name="Wk 2 2026" dataDxfId="548"/>
-    <tableColumn id="38" xr3:uid="{BD06E569-07F1-4FC6-BF94-B704212DCE2B}" name="Wk 3 2026" dataDxfId="547"/>
-    <tableColumn id="39" xr3:uid="{CA87DDE3-6416-454C-9D7E-CC5790CB690F}" name="Wk 4 2026" dataDxfId="546"/>
-    <tableColumn id="40" xr3:uid="{6EEF7AA1-9CFA-4D53-A58B-F48937239DEE}" name="Wk 5 2026" dataDxfId="545"/>
-    <tableColumn id="41" xr3:uid="{46401BB9-07EB-44E4-B399-4F2C970136E1}" name="Wk 6 2026" dataDxfId="544"/>
-    <tableColumn id="42" xr3:uid="{95245AC5-7323-4BAD-AD8F-8530AABAB90F}" name="Wk 7 2026" dataDxfId="543"/>
-    <tableColumn id="43" xr3:uid="{5EE0D4E5-69C9-438F-98EF-E3C4D74E829D}" name="Wk 8 2026" dataDxfId="542"/>
-    <tableColumn id="44" xr3:uid="{AA0A71B5-4607-4776-9EF0-970C84C0E11D}" name="Wk 9 2026" dataDxfId="541"/>
-    <tableColumn id="45" xr3:uid="{E6E6DBB9-44EE-4B71-A5A2-EA40CCF528A7}" name="Wk 10 2026" dataDxfId="540"/>
-    <tableColumn id="46" xr3:uid="{ACE31F9D-6F4E-4E84-B7CC-F5EB5C471259}" name="Wk 11 2026" dataDxfId="539"/>
-    <tableColumn id="47" xr3:uid="{65201ADE-1F38-499B-99F3-4CD9E250EB01}" name="Wk 12 2026" dataDxfId="538"/>
-    <tableColumn id="48" xr3:uid="{572C4DC1-4AD6-4F4D-83FA-6A030761102C}" name="Wk 13 2026" dataDxfId="537"/>
-    <tableColumn id="49" xr3:uid="{4557144E-A735-4EDF-86B1-D93604944B45}" name="Wk 14 2026" dataDxfId="536"/>
-    <tableColumn id="50" xr3:uid="{5EFA0D92-D65E-49B8-9DE4-A3ABD131057D}" name="Wk 15 2026" dataDxfId="535"/>
-    <tableColumn id="51" xr3:uid="{30D2A5ED-B5F4-4F35-81B0-024D0F17C7F7}" name="Wk 16 2026" dataDxfId="534"/>
-    <tableColumn id="52" xr3:uid="{A9C850FC-31FE-433E-8223-7E0714A09E3F}" name="Wk 17 2026" dataDxfId="533"/>
-    <tableColumn id="53" xr3:uid="{E7DCE4A6-FAF8-43A8-84A4-9836532DCE16}" name="Wk 18 2026" dataDxfId="532"/>
-    <tableColumn id="54" xr3:uid="{16C4AC0B-3AA0-470A-A748-73654B61A92C}" name="Wk 19 2026" dataDxfId="531"/>
-    <tableColumn id="55" xr3:uid="{3E03351C-A883-462F-B3DC-42CD76734667}" name="Wk 20 2026" dataDxfId="530"/>
-    <tableColumn id="56" xr3:uid="{111A8410-AE9C-4792-B0A8-894D8F0F26C0}" name="Wk 21 2026" dataDxfId="529"/>
-    <tableColumn id="57" xr3:uid="{0362EDB7-6B20-4890-863C-B0FD1C04F93B}" name="Wk 22 2026" dataDxfId="528"/>
-    <tableColumn id="58" xr3:uid="{8C3E4134-A7C2-42F5-B34C-3A889A9F1412}" name="Wk 23 2026" dataDxfId="527"/>
-    <tableColumn id="59" xr3:uid="{51D857B9-8DF2-40EB-B685-4B3083C00D81}" name="Wk 24 2026" dataDxfId="526"/>
-    <tableColumn id="60" xr3:uid="{8AB833B8-A264-4BC9-A613-5A8424E84554}" name="Wk 25 2026" dataDxfId="525"/>
-    <tableColumn id="61" xr3:uid="{E3A4361D-040A-4BF4-9067-0848206C05DA}" name="Wk 26 2026" dataDxfId="524"/>
-    <tableColumn id="62" xr3:uid="{5761BEE7-9629-4E91-B703-AE2D19CF8013}" name="Wk 27 2026" dataDxfId="523"/>
-    <tableColumn id="63" xr3:uid="{70065DA2-F065-4E86-81F7-ACF9FFF2A01A}" name="Wk 28 2026" dataDxfId="522"/>
-    <tableColumn id="64" xr3:uid="{BEDF1643-1916-4719-BCE4-2D3321BAF7C7}" name="Wk 29 2026" dataDxfId="521"/>
-    <tableColumn id="65" xr3:uid="{5336462A-C484-4DC0-AB1C-F03C5DB3DE0F}" name="Wk 30 2026" dataDxfId="520"/>
-    <tableColumn id="66" xr3:uid="{4BDEC5F9-20DA-4CCF-8B5A-742FEA192E85}" name="Wk 31 2026" dataDxfId="519"/>
-    <tableColumn id="67" xr3:uid="{291B5CB3-F692-43FA-819A-F319D37CCDDE}" name="Wk 32 2026" dataDxfId="518"/>
-    <tableColumn id="68" xr3:uid="{2163603E-7D1E-47DB-88DA-2C8CC973F723}" name="Wk 33 2026" dataDxfId="517"/>
-    <tableColumn id="69" xr3:uid="{3B499C30-E189-45A4-B3B6-4EF44EE5FD7F}" name="Wk 34 2026" dataDxfId="516"/>
-    <tableColumn id="70" xr3:uid="{B95C85AD-B5AA-48AB-BB10-5E0558FD3022}" name="Wk 35 2026" dataDxfId="515"/>
-    <tableColumn id="71" xr3:uid="{D118CFC2-27B6-4806-824D-3093FB03C4C6}" name="Wk 36 2026" dataDxfId="514"/>
-    <tableColumn id="72" xr3:uid="{25EFA270-FF47-49BC-A1B7-0D21B54579DF}" name="Wk 37 2026" dataDxfId="513"/>
-    <tableColumn id="73" xr3:uid="{19F55CE1-2B13-4271-8428-C233DFFE07D8}" name="Wk 38 2026" dataDxfId="512"/>
-    <tableColumn id="74" xr3:uid="{4B36CD4A-6E63-4181-B3D5-A5CE66E1DA9F}" name="Wk 39 2026" dataDxfId="511"/>
-    <tableColumn id="75" xr3:uid="{D8A64CDC-14A7-4AF9-B3E7-C65BBCDF3171}" name="Wk 40 2026" dataDxfId="510"/>
-    <tableColumn id="76" xr3:uid="{BDB569E9-40D8-4335-B699-4F10D11CD341}" name="Wk 41 2026" dataDxfId="509"/>
-    <tableColumn id="77" xr3:uid="{2E41A7AB-5341-4688-B5CD-AFEF651DF3AA}" name="Wk 42 2026" dataDxfId="508"/>
-    <tableColumn id="78" xr3:uid="{16B3987D-76E5-40F6-9B80-56F08BC13B1C}" name="Wk 43 2026" dataDxfId="507"/>
-    <tableColumn id="79" xr3:uid="{047842C3-68C0-4214-82ED-70957E66DB4E}" name="Wk 44 2026" dataDxfId="506"/>
-    <tableColumn id="80" xr3:uid="{5075A64F-88BC-4E73-885D-04A7B8F23CA9}" name="Wk 45 2026" dataDxfId="505"/>
-    <tableColumn id="81" xr3:uid="{FC6545C1-7C0A-403C-B077-B0F964CE81CA}" name="Wk 46 2026" dataDxfId="504"/>
-    <tableColumn id="82" xr3:uid="{7D2EECE4-68D2-4455-AE18-8DC628DF1FED}" name="Wk 47 2026" dataDxfId="503"/>
-    <tableColumn id="83" xr3:uid="{71CD6BB7-F3CE-466A-8E17-4A13F7D3650D}" name="Wk 48 2026" dataDxfId="502"/>
-    <tableColumn id="84" xr3:uid="{D6CDBF70-A69F-4163-80DF-EE7D03FAFB88}" name="Wk 49 2026" dataDxfId="501"/>
-    <tableColumn id="85" xr3:uid="{87EA7AB9-9593-4DCD-9A17-C309207ED5FF}" name="Wk 50 2026" dataDxfId="500"/>
-    <tableColumn id="86" xr3:uid="{12CE7E2F-5DBB-4CE7-BCAD-AF074BAD5DBB}" name="Wk 51 2026" dataDxfId="499"/>
-    <tableColumn id="87" xr3:uid="{39A1509C-0384-4DEA-A35F-9738B236382F}" name="Wk 52 2026" dataDxfId="498"/>
+    <tableColumn id="23" xr3:uid="{B26205EF-14E9-4DD1-9C3A-C94A1ED3A259}" name="Wk40 2025" dataDxfId="558"/>
+    <tableColumn id="24" xr3:uid="{4E8B04B3-5B41-4D68-9275-B413B0485146}" name="Wk41 2025" dataDxfId="557"/>
+    <tableColumn id="25" xr3:uid="{62CF15B3-EAFE-4A97-844E-A4065946591D}" name="Wk42 2025" dataDxfId="556"/>
+    <tableColumn id="26" xr3:uid="{D4B6DD7F-CC54-48FE-AC7E-89776AB8C5FE}" name="Wk43 2025" dataDxfId="555"/>
+    <tableColumn id="27" xr3:uid="{10941D27-8F64-4156-BDFD-C56CE3FC2163}" name="Wk44 2025" dataDxfId="554"/>
+    <tableColumn id="28" xr3:uid="{F64445E6-4172-4FAA-9E8F-FC3137C4832F}" name="Wk45 2025" dataDxfId="553"/>
+    <tableColumn id="29" xr3:uid="{8151F958-E7EA-4B9D-863B-C57080849EC2}" name="Wk46 2025" dataDxfId="552"/>
+    <tableColumn id="30" xr3:uid="{6C4DCFBC-E342-48F3-B774-80A0DCFAAEE1}" name="Wk47 2025" dataDxfId="551"/>
+    <tableColumn id="31" xr3:uid="{49227077-12C2-4DAB-8607-6A807925F88B}" name="Wk48 2025" dataDxfId="550"/>
+    <tableColumn id="32" xr3:uid="{B4B9AAEB-CC82-4FD1-B714-8BCB374A521A}" name="Wk49 2025" dataDxfId="549"/>
+    <tableColumn id="33" xr3:uid="{5A90B961-E796-4C65-BA99-43EDB17D4EDA}" name="Wk50 2025" dataDxfId="548"/>
+    <tableColumn id="34" xr3:uid="{D4AFF83E-AD4D-4FDA-AF87-34821AEAD64D}" name="Wk51 2025" dataDxfId="547"/>
+    <tableColumn id="35" xr3:uid="{14FD9D8B-7FB6-494F-A6B3-D6B972357258}" name="Wk52 2025" dataDxfId="546"/>
+    <tableColumn id="36" xr3:uid="{442148C4-4271-4EED-ABAD-A34D33D9926F}" name="Wk 1 2026" dataDxfId="545"/>
+    <tableColumn id="37" xr3:uid="{11B60504-DD63-4937-94FB-2D4A06DEF060}" name="Wk 2 2026" dataDxfId="544"/>
+    <tableColumn id="38" xr3:uid="{BD06E569-07F1-4FC6-BF94-B704212DCE2B}" name="Wk 3 2026" dataDxfId="543"/>
+    <tableColumn id="39" xr3:uid="{CA87DDE3-6416-454C-9D7E-CC5790CB690F}" name="Wk 4 2026" dataDxfId="542"/>
+    <tableColumn id="40" xr3:uid="{6EEF7AA1-9CFA-4D53-A58B-F48937239DEE}" name="Wk 5 2026" dataDxfId="2"/>
+    <tableColumn id="41" xr3:uid="{46401BB9-07EB-44E4-B399-4F2C970136E1}" name="Wk 6 2026" dataDxfId="541"/>
+    <tableColumn id="42" xr3:uid="{95245AC5-7323-4BAD-AD8F-8530AABAB90F}" name="Wk 7 2026" dataDxfId="540"/>
+    <tableColumn id="43" xr3:uid="{5EE0D4E5-69C9-438F-98EF-E3C4D74E829D}" name="Wk 8 2026" dataDxfId="539"/>
+    <tableColumn id="44" xr3:uid="{AA0A71B5-4607-4776-9EF0-970C84C0E11D}" name="Wk 9 2026" dataDxfId="538"/>
+    <tableColumn id="45" xr3:uid="{E6E6DBB9-44EE-4B71-A5A2-EA40CCF528A7}" name="Wk 10 2026" dataDxfId="537"/>
+    <tableColumn id="46" xr3:uid="{ACE31F9D-6F4E-4E84-B7CC-F5EB5C471259}" name="Wk 11 2026" dataDxfId="536"/>
+    <tableColumn id="47" xr3:uid="{65201ADE-1F38-499B-99F3-4CD9E250EB01}" name="Wk 12 2026" dataDxfId="535"/>
+    <tableColumn id="48" xr3:uid="{572C4DC1-4AD6-4F4D-83FA-6A030761102C}" name="Wk 13 2026" dataDxfId="534"/>
+    <tableColumn id="49" xr3:uid="{4557144E-A735-4EDF-86B1-D93604944B45}" name="Wk 14 2026" dataDxfId="533"/>
+    <tableColumn id="50" xr3:uid="{5EFA0D92-D65E-49B8-9DE4-A3ABD131057D}" name="Wk 15 2026" dataDxfId="532"/>
+    <tableColumn id="51" xr3:uid="{30D2A5ED-B5F4-4F35-81B0-024D0F17C7F7}" name="Wk 16 2026" dataDxfId="531"/>
+    <tableColumn id="52" xr3:uid="{A9C850FC-31FE-433E-8223-7E0714A09E3F}" name="Wk 17 2026" dataDxfId="530"/>
+    <tableColumn id="53" xr3:uid="{E7DCE4A6-FAF8-43A8-84A4-9836532DCE16}" name="Wk 18 2026" dataDxfId="529"/>
+    <tableColumn id="54" xr3:uid="{16C4AC0B-3AA0-470A-A748-73654B61A92C}" name="Wk 19 2026" dataDxfId="528"/>
+    <tableColumn id="55" xr3:uid="{3E03351C-A883-462F-B3DC-42CD76734667}" name="Wk 20 2026" dataDxfId="527"/>
+    <tableColumn id="56" xr3:uid="{111A8410-AE9C-4792-B0A8-894D8F0F26C0}" name="Wk 21 2026" dataDxfId="526"/>
+    <tableColumn id="57" xr3:uid="{0362EDB7-6B20-4890-863C-B0FD1C04F93B}" name="Wk 22 2026" dataDxfId="525"/>
+    <tableColumn id="58" xr3:uid="{8C3E4134-A7C2-42F5-B34C-3A889A9F1412}" name="Wk 23 2026" dataDxfId="524"/>
+    <tableColumn id="59" xr3:uid="{51D857B9-8DF2-40EB-B685-4B3083C00D81}" name="Wk 24 2026" dataDxfId="523"/>
+    <tableColumn id="60" xr3:uid="{8AB833B8-A264-4BC9-A613-5A8424E84554}" name="Wk 25 2026" dataDxfId="522"/>
+    <tableColumn id="61" xr3:uid="{E3A4361D-040A-4BF4-9067-0848206C05DA}" name="Wk 26 2026" dataDxfId="521"/>
+    <tableColumn id="62" xr3:uid="{5761BEE7-9629-4E91-B703-AE2D19CF8013}" name="Wk 27 2026" dataDxfId="520"/>
+    <tableColumn id="63" xr3:uid="{70065DA2-F065-4E86-81F7-ACF9FFF2A01A}" name="Wk 28 2026" dataDxfId="519"/>
+    <tableColumn id="64" xr3:uid="{BEDF1643-1916-4719-BCE4-2D3321BAF7C7}" name="Wk 29 2026" dataDxfId="518"/>
+    <tableColumn id="65" xr3:uid="{5336462A-C484-4DC0-AB1C-F03C5DB3DE0F}" name="Wk 30 2026" dataDxfId="517"/>
+    <tableColumn id="66" xr3:uid="{4BDEC5F9-20DA-4CCF-8B5A-742FEA192E85}" name="Wk 31 2026" dataDxfId="516"/>
+    <tableColumn id="67" xr3:uid="{291B5CB3-F692-43FA-819A-F319D37CCDDE}" name="Wk 32 2026" dataDxfId="515"/>
+    <tableColumn id="68" xr3:uid="{2163603E-7D1E-47DB-88DA-2C8CC973F723}" name="Wk 33 2026" dataDxfId="514"/>
+    <tableColumn id="69" xr3:uid="{3B499C30-E189-45A4-B3B6-4EF44EE5FD7F}" name="Wk 34 2026" dataDxfId="513"/>
+    <tableColumn id="70" xr3:uid="{B95C85AD-B5AA-48AB-BB10-5E0558FD3022}" name="Wk 35 2026" dataDxfId="512"/>
+    <tableColumn id="71" xr3:uid="{D118CFC2-27B6-4806-824D-3093FB03C4C6}" name="Wk 36 2026" dataDxfId="511"/>
+    <tableColumn id="72" xr3:uid="{25EFA270-FF47-49BC-A1B7-0D21B54579DF}" name="Wk 37 2026" dataDxfId="510"/>
+    <tableColumn id="73" xr3:uid="{19F55CE1-2B13-4271-8428-C233DFFE07D8}" name="Wk 38 2026" dataDxfId="509"/>
+    <tableColumn id="74" xr3:uid="{4B36CD4A-6E63-4181-B3D5-A5CE66E1DA9F}" name="Wk 39 2026" dataDxfId="508"/>
+    <tableColumn id="75" xr3:uid="{D8A64CDC-14A7-4AF9-B3E7-C65BBCDF3171}" name="Wk 40 2026" dataDxfId="507"/>
+    <tableColumn id="76" xr3:uid="{BDB569E9-40D8-4335-B699-4F10D11CD341}" name="Wk 41 2026" dataDxfId="506"/>
+    <tableColumn id="77" xr3:uid="{2E41A7AB-5341-4688-B5CD-AFEF651DF3AA}" name="Wk 42 2026" dataDxfId="505"/>
+    <tableColumn id="78" xr3:uid="{16B3987D-76E5-40F6-9B80-56F08BC13B1C}" name="Wk 43 2026" dataDxfId="504"/>
+    <tableColumn id="79" xr3:uid="{047842C3-68C0-4214-82ED-70957E66DB4E}" name="Wk 44 2026" dataDxfId="503"/>
+    <tableColumn id="80" xr3:uid="{5075A64F-88BC-4E73-885D-04A7B8F23CA9}" name="Wk 45 2026" dataDxfId="502"/>
+    <tableColumn id="81" xr3:uid="{FC6545C1-7C0A-403C-B077-B0F964CE81CA}" name="Wk 46 2026" dataDxfId="501"/>
+    <tableColumn id="82" xr3:uid="{7D2EECE4-68D2-4455-AE18-8DC628DF1FED}" name="Wk 47 2026" dataDxfId="500"/>
+    <tableColumn id="83" xr3:uid="{71CD6BB7-F3CE-466A-8E17-4A13F7D3650D}" name="Wk 48 2026" dataDxfId="499"/>
+    <tableColumn id="84" xr3:uid="{D6CDBF70-A69F-4163-80DF-EE7D03FAFB88}" name="Wk 49 2026" dataDxfId="498"/>
+    <tableColumn id="85" xr3:uid="{87EA7AB9-9593-4DCD-9A17-C309207ED5FF}" name="Wk 50 2026" dataDxfId="497"/>
+    <tableColumn id="86" xr3:uid="{12CE7E2F-5DBB-4CE7-BCAD-AF074BAD5DBB}" name="Wk 51 2026" dataDxfId="496"/>
+    <tableColumn id="87" xr3:uid="{39A1509C-0384-4DEA-A35F-9738B236382F}" name="Wk 52 2026" dataDxfId="495"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D94A8E4D-A3EA-4F8D-87A1-91E37E9EDB1D}" name="tblActualsConversion" displayName="tblActualsConversion" ref="B21:CJ27" totalsRowShown="0" headerRowDxfId="497" dataDxfId="496">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D94A8E4D-A3EA-4F8D-87A1-91E37E9EDB1D}" name="tblActualsConversion" displayName="tblActualsConversion" ref="B21:CJ27" totalsRowShown="0" headerRowDxfId="494" dataDxfId="493">
   <autoFilter ref="B21:CJ27" xr:uid="{D94A8E4D-A3EA-4F8D-87A1-91E37E9EDB1D}"/>
   <tableColumns count="87">
-    <tableColumn id="1" xr3:uid="{5BCA36AD-5ED6-4BD2-82C6-9514EB6C8E39}" name="MP" dataDxfId="495"/>
-    <tableColumn id="2" xr3:uid="{E0B512F1-81AA-4777-83A7-91B19281DC01}" name="Wk19 2025" dataDxfId="494"/>
-    <tableColumn id="3" xr3:uid="{ADF0495B-64C9-464F-B4F1-1B999F877A70}" name="Wk20 2025" dataDxfId="493"/>
-    <tableColumn id="4" xr3:uid="{AAA28000-BBB9-43B0-96A2-F14F4115A44F}" name="Wk21 2025" dataDxfId="492"/>
-    <tableColumn id="5" xr3:uid="{867C7A38-1F05-48EC-9E45-D81120B87575}" name="Wk22 2025" dataDxfId="491"/>
-    <tableColumn id="6" xr3:uid="{FE9E06F2-6DEF-4E69-B058-76BAAFA9E597}" name="Wk23 2025" dataDxfId="490"/>
-    <tableColumn id="7" xr3:uid="{0ECB0B5E-176D-4229-A87A-C2A41E188E14}" name="Wk24 2025" dataDxfId="489"/>
-    <tableColumn id="8" xr3:uid="{C3FE39BE-3AA1-47B1-BB14-DB9B5D06E3D4}" name="Wk25 2025" dataDxfId="488"/>
-    <tableColumn id="9" xr3:uid="{E15F5E82-567D-4EA7-B0FF-0F0F5AA4EF07}" name="Wk26 2025" dataDxfId="487"/>
-    <tableColumn id="10" xr3:uid="{2F64D629-5535-490F-8B73-7C5E5946C95C}" name="Wk27 2025" dataDxfId="486"/>
-    <tableColumn id="11" xr3:uid="{A7D2AA51-7E39-45EC-A1AF-3AD0ED7B4FEB}" name="Wk28 2025" dataDxfId="485"/>
-    <tableColumn id="12" xr3:uid="{5877E484-4A49-4F53-8DAD-69FC96E3C88B}" name="Wk29 2025" dataDxfId="484"/>
-    <tableColumn id="13" xr3:uid="{35F7EC93-39F3-424E-A574-8491DA11C419}" name="Wk30 2025" dataDxfId="483"/>
-    <tableColumn id="14" xr3:uid="{D12E41AC-2CF4-45BF-BA33-6541F8092902}" name="Wk31 2025" dataDxfId="482"/>
-    <tableColumn id="15" xr3:uid="{AC2E1D16-8999-4552-AFCA-093F0E20266C}" name="Wk32 2025" dataDxfId="481"/>
-    <tableColumn id="16" xr3:uid="{B0ECF92A-CEE6-42ED-994E-7CEC6ED0C3FF}" name="Wk33 2025" dataDxfId="480"/>
-    <tableColumn id="17" xr3:uid="{252E88F5-331D-4D1D-A862-965D7EE83B14}" name="Wk34 2025" dataDxfId="479"/>
-    <tableColumn id="18" xr3:uid="{3F1619A4-1F4A-4AA3-B78F-CC17B4219BF7}" name="Wk35 2025" dataDxfId="478"/>
-    <tableColumn id="19" xr3:uid="{D37CF251-9CBA-47CF-90F3-9832F6491757}" name="Wk36 2025" dataDxfId="477"/>
-    <tableColumn id="20" xr3:uid="{2B42A392-F058-4B55-840D-45F390CA40BD}" name="Wk37 2025" dataDxfId="476"/>
-    <tableColumn id="21" xr3:uid="{F8B2B06E-1C89-4881-B690-FDA929360DE4}" name="Wk38 2025" dataDxfId="475"/>
-    <tableColumn id="22" xr3:uid="{984EE42D-9ECD-4A41-ABB7-77EFB728499E}" name="Wk39 2025" dataDxfId="474"/>
-    <tableColumn id="23" xr3:uid="{D783F65F-027D-40A3-930F-1ABE09D70996}" name="Wk40 2025" dataDxfId="473" dataCellStyle="Percent"/>
-    <tableColumn id="24" xr3:uid="{B1150C25-BBE4-4842-9B98-8CEB5DBE6AB1}" name="Wk41 2025" dataDxfId="472" dataCellStyle="Percent"/>
-    <tableColumn id="25" xr3:uid="{264979D8-1A3C-4E70-BF08-BCA8F44DD4E9}" name="Wk42 2025" dataDxfId="471" dataCellStyle="Percent"/>
-    <tableColumn id="26" xr3:uid="{7E03177B-2FD1-48AD-8020-48B71FDE6168}" name="Wk43 2025" dataDxfId="470" dataCellStyle="Percent"/>
-    <tableColumn id="27" xr3:uid="{47463794-0CBF-48E7-8A49-18A15ED419B1}" name="Wk44 2025" dataDxfId="469" dataCellStyle="Percent"/>
-    <tableColumn id="28" xr3:uid="{6D71255E-0304-4768-B806-1C188309AC23}" name="Wk45 2025" dataDxfId="468" dataCellStyle="Percent"/>
-    <tableColumn id="29" xr3:uid="{7B2ABC70-6901-4C50-9545-797DA7521C0A}" name="Wk46 2025" dataDxfId="467" dataCellStyle="Percent"/>
-    <tableColumn id="30" xr3:uid="{82BAECB3-50F7-49AE-BA46-AE7F37B085F7}" name="Wk47 2025" dataDxfId="466" dataCellStyle="Percent"/>
-    <tableColumn id="31" xr3:uid="{2764F785-0591-433A-959E-348BC8C85FB1}" name="Wk48 2025" dataDxfId="465" dataCellStyle="Percent"/>
-    <tableColumn id="32" xr3:uid="{5C934707-29EC-42D2-8D2C-B4160115F94D}" name="Wk49 2025" dataDxfId="464" dataCellStyle="Percent"/>
-    <tableColumn id="33" xr3:uid="{2DC6649A-600D-4B9A-B55D-8C8AD53DE891}" name="Wk50 2025" dataDxfId="463" dataCellStyle="Percent"/>
-    <tableColumn id="34" xr3:uid="{59F6FC88-B0E8-4E7F-BC1F-8926D8DB3525}" name="Wk51 2025" dataDxfId="462" dataCellStyle="Percent"/>
-    <tableColumn id="35" xr3:uid="{20AC0F5D-7547-431A-A70C-0C9ED683E230}" name="Wk52 2025" dataDxfId="70" dataCellStyle="Percent"/>
-    <tableColumn id="36" xr3:uid="{36F0C266-29AD-4FF9-B5F6-98E9E45CB123}" name="Wk 1 2026" dataDxfId="69" dataCellStyle="Percent"/>
-    <tableColumn id="37" xr3:uid="{338F823B-1750-4E1B-8067-969D7F77D0FF}" name="Wk 2 2026" dataDxfId="461" dataCellStyle="Percent"/>
-    <tableColumn id="38" xr3:uid="{21594A9B-C8AF-47BE-8004-34E3369173DE}" name="Wk 3 2026" dataDxfId="460" dataCellStyle="Percent"/>
-    <tableColumn id="39" xr3:uid="{D5F2887D-0DD4-4D96-9934-12684CBE26AF}" name="Wk 4 2026" dataDxfId="459" dataCellStyle="Percent"/>
-    <tableColumn id="40" xr3:uid="{FD966E31-4260-43EC-AD95-18BC9C146A4D}" name="Wk 5 2026" dataDxfId="458" dataCellStyle="Percent"/>
-    <tableColumn id="41" xr3:uid="{3E17D987-866E-4E6B-898A-E56A11ACA7BE}" name="Wk 6 2026" dataDxfId="457" dataCellStyle="Percent"/>
-    <tableColumn id="42" xr3:uid="{F695E36B-28E0-4EEC-B21A-45718DE82759}" name="Wk 7 2026" dataDxfId="456" dataCellStyle="Percent"/>
-    <tableColumn id="43" xr3:uid="{3C5FA813-A8E5-42D2-8E1C-65F19FEB108D}" name="Wk 8 2026" dataDxfId="455" dataCellStyle="Percent"/>
-    <tableColumn id="44" xr3:uid="{40450379-2F63-42C8-BDE4-CC381D409F01}" name="Wk 9 2026" dataDxfId="454" dataCellStyle="Percent"/>
-    <tableColumn id="45" xr3:uid="{959A18B3-226B-47B6-AC9D-324E60AB7335}" name="Wk 10 2026" dataDxfId="453" dataCellStyle="Percent"/>
-    <tableColumn id="46" xr3:uid="{718656E3-6EAB-4FEE-9805-4D7E7CA08D95}" name="Wk 11 2026" dataDxfId="452" dataCellStyle="Percent"/>
-    <tableColumn id="47" xr3:uid="{F4EED23F-2153-4495-93A6-0AE6352E93D2}" name="Wk 12 2026" dataDxfId="451" dataCellStyle="Percent"/>
-    <tableColumn id="48" xr3:uid="{50D6A3A5-3656-4E8A-85EC-014541A36615}" name="Wk 13 2026" dataDxfId="450" dataCellStyle="Percent"/>
-    <tableColumn id="49" xr3:uid="{7B8CAEA9-E4F7-4AFC-B363-D9DA4DD34E59}" name="Wk 14 2026" dataDxfId="449" dataCellStyle="Percent"/>
-    <tableColumn id="50" xr3:uid="{3E150CC9-84DD-4984-BA62-40D2355AA88E}" name="Wk 15 2026" dataDxfId="448" dataCellStyle="Percent"/>
-    <tableColumn id="51" xr3:uid="{9DAA22D5-D353-43D8-AEFB-493F9DC3B04E}" name="Wk 16 2026" dataDxfId="447" dataCellStyle="Percent"/>
-    <tableColumn id="52" xr3:uid="{3FD7A65B-632E-47FC-9A40-837CDA2763F2}" name="Wk 17 2026" dataDxfId="446" dataCellStyle="Percent"/>
-    <tableColumn id="53" xr3:uid="{18D37E87-2462-428E-A1C5-3AF89CBE351B}" name="Wk 18 2026" dataDxfId="445" dataCellStyle="Percent"/>
-    <tableColumn id="54" xr3:uid="{759D783E-2251-4AC0-BEAD-70CE7CA973E8}" name="Wk 19 2026" dataDxfId="444" dataCellStyle="Percent"/>
-    <tableColumn id="55" xr3:uid="{189BFD1D-5F97-4032-9626-96C1DD1ABF89}" name="Wk 20 2026" dataDxfId="443" dataCellStyle="Percent"/>
-    <tableColumn id="56" xr3:uid="{C4EF5625-E6E2-403E-A0A0-D31419673640}" name="Wk 21 2026" dataDxfId="442" dataCellStyle="Percent"/>
-    <tableColumn id="57" xr3:uid="{8555CA77-8EFB-4CA3-B5EF-7217EBF33553}" name="Wk 22 2026" dataDxfId="441" dataCellStyle="Percent"/>
-    <tableColumn id="58" xr3:uid="{C01E6A09-AB75-4A53-82BE-C0D77347E41B}" name="Wk 23 2026" dataDxfId="440" dataCellStyle="Percent"/>
-    <tableColumn id="59" xr3:uid="{80901ADD-FB23-458E-A355-FA8531334766}" name="Wk 24 2026" dataDxfId="439" dataCellStyle="Percent"/>
-    <tableColumn id="60" xr3:uid="{BEB995A6-53E6-4C56-9FCE-24C39723C622}" name="Wk 25 2026" dataDxfId="438" dataCellStyle="Percent"/>
-    <tableColumn id="61" xr3:uid="{905B51AE-0664-4B76-A24B-7F74A047D11F}" name="Wk 26 2026" dataDxfId="437" dataCellStyle="Percent"/>
-    <tableColumn id="62" xr3:uid="{6C89C269-10B4-4202-89E8-1DE1D3BF3C08}" name="Wk 27 2026" dataDxfId="436" dataCellStyle="Percent"/>
-    <tableColumn id="63" xr3:uid="{72C7ACA0-0D3B-4C6D-BE88-EE8728D56C1B}" name="Wk 28 2026" dataDxfId="435" dataCellStyle="Percent"/>
-    <tableColumn id="64" xr3:uid="{D0F1B34E-B2D8-4CA2-B633-4BD4E8D7E676}" name="Wk 29 2026" dataDxfId="434" dataCellStyle="Percent"/>
-    <tableColumn id="65" xr3:uid="{164D3D6B-4F1C-47BC-8C3A-42D8B0DACD02}" name="Wk 30 2026" dataDxfId="433" dataCellStyle="Percent"/>
-    <tableColumn id="66" xr3:uid="{02BF2A00-88FD-4084-B2E6-9446A001CC43}" name="Wk 31 2026" dataDxfId="432" dataCellStyle="Percent"/>
-    <tableColumn id="67" xr3:uid="{C5EFD435-0242-4482-9D98-D4CC41A6A7AF}" name="Wk 32 2026" dataDxfId="431" dataCellStyle="Percent"/>
-    <tableColumn id="68" xr3:uid="{1CE6F0BC-F07B-405D-90AE-CC1C4F8ADF52}" name="Wk 33 2026" dataDxfId="430" dataCellStyle="Percent"/>
-    <tableColumn id="69" xr3:uid="{2A3A92FD-16CC-4105-959F-64B83C997902}" name="Wk 34 2026" dataDxfId="429" dataCellStyle="Percent"/>
-    <tableColumn id="70" xr3:uid="{8116DA30-D266-4207-ACE3-7C14945389DA}" name="Wk 35 2026" dataDxfId="428" dataCellStyle="Percent"/>
-    <tableColumn id="71" xr3:uid="{CAECEBB9-A748-4769-857B-3342E4C729FF}" name="Wk 36 2026" dataDxfId="427" dataCellStyle="Percent"/>
-    <tableColumn id="72" xr3:uid="{8CB2587A-2C8D-4A3E-BBB2-D6E711E52ED2}" name="Wk 37 2026" dataDxfId="426" dataCellStyle="Percent"/>
-    <tableColumn id="73" xr3:uid="{71C06ADC-AA5D-4D8E-9311-76770D90E06C}" name="Wk 38 2026" dataDxfId="425" dataCellStyle="Percent"/>
-    <tableColumn id="74" xr3:uid="{48198F49-F131-4C76-A1D2-27CA0FD939FD}" name="Wk 39 2026" dataDxfId="424" dataCellStyle="Percent"/>
-    <tableColumn id="75" xr3:uid="{5D0AB91D-9077-4870-958C-030B842625A4}" name="Wk 40 2026" dataDxfId="423" dataCellStyle="Percent"/>
-    <tableColumn id="76" xr3:uid="{E5775D4C-09A6-4222-9DCC-7844B3E81D90}" name="Wk 41 2026" dataDxfId="422" dataCellStyle="Percent"/>
-    <tableColumn id="77" xr3:uid="{C1BF29EC-BACC-454D-ABEC-E327A1CA30C3}" name="Wk 42 2026" dataDxfId="421" dataCellStyle="Percent"/>
-    <tableColumn id="78" xr3:uid="{19E0BAB5-42D8-4B8E-AA57-D0E3F9A7C34E}" name="Wk 43 2026" dataDxfId="420" dataCellStyle="Percent"/>
-    <tableColumn id="79" xr3:uid="{BB9CE3BE-C0D0-49D9-BD2A-9FAEEEB31D6D}" name="Wk 44 2026" dataDxfId="419" dataCellStyle="Percent"/>
-    <tableColumn id="80" xr3:uid="{30D70071-2E17-4433-BAEC-65EC8EC8D3E9}" name="Wk 45 2026" dataDxfId="418" dataCellStyle="Percent"/>
-    <tableColumn id="81" xr3:uid="{E63760E7-9CC6-4AAC-8114-7FBAE4AA0B55}" name="Wk 46 2026" dataDxfId="417" dataCellStyle="Percent"/>
-    <tableColumn id="82" xr3:uid="{21ACBE91-92F3-457E-B81E-FFF488FDE917}" name="Wk 47 2026" dataDxfId="416" dataCellStyle="Percent"/>
-    <tableColumn id="83" xr3:uid="{437FA868-1251-45EB-ABBD-1C60F4AFB117}" name="Wk 48 2026" dataDxfId="415" dataCellStyle="Percent"/>
-    <tableColumn id="84" xr3:uid="{16C16432-FBA2-4A1E-9070-92F4447C89E1}" name="Wk 49 2026" dataDxfId="414" dataCellStyle="Percent"/>
-    <tableColumn id="85" xr3:uid="{88BD1C03-0653-480B-826D-EFF52AC09DC1}" name="Wk 50 2026" dataDxfId="413" dataCellStyle="Percent"/>
-    <tableColumn id="86" xr3:uid="{6F6ABEE0-3EDF-4F28-AF74-86A5B8128E83}" name="Wk 51 2026" dataDxfId="412" dataCellStyle="Percent"/>
-    <tableColumn id="87" xr3:uid="{12A48B29-AF32-4A2A-B981-6338D988BBA3}" name="Wk 52 2026" dataDxfId="411" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{5BCA36AD-5ED6-4BD2-82C6-9514EB6C8E39}" name="MP" dataDxfId="492"/>
+    <tableColumn id="2" xr3:uid="{E0B512F1-81AA-4777-83A7-91B19281DC01}" name="Wk19 2025" dataDxfId="491"/>
+    <tableColumn id="3" xr3:uid="{ADF0495B-64C9-464F-B4F1-1B999F877A70}" name="Wk20 2025" dataDxfId="490"/>
+    <tableColumn id="4" xr3:uid="{AAA28000-BBB9-43B0-96A2-F14F4115A44F}" name="Wk21 2025" dataDxfId="489"/>
+    <tableColumn id="5" xr3:uid="{867C7A38-1F05-48EC-9E45-D81120B87575}" name="Wk22 2025" dataDxfId="488"/>
+    <tableColumn id="6" xr3:uid="{FE9E06F2-6DEF-4E69-B058-76BAAFA9E597}" name="Wk23 2025" dataDxfId="487"/>
+    <tableColumn id="7" xr3:uid="{0ECB0B5E-176D-4229-A87A-C2A41E188E14}" name="Wk24 2025" dataDxfId="486"/>
+    <tableColumn id="8" xr3:uid="{C3FE39BE-3AA1-47B1-BB14-DB9B5D06E3D4}" name="Wk25 2025" dataDxfId="485"/>
+    <tableColumn id="9" xr3:uid="{E15F5E82-567D-4EA7-B0FF-0F0F5AA4EF07}" name="Wk26 2025" dataDxfId="484"/>
+    <tableColumn id="10" xr3:uid="{2F64D629-5535-490F-8B73-7C5E5946C95C}" name="Wk27 2025" dataDxfId="483"/>
+    <tableColumn id="11" xr3:uid="{A7D2AA51-7E39-45EC-A1AF-3AD0ED7B4FEB}" name="Wk28 2025" dataDxfId="482"/>
+    <tableColumn id="12" xr3:uid="{5877E484-4A49-4F53-8DAD-69FC96E3C88B}" name="Wk29 2025" dataDxfId="481"/>
+    <tableColumn id="13" xr3:uid="{35F7EC93-39F3-424E-A574-8491DA11C419}" name="Wk30 2025" dataDxfId="480"/>
+    <tableColumn id="14" xr3:uid="{D12E41AC-2CF4-45BF-BA33-6541F8092902}" name="Wk31 2025" dataDxfId="479"/>
+    <tableColumn id="15" xr3:uid="{AC2E1D16-8999-4552-AFCA-093F0E20266C}" name="Wk32 2025" dataDxfId="478"/>
+    <tableColumn id="16" xr3:uid="{B0ECF92A-CEE6-42ED-994E-7CEC6ED0C3FF}" name="Wk33 2025" dataDxfId="477"/>
+    <tableColumn id="17" xr3:uid="{252E88F5-331D-4D1D-A862-965D7EE83B14}" name="Wk34 2025" dataDxfId="476"/>
+    <tableColumn id="18" xr3:uid="{3F1619A4-1F4A-4AA3-B78F-CC17B4219BF7}" name="Wk35 2025" dataDxfId="475"/>
+    <tableColumn id="19" xr3:uid="{D37CF251-9CBA-47CF-90F3-9832F6491757}" name="Wk36 2025" dataDxfId="474"/>
+    <tableColumn id="20" xr3:uid="{2B42A392-F058-4B55-840D-45F390CA40BD}" name="Wk37 2025" dataDxfId="473"/>
+    <tableColumn id="21" xr3:uid="{F8B2B06E-1C89-4881-B690-FDA929360DE4}" name="Wk38 2025" dataDxfId="472"/>
+    <tableColumn id="22" xr3:uid="{984EE42D-9ECD-4A41-ABB7-77EFB728499E}" name="Wk39 2025" dataDxfId="471"/>
+    <tableColumn id="23" xr3:uid="{D783F65F-027D-40A3-930F-1ABE09D70996}" name="Wk40 2025" dataDxfId="470" dataCellStyle="Percent"/>
+    <tableColumn id="24" xr3:uid="{B1150C25-BBE4-4842-9B98-8CEB5DBE6AB1}" name="Wk41 2025" dataDxfId="469" dataCellStyle="Percent"/>
+    <tableColumn id="25" xr3:uid="{264979D8-1A3C-4E70-BF08-BCA8F44DD4E9}" name="Wk42 2025" dataDxfId="468" dataCellStyle="Percent"/>
+    <tableColumn id="26" xr3:uid="{7E03177B-2FD1-48AD-8020-48B71FDE6168}" name="Wk43 2025" dataDxfId="467" dataCellStyle="Percent"/>
+    <tableColumn id="27" xr3:uid="{47463794-0CBF-48E7-8A49-18A15ED419B1}" name="Wk44 2025" dataDxfId="466" dataCellStyle="Percent"/>
+    <tableColumn id="28" xr3:uid="{6D71255E-0304-4768-B806-1C188309AC23}" name="Wk45 2025" dataDxfId="465" dataCellStyle="Percent"/>
+    <tableColumn id="29" xr3:uid="{7B2ABC70-6901-4C50-9545-797DA7521C0A}" name="Wk46 2025" dataDxfId="464" dataCellStyle="Percent"/>
+    <tableColumn id="30" xr3:uid="{82BAECB3-50F7-49AE-BA46-AE7F37B085F7}" name="Wk47 2025" dataDxfId="463" dataCellStyle="Percent"/>
+    <tableColumn id="31" xr3:uid="{2764F785-0591-433A-959E-348BC8C85FB1}" name="Wk48 2025" dataDxfId="462" dataCellStyle="Percent"/>
+    <tableColumn id="32" xr3:uid="{5C934707-29EC-42D2-8D2C-B4160115F94D}" name="Wk49 2025" dataDxfId="461" dataCellStyle="Percent"/>
+    <tableColumn id="33" xr3:uid="{2DC6649A-600D-4B9A-B55D-8C8AD53DE891}" name="Wk50 2025" dataDxfId="460" dataCellStyle="Percent"/>
+    <tableColumn id="34" xr3:uid="{59F6FC88-B0E8-4E7F-BC1F-8926D8DB3525}" name="Wk51 2025" dataDxfId="459" dataCellStyle="Percent"/>
+    <tableColumn id="35" xr3:uid="{20AC0F5D-7547-431A-A70C-0C9ED683E230}" name="Wk52 2025" dataDxfId="458" dataCellStyle="Percent"/>
+    <tableColumn id="36" xr3:uid="{36F0C266-29AD-4FF9-B5F6-98E9E45CB123}" name="Wk 1 2026" dataDxfId="457" dataCellStyle="Percent"/>
+    <tableColumn id="37" xr3:uid="{338F823B-1750-4E1B-8067-969D7F77D0FF}" name="Wk 2 2026" dataDxfId="456" dataCellStyle="Percent"/>
+    <tableColumn id="38" xr3:uid="{21594A9B-C8AF-47BE-8004-34E3369173DE}" name="Wk 3 2026" dataDxfId="455" dataCellStyle="Percent"/>
+    <tableColumn id="39" xr3:uid="{D5F2887D-0DD4-4D96-9934-12684CBE26AF}" name="Wk 4 2026" dataDxfId="454" dataCellStyle="Percent"/>
+    <tableColumn id="40" xr3:uid="{FD966E31-4260-43EC-AD95-18BC9C146A4D}" name="Wk 5 2026" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="41" xr3:uid="{3E17D987-866E-4E6B-898A-E56A11ACA7BE}" name="Wk 6 2026" dataDxfId="453" dataCellStyle="Percent"/>
+    <tableColumn id="42" xr3:uid="{F695E36B-28E0-4EEC-B21A-45718DE82759}" name="Wk 7 2026" dataDxfId="452" dataCellStyle="Percent"/>
+    <tableColumn id="43" xr3:uid="{3C5FA813-A8E5-42D2-8E1C-65F19FEB108D}" name="Wk 8 2026" dataDxfId="451" dataCellStyle="Percent"/>
+    <tableColumn id="44" xr3:uid="{40450379-2F63-42C8-BDE4-CC381D409F01}" name="Wk 9 2026" dataDxfId="450" dataCellStyle="Percent"/>
+    <tableColumn id="45" xr3:uid="{959A18B3-226B-47B6-AC9D-324E60AB7335}" name="Wk 10 2026" dataDxfId="449" dataCellStyle="Percent"/>
+    <tableColumn id="46" xr3:uid="{718656E3-6EAB-4FEE-9805-4D7E7CA08D95}" name="Wk 11 2026" dataDxfId="448" dataCellStyle="Percent"/>
+    <tableColumn id="47" xr3:uid="{F4EED23F-2153-4495-93A6-0AE6352E93D2}" name="Wk 12 2026" dataDxfId="447" dataCellStyle="Percent"/>
+    <tableColumn id="48" xr3:uid="{50D6A3A5-3656-4E8A-85EC-014541A36615}" name="Wk 13 2026" dataDxfId="446" dataCellStyle="Percent"/>
+    <tableColumn id="49" xr3:uid="{7B8CAEA9-E4F7-4AFC-B363-D9DA4DD34E59}" name="Wk 14 2026" dataDxfId="445" dataCellStyle="Percent"/>
+    <tableColumn id="50" xr3:uid="{3E150CC9-84DD-4984-BA62-40D2355AA88E}" name="Wk 15 2026" dataDxfId="444" dataCellStyle="Percent"/>
+    <tableColumn id="51" xr3:uid="{9DAA22D5-D353-43D8-AEFB-493F9DC3B04E}" name="Wk 16 2026" dataDxfId="443" dataCellStyle="Percent"/>
+    <tableColumn id="52" xr3:uid="{3FD7A65B-632E-47FC-9A40-837CDA2763F2}" name="Wk 17 2026" dataDxfId="442" dataCellStyle="Percent"/>
+    <tableColumn id="53" xr3:uid="{18D37E87-2462-428E-A1C5-3AF89CBE351B}" name="Wk 18 2026" dataDxfId="441" dataCellStyle="Percent"/>
+    <tableColumn id="54" xr3:uid="{759D783E-2251-4AC0-BEAD-70CE7CA973E8}" name="Wk 19 2026" dataDxfId="440" dataCellStyle="Percent"/>
+    <tableColumn id="55" xr3:uid="{189BFD1D-5F97-4032-9626-96C1DD1ABF89}" name="Wk 20 2026" dataDxfId="439" dataCellStyle="Percent"/>
+    <tableColumn id="56" xr3:uid="{C4EF5625-E6E2-403E-A0A0-D31419673640}" name="Wk 21 2026" dataDxfId="438" dataCellStyle="Percent"/>
+    <tableColumn id="57" xr3:uid="{8555CA77-8EFB-4CA3-B5EF-7217EBF33553}" name="Wk 22 2026" dataDxfId="437" dataCellStyle="Percent"/>
+    <tableColumn id="58" xr3:uid="{C01E6A09-AB75-4A53-82BE-C0D77347E41B}" name="Wk 23 2026" dataDxfId="436" dataCellStyle="Percent"/>
+    <tableColumn id="59" xr3:uid="{80901ADD-FB23-458E-A355-FA8531334766}" name="Wk 24 2026" dataDxfId="435" dataCellStyle="Percent"/>
+    <tableColumn id="60" xr3:uid="{BEB995A6-53E6-4C56-9FCE-24C39723C622}" name="Wk 25 2026" dataDxfId="434" dataCellStyle="Percent"/>
+    <tableColumn id="61" xr3:uid="{905B51AE-0664-4B76-A24B-7F74A047D11F}" name="Wk 26 2026" dataDxfId="433" dataCellStyle="Percent"/>
+    <tableColumn id="62" xr3:uid="{6C89C269-10B4-4202-89E8-1DE1D3BF3C08}" name="Wk 27 2026" dataDxfId="432" dataCellStyle="Percent"/>
+    <tableColumn id="63" xr3:uid="{72C7ACA0-0D3B-4C6D-BE88-EE8728D56C1B}" name="Wk 28 2026" dataDxfId="431" dataCellStyle="Percent"/>
+    <tableColumn id="64" xr3:uid="{D0F1B34E-B2D8-4CA2-B633-4BD4E8D7E676}" name="Wk 29 2026" dataDxfId="430" dataCellStyle="Percent"/>
+    <tableColumn id="65" xr3:uid="{164D3D6B-4F1C-47BC-8C3A-42D8B0DACD02}" name="Wk 30 2026" dataDxfId="429" dataCellStyle="Percent"/>
+    <tableColumn id="66" xr3:uid="{02BF2A00-88FD-4084-B2E6-9446A001CC43}" name="Wk 31 2026" dataDxfId="428" dataCellStyle="Percent"/>
+    <tableColumn id="67" xr3:uid="{C5EFD435-0242-4482-9D98-D4CC41A6A7AF}" name="Wk 32 2026" dataDxfId="427" dataCellStyle="Percent"/>
+    <tableColumn id="68" xr3:uid="{1CE6F0BC-F07B-405D-90AE-CC1C4F8ADF52}" name="Wk 33 2026" dataDxfId="426" dataCellStyle="Percent"/>
+    <tableColumn id="69" xr3:uid="{2A3A92FD-16CC-4105-959F-64B83C997902}" name="Wk 34 2026" dataDxfId="425" dataCellStyle="Percent"/>
+    <tableColumn id="70" xr3:uid="{8116DA30-D266-4207-ACE3-7C14945389DA}" name="Wk 35 2026" dataDxfId="424" dataCellStyle="Percent"/>
+    <tableColumn id="71" xr3:uid="{CAECEBB9-A748-4769-857B-3342E4C729FF}" name="Wk 36 2026" dataDxfId="423" dataCellStyle="Percent"/>
+    <tableColumn id="72" xr3:uid="{8CB2587A-2C8D-4A3E-BBB2-D6E711E52ED2}" name="Wk 37 2026" dataDxfId="422" dataCellStyle="Percent"/>
+    <tableColumn id="73" xr3:uid="{71C06ADC-AA5D-4D8E-9311-76770D90E06C}" name="Wk 38 2026" dataDxfId="421" dataCellStyle="Percent"/>
+    <tableColumn id="74" xr3:uid="{48198F49-F131-4C76-A1D2-27CA0FD939FD}" name="Wk 39 2026" dataDxfId="420" dataCellStyle="Percent"/>
+    <tableColumn id="75" xr3:uid="{5D0AB91D-9077-4870-958C-030B842625A4}" name="Wk 40 2026" dataDxfId="419" dataCellStyle="Percent"/>
+    <tableColumn id="76" xr3:uid="{E5775D4C-09A6-4222-9DCC-7844B3E81D90}" name="Wk 41 2026" dataDxfId="418" dataCellStyle="Percent"/>
+    <tableColumn id="77" xr3:uid="{C1BF29EC-BACC-454D-ABEC-E327A1CA30C3}" name="Wk 42 2026" dataDxfId="417" dataCellStyle="Percent"/>
+    <tableColumn id="78" xr3:uid="{19E0BAB5-42D8-4B8E-AA57-D0E3F9A7C34E}" name="Wk 43 2026" dataDxfId="416" dataCellStyle="Percent"/>
+    <tableColumn id="79" xr3:uid="{BB9CE3BE-C0D0-49D9-BD2A-9FAEEEB31D6D}" name="Wk 44 2026" dataDxfId="415" dataCellStyle="Percent"/>
+    <tableColumn id="80" xr3:uid="{30D70071-2E17-4433-BAEC-65EC8EC8D3E9}" name="Wk 45 2026" dataDxfId="414" dataCellStyle="Percent"/>
+    <tableColumn id="81" xr3:uid="{E63760E7-9CC6-4AAC-8114-7FBAE4AA0B55}" name="Wk 46 2026" dataDxfId="413" dataCellStyle="Percent"/>
+    <tableColumn id="82" xr3:uid="{21ACBE91-92F3-457E-B81E-FFF488FDE917}" name="Wk 47 2026" dataDxfId="412" dataCellStyle="Percent"/>
+    <tableColumn id="83" xr3:uid="{437FA868-1251-45EB-ABBD-1C60F4AFB117}" name="Wk 48 2026" dataDxfId="411" dataCellStyle="Percent"/>
+    <tableColumn id="84" xr3:uid="{16C16432-FBA2-4A1E-9070-92F4447C89E1}" name="Wk 49 2026" dataDxfId="410" dataCellStyle="Percent"/>
+    <tableColumn id="85" xr3:uid="{88BD1C03-0653-480B-826D-EFF52AC09DC1}" name="Wk 50 2026" dataDxfId="409" dataCellStyle="Percent"/>
+    <tableColumn id="86" xr3:uid="{6F6ABEE0-3EDF-4F28-AF74-86A5B8128E83}" name="Wk 51 2026" dataDxfId="408" dataCellStyle="Percent"/>
+    <tableColumn id="87" xr3:uid="{12A48B29-AF32-4A2A-B981-6338D988BBA3}" name="Wk 52 2026" dataDxfId="407" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24684,325 +24712,325 @@
   </sortState>
   <tableColumns count="87">
     <tableColumn id="1" xr3:uid="{6F7AD7A3-0B00-4DE0-8395-BF95BFCFC306}" name="MP"/>
-    <tableColumn id="2" xr3:uid="{82AE0BF2-643C-47C7-A295-BF7F2E090858}" name="Wk19 2025" dataDxfId="410"/>
-    <tableColumn id="3" xr3:uid="{D1A45108-D473-4B17-AF60-98FCC7B30E60}" name="Wk20 2025" dataDxfId="409"/>
-    <tableColumn id="4" xr3:uid="{64169490-74A4-4F4B-8C39-B12C54B05546}" name="Wk21 2025" dataDxfId="408"/>
-    <tableColumn id="5" xr3:uid="{0633B441-4546-4F48-B71F-3D03EE2106AB}" name="Wk22 2025" dataDxfId="407"/>
-    <tableColumn id="6" xr3:uid="{D2073EA0-C84D-451D-AEC0-DC18EAA20496}" name="Wk23 2025" dataDxfId="406"/>
-    <tableColumn id="7" xr3:uid="{44955FBC-F8D7-4ACD-B86F-38D1D8AE6408}" name="Wk24 2025" dataDxfId="405"/>
-    <tableColumn id="8" xr3:uid="{E14795C9-BC98-4465-880D-B83B173A7FAD}" name="Wk25 2025" dataDxfId="404"/>
-    <tableColumn id="9" xr3:uid="{64C9C2E1-4EBC-4BB2-999F-2F014584D5DD}" name="Wk26 2025" dataDxfId="403"/>
-    <tableColumn id="10" xr3:uid="{79022431-D70F-4BFF-A33B-3A15A0DF8200}" name="Wk27 2025" dataDxfId="402"/>
-    <tableColumn id="11" xr3:uid="{992EDDF4-BC56-4158-A699-5DE2FD1BDBEF}" name="Wk28 2025" dataDxfId="401"/>
-    <tableColumn id="12" xr3:uid="{B95F51E2-765E-4B30-B288-C20129A915AB}" name="Wk29 2025" dataDxfId="400"/>
-    <tableColumn id="13" xr3:uid="{8352C3BE-8A8C-452B-BDBB-B3D4AA723795}" name="Wk30 2025" dataDxfId="399"/>
-    <tableColumn id="14" xr3:uid="{3D2CC433-074B-44BB-9600-3B9A96817DB3}" name="Wk31 2025" dataDxfId="398"/>
-    <tableColumn id="15" xr3:uid="{1CBC213C-0913-4ACF-A9EA-403F43DDC321}" name="Wk32 2025" dataDxfId="397"/>
-    <tableColumn id="16" xr3:uid="{80B01D3F-F5F4-4EAE-8D58-0592585472FD}" name="Wk33 2025" dataDxfId="396"/>
-    <tableColumn id="17" xr3:uid="{F8804579-0EFF-4577-A7E2-4B107966C748}" name="Wk34 2025" dataDxfId="395"/>
-    <tableColumn id="18" xr3:uid="{9CD12014-3DC6-4EB5-8989-2A80D3B3DB9C}" name="Wk35 2025" dataDxfId="394"/>
-    <tableColumn id="19" xr3:uid="{DD728F30-644B-4534-92B2-B4FD8B75021B}" name="Wk36 2025" dataDxfId="393"/>
-    <tableColumn id="20" xr3:uid="{09E0B769-20D5-4B93-8631-D012F554AA7E}" name="Wk37 2025" dataDxfId="392"/>
-    <tableColumn id="21" xr3:uid="{2C9E2965-EF47-4023-B252-3874AA50BE57}" name="Wk38 2025" dataDxfId="391"/>
-    <tableColumn id="22" xr3:uid="{1F700844-D8D7-4D3A-A3D5-62DD7273CB7F}" name="Wk39 2025" dataDxfId="390"/>
-    <tableColumn id="23" xr3:uid="{1CFD1B1A-F41A-4886-91E4-788C3F16ED83}" name="Wk40 2025" dataDxfId="389"/>
-    <tableColumn id="24" xr3:uid="{8998402E-2604-4177-9891-12012C80FFC3}" name="Wk41 2025" dataDxfId="388"/>
-    <tableColumn id="25" xr3:uid="{B32BF0EB-CFB8-4205-AF74-D140A89DB6EB}" name="Wk42 2025" dataDxfId="387"/>
-    <tableColumn id="26" xr3:uid="{8FF2928C-9A47-4EDD-BE8B-93C3B8B6CD3F}" name="Wk43 2025" dataDxfId="386"/>
-    <tableColumn id="27" xr3:uid="{0FF56462-5727-4D97-B4B7-C886DE4A70BB}" name="Wk44 2025" dataDxfId="385"/>
-    <tableColumn id="28" xr3:uid="{050C6E74-83D6-4576-BBD7-17B35AC028A3}" name="Wk45 2025" dataDxfId="384"/>
-    <tableColumn id="29" xr3:uid="{D555B4E6-9948-4427-BC22-591177795635}" name="Wk46 2025" dataDxfId="383"/>
-    <tableColumn id="30" xr3:uid="{DEEC19EC-977D-4EC4-A0B0-CA508661C303}" name="Wk47 2025" dataDxfId="382"/>
-    <tableColumn id="31" xr3:uid="{CAE548B3-2CFA-4DB9-8C63-228F94D909C1}" name="Wk48 2025" dataDxfId="381"/>
-    <tableColumn id="32" xr3:uid="{3F320FCA-92BE-4897-BF4C-4F9E36E925EC}" name="Wk49 2025" dataDxfId="380"/>
-    <tableColumn id="33" xr3:uid="{31B76E02-88F4-4D39-8B56-6E282B47923E}" name="Wk50 2025" dataDxfId="379"/>
-    <tableColumn id="34" xr3:uid="{64443C4E-D44E-4126-991C-CA6E6A3B219C}" name="Wk51 2025" dataDxfId="378"/>
-    <tableColumn id="35" xr3:uid="{2353AEB6-B866-43D8-BD87-690FE9C9AD8A}" name="Wk52 2025" dataDxfId="377"/>
-    <tableColumn id="36" xr3:uid="{215B08D4-C31A-4DAE-B203-1C7EEEE6312D}" name="Wk 1 2026" dataDxfId="376">
+    <tableColumn id="2" xr3:uid="{82AE0BF2-643C-47C7-A295-BF7F2E090858}" name="Wk19 2025" dataDxfId="406"/>
+    <tableColumn id="3" xr3:uid="{D1A45108-D473-4B17-AF60-98FCC7B30E60}" name="Wk20 2025" dataDxfId="405"/>
+    <tableColumn id="4" xr3:uid="{64169490-74A4-4F4B-8C39-B12C54B05546}" name="Wk21 2025" dataDxfId="404"/>
+    <tableColumn id="5" xr3:uid="{0633B441-4546-4F48-B71F-3D03EE2106AB}" name="Wk22 2025" dataDxfId="403"/>
+    <tableColumn id="6" xr3:uid="{D2073EA0-C84D-451D-AEC0-DC18EAA20496}" name="Wk23 2025" dataDxfId="402"/>
+    <tableColumn id="7" xr3:uid="{44955FBC-F8D7-4ACD-B86F-38D1D8AE6408}" name="Wk24 2025" dataDxfId="401"/>
+    <tableColumn id="8" xr3:uid="{E14795C9-BC98-4465-880D-B83B173A7FAD}" name="Wk25 2025" dataDxfId="400"/>
+    <tableColumn id="9" xr3:uid="{64C9C2E1-4EBC-4BB2-999F-2F014584D5DD}" name="Wk26 2025" dataDxfId="399"/>
+    <tableColumn id="10" xr3:uid="{79022431-D70F-4BFF-A33B-3A15A0DF8200}" name="Wk27 2025" dataDxfId="398"/>
+    <tableColumn id="11" xr3:uid="{992EDDF4-BC56-4158-A699-5DE2FD1BDBEF}" name="Wk28 2025" dataDxfId="397"/>
+    <tableColumn id="12" xr3:uid="{B95F51E2-765E-4B30-B288-C20129A915AB}" name="Wk29 2025" dataDxfId="396"/>
+    <tableColumn id="13" xr3:uid="{8352C3BE-8A8C-452B-BDBB-B3D4AA723795}" name="Wk30 2025" dataDxfId="395"/>
+    <tableColumn id="14" xr3:uid="{3D2CC433-074B-44BB-9600-3B9A96817DB3}" name="Wk31 2025" dataDxfId="394"/>
+    <tableColumn id="15" xr3:uid="{1CBC213C-0913-4ACF-A9EA-403F43DDC321}" name="Wk32 2025" dataDxfId="393"/>
+    <tableColumn id="16" xr3:uid="{80B01D3F-F5F4-4EAE-8D58-0592585472FD}" name="Wk33 2025" dataDxfId="392"/>
+    <tableColumn id="17" xr3:uid="{F8804579-0EFF-4577-A7E2-4B107966C748}" name="Wk34 2025" dataDxfId="391"/>
+    <tableColumn id="18" xr3:uid="{9CD12014-3DC6-4EB5-8989-2A80D3B3DB9C}" name="Wk35 2025" dataDxfId="390"/>
+    <tableColumn id="19" xr3:uid="{DD728F30-644B-4534-92B2-B4FD8B75021B}" name="Wk36 2025" dataDxfId="389"/>
+    <tableColumn id="20" xr3:uid="{09E0B769-20D5-4B93-8631-D012F554AA7E}" name="Wk37 2025" dataDxfId="388"/>
+    <tableColumn id="21" xr3:uid="{2C9E2965-EF47-4023-B252-3874AA50BE57}" name="Wk38 2025" dataDxfId="387"/>
+    <tableColumn id="22" xr3:uid="{1F700844-D8D7-4D3A-A3D5-62DD7273CB7F}" name="Wk39 2025" dataDxfId="386"/>
+    <tableColumn id="23" xr3:uid="{1CFD1B1A-F41A-4886-91E4-788C3F16ED83}" name="Wk40 2025" dataDxfId="385"/>
+    <tableColumn id="24" xr3:uid="{8998402E-2604-4177-9891-12012C80FFC3}" name="Wk41 2025" dataDxfId="384"/>
+    <tableColumn id="25" xr3:uid="{B32BF0EB-CFB8-4205-AF74-D140A89DB6EB}" name="Wk42 2025" dataDxfId="383"/>
+    <tableColumn id="26" xr3:uid="{8FF2928C-9A47-4EDD-BE8B-93C3B8B6CD3F}" name="Wk43 2025" dataDxfId="382"/>
+    <tableColumn id="27" xr3:uid="{0FF56462-5727-4D97-B4B7-C886DE4A70BB}" name="Wk44 2025" dataDxfId="381"/>
+    <tableColumn id="28" xr3:uid="{050C6E74-83D6-4576-BBD7-17B35AC028A3}" name="Wk45 2025" dataDxfId="380"/>
+    <tableColumn id="29" xr3:uid="{D555B4E6-9948-4427-BC22-591177795635}" name="Wk46 2025" dataDxfId="379"/>
+    <tableColumn id="30" xr3:uid="{DEEC19EC-977D-4EC4-A0B0-CA508661C303}" name="Wk47 2025" dataDxfId="378"/>
+    <tableColumn id="31" xr3:uid="{CAE548B3-2CFA-4DB9-8C63-228F94D909C1}" name="Wk48 2025" dataDxfId="377"/>
+    <tableColumn id="32" xr3:uid="{3F320FCA-92BE-4897-BF4C-4F9E36E925EC}" name="Wk49 2025" dataDxfId="376"/>
+    <tableColumn id="33" xr3:uid="{31B76E02-88F4-4D39-8B56-6E282B47923E}" name="Wk50 2025" dataDxfId="375"/>
+    <tableColumn id="34" xr3:uid="{64443C4E-D44E-4126-991C-CA6E6A3B219C}" name="Wk51 2025" dataDxfId="374"/>
+    <tableColumn id="35" xr3:uid="{2353AEB6-B866-43D8-BD87-690FE9C9AD8A}" name="Wk52 2025" dataDxfId="373"/>
+    <tableColumn id="36" xr3:uid="{215B08D4-C31A-4DAE-B203-1C7EEEE6312D}" name="Wk 1 2026" dataDxfId="372">
       <calculatedColumnFormula>AK15*AK26*AK37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{BF76241F-CA8C-4532-81F8-FF349C0D3DDB}" name="Wk 2 2026" dataDxfId="375">
+    <tableColumn id="37" xr3:uid="{BF76241F-CA8C-4532-81F8-FF349C0D3DDB}" name="Wk 2 2026" dataDxfId="371">
       <calculatedColumnFormula>AL15*AL26*AL37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{315932D2-9717-4A68-94B3-0E28B012C763}" name="Wk 3 2026" dataDxfId="374">
+    <tableColumn id="38" xr3:uid="{315932D2-9717-4A68-94B3-0E28B012C763}" name="Wk 3 2026" dataDxfId="370">
       <calculatedColumnFormula>AM15*AM26*AM37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{32F496E4-0F53-4CCC-A06F-7B4AF13E7063}" name="Wk 4 2026" dataDxfId="373">
+    <tableColumn id="39" xr3:uid="{32F496E4-0F53-4CCC-A06F-7B4AF13E7063}" name="Wk 4 2026" dataDxfId="369">
       <calculatedColumnFormula>AN15*AN26*AN37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{E17B134F-B2B4-4593-91A7-B3BC8653A14E}" name="Wk 5 2026" dataDxfId="372">
+    <tableColumn id="40" xr3:uid="{E17B134F-B2B4-4593-91A7-B3BC8653A14E}" name="Wk 5 2026" dataDxfId="368">
       <calculatedColumnFormula>AO15*AO26*AO37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" xr3:uid="{9903557C-C4BE-4F30-BC67-4EFD77E34CD8}" name="Wk 6 2026" dataDxfId="371">
+    <tableColumn id="41" xr3:uid="{9903557C-C4BE-4F30-BC67-4EFD77E34CD8}" name="Wk 6 2026" dataDxfId="367">
       <calculatedColumnFormula>AP15*AP26*AP37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="42" xr3:uid="{F356BF98-D032-4987-A960-8A06217DF85E}" name="Wk 7 2026" dataDxfId="370">
+    <tableColumn id="42" xr3:uid="{F356BF98-D032-4987-A960-8A06217DF85E}" name="Wk 7 2026" dataDxfId="366">
       <calculatedColumnFormula>AQ15*AQ26*AQ37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{54FC261B-C916-49E1-9164-CAE938C3509E}" name="Wk 8 2026" dataDxfId="369">
+    <tableColumn id="43" xr3:uid="{54FC261B-C916-49E1-9164-CAE938C3509E}" name="Wk 8 2026" dataDxfId="365">
       <calculatedColumnFormula>AR15*AR26*AR37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="44" xr3:uid="{7973A7F7-2C6E-4E78-BA49-5F0AF268823C}" name="Wk 9 2026" dataDxfId="368">
+    <tableColumn id="44" xr3:uid="{7973A7F7-2C6E-4E78-BA49-5F0AF268823C}" name="Wk 9 2026" dataDxfId="364">
       <calculatedColumnFormula>AS15*AS26*AS37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="45" xr3:uid="{00718727-9536-45D5-A31D-B9A51E6A7670}" name="Wk 10 2026" dataDxfId="367">
+    <tableColumn id="45" xr3:uid="{00718727-9536-45D5-A31D-B9A51E6A7670}" name="Wk 10 2026" dataDxfId="363">
       <calculatedColumnFormula>AT15*AT26*AT37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="46" xr3:uid="{5558F1C9-6B0F-471F-88A0-3781D6AC7008}" name="Wk 11 2026" dataDxfId="366"/>
-    <tableColumn id="47" xr3:uid="{81D07BF5-30B7-4481-B2EA-564548D5F057}" name="Wk 12 2026" dataDxfId="365"/>
-    <tableColumn id="48" xr3:uid="{DA2E7AC0-ECC3-4A92-81DE-B3D13A9336D3}" name="Wk 13 2026" dataDxfId="364"/>
-    <tableColumn id="49" xr3:uid="{F3FB5C80-0D63-44B2-B201-6BE98CDE8557}" name="Wk 14 2026" dataDxfId="363"/>
-    <tableColumn id="50" xr3:uid="{31BE2037-E8D4-46EA-8BDD-462364A69815}" name="Wk 15 2026" dataDxfId="362"/>
-    <tableColumn id="51" xr3:uid="{A2BD5682-969C-4ED5-B03A-1A0D2AAB6841}" name="Wk 16 2026" dataDxfId="361"/>
-    <tableColumn id="52" xr3:uid="{D4E5776D-1260-4A98-9352-6F6D02EE6EC6}" name="Wk 17 2026" dataDxfId="360"/>
-    <tableColumn id="53" xr3:uid="{7838DC5F-AB19-4674-A637-471E81E935C9}" name="Wk 18 2026" dataDxfId="359"/>
-    <tableColumn id="54" xr3:uid="{3E47D739-5211-46A8-A682-1B683AED9B06}" name="Wk 19 2026" dataDxfId="358"/>
-    <tableColumn id="55" xr3:uid="{6ABF9A2D-D6D0-4FE8-BD36-071136DF4D42}" name="Wk 20 2026" dataDxfId="357"/>
-    <tableColumn id="56" xr3:uid="{6F68460E-C749-4E9C-85AC-7ACA683CD5F4}" name="Wk 21 2026" dataDxfId="356"/>
-    <tableColumn id="57" xr3:uid="{94023E84-FC5E-4D09-8E87-25D731C1CA53}" name="Wk 22 2026" dataDxfId="355"/>
-    <tableColumn id="58" xr3:uid="{D7916816-E553-4F2D-8AA1-8B73AE689CBE}" name="Wk 23 2026" dataDxfId="354"/>
-    <tableColumn id="59" xr3:uid="{FB91BBB5-D7BA-4F4C-87E9-19F8E811C8DF}" name="Wk 24 2026" dataDxfId="353"/>
-    <tableColumn id="60" xr3:uid="{160E7DB0-160A-4EEC-99A8-7099D5E36A98}" name="Wk 25 2026" dataDxfId="352"/>
-    <tableColumn id="61" xr3:uid="{1DF41442-370E-4036-BF10-C41DD3F86F8D}" name="Wk 26 2026" dataDxfId="351"/>
-    <tableColumn id="62" xr3:uid="{777383E0-737E-41ED-990E-AA49E980420D}" name="Wk 27 2026" dataDxfId="350"/>
-    <tableColumn id="63" xr3:uid="{118EE8B6-61F5-4F11-862F-4F5A9A3F209D}" name="Wk 28 2026" dataDxfId="349"/>
-    <tableColumn id="64" xr3:uid="{92636CCD-AE3A-4C24-8EF7-40B16C39CE29}" name="Wk 29 2026" dataDxfId="348"/>
-    <tableColumn id="65" xr3:uid="{CA7D1538-48D0-45B3-92D4-EB88707FBC0E}" name="Wk 30 2026" dataDxfId="347"/>
-    <tableColumn id="66" xr3:uid="{80C36D3A-590C-4889-B412-79A1060EF41C}" name="Wk 31 2026" dataDxfId="346"/>
-    <tableColumn id="67" xr3:uid="{A229E8B6-C900-4967-89CD-263ED049DDEE}" name="Wk 32 2026" dataDxfId="345"/>
-    <tableColumn id="68" xr3:uid="{CC75C4AF-50E9-4F08-8A63-B1CD63F7A456}" name="Wk 33 2026" dataDxfId="344"/>
-    <tableColumn id="69" xr3:uid="{E00D699B-3BF1-4B96-A41F-1C7D94B04B54}" name="Wk 34 2026" dataDxfId="343"/>
-    <tableColumn id="70" xr3:uid="{F058CC15-5D67-4E65-829C-E0DFA3D6E472}" name="Wk 35 2026" dataDxfId="342"/>
-    <tableColumn id="71" xr3:uid="{B60EB0D0-64FC-4EE6-BDA5-7E4108469F12}" name="Wk 36 2026" dataDxfId="341"/>
-    <tableColumn id="72" xr3:uid="{E526BAC9-2190-4412-BE67-E9CF22014CA4}" name="Wk 37 2026" dataDxfId="340"/>
-    <tableColumn id="73" xr3:uid="{E83D517C-3CBB-41DE-B9E7-EBA588A6CAEE}" name="Wk 38 2026" dataDxfId="339"/>
-    <tableColumn id="74" xr3:uid="{55BFABC1-4178-45DD-A896-27C068139EA8}" name="Wk 39 2026" dataDxfId="338"/>
-    <tableColumn id="75" xr3:uid="{D7BB7615-FEC1-46C1-84B9-FB3F73AAC80C}" name="Wk 40 2026" dataDxfId="337"/>
-    <tableColumn id="76" xr3:uid="{D3945D6B-0E4C-47F2-AAC8-94EB6A31D77E}" name="Wk 41 2026" dataDxfId="336"/>
-    <tableColumn id="77" xr3:uid="{DCCE0153-DE92-424D-9C05-74F3CE412ACD}" name="Wk 42 2026" dataDxfId="335"/>
-    <tableColumn id="78" xr3:uid="{87223B2A-8EA0-4CD9-889D-26364DF683BB}" name="Wk 43 2026" dataDxfId="334"/>
-    <tableColumn id="79" xr3:uid="{C65EA61A-42A5-415F-8BF5-0BC0C4933507}" name="Wk 44 2026" dataDxfId="333"/>
-    <tableColumn id="80" xr3:uid="{35112091-BE1C-49BC-BBCF-DBB6539B0A6A}" name="Wk 45 2026" dataDxfId="332"/>
-    <tableColumn id="81" xr3:uid="{15480499-A158-493A-83DA-04E36B34A71A}" name="Wk 46 2026" dataDxfId="331"/>
-    <tableColumn id="82" xr3:uid="{03BCFECB-C4EA-4501-9287-8B5E353A4403}" name="Wk 47 2026" dataDxfId="330"/>
-    <tableColumn id="83" xr3:uid="{1843CFBA-F680-4990-8FE2-F2A7528747EF}" name="Wk 48 2026" dataDxfId="329"/>
-    <tableColumn id="84" xr3:uid="{26FF27B0-45AE-4D7B-80A7-128DF6F466EC}" name="Wk 49 2026" dataDxfId="328"/>
-    <tableColumn id="85" xr3:uid="{FBBCBBBC-332F-42C9-9FFC-3FE52724F052}" name="Wk 50 2026" dataDxfId="327"/>
-    <tableColumn id="86" xr3:uid="{92BECC55-7534-4C9C-AE28-829D72A18D5F}" name="Wk 51 2026" dataDxfId="326"/>
-    <tableColumn id="87" xr3:uid="{FA9411C3-37F9-40EE-A5DA-00EB785FEBFB}" name="Wk 52 2026" dataDxfId="325"/>
+    <tableColumn id="46" xr3:uid="{5558F1C9-6B0F-471F-88A0-3781D6AC7008}" name="Wk 11 2026" dataDxfId="362"/>
+    <tableColumn id="47" xr3:uid="{81D07BF5-30B7-4481-B2EA-564548D5F057}" name="Wk 12 2026" dataDxfId="361"/>
+    <tableColumn id="48" xr3:uid="{DA2E7AC0-ECC3-4A92-81DE-B3D13A9336D3}" name="Wk 13 2026" dataDxfId="360"/>
+    <tableColumn id="49" xr3:uid="{F3FB5C80-0D63-44B2-B201-6BE98CDE8557}" name="Wk 14 2026" dataDxfId="359"/>
+    <tableColumn id="50" xr3:uid="{31BE2037-E8D4-46EA-8BDD-462364A69815}" name="Wk 15 2026" dataDxfId="358"/>
+    <tableColumn id="51" xr3:uid="{A2BD5682-969C-4ED5-B03A-1A0D2AAB6841}" name="Wk 16 2026" dataDxfId="357"/>
+    <tableColumn id="52" xr3:uid="{D4E5776D-1260-4A98-9352-6F6D02EE6EC6}" name="Wk 17 2026" dataDxfId="356"/>
+    <tableColumn id="53" xr3:uid="{7838DC5F-AB19-4674-A637-471E81E935C9}" name="Wk 18 2026" dataDxfId="355"/>
+    <tableColumn id="54" xr3:uid="{3E47D739-5211-46A8-A682-1B683AED9B06}" name="Wk 19 2026" dataDxfId="354"/>
+    <tableColumn id="55" xr3:uid="{6ABF9A2D-D6D0-4FE8-BD36-071136DF4D42}" name="Wk 20 2026" dataDxfId="353"/>
+    <tableColumn id="56" xr3:uid="{6F68460E-C749-4E9C-85AC-7ACA683CD5F4}" name="Wk 21 2026" dataDxfId="352"/>
+    <tableColumn id="57" xr3:uid="{94023E84-FC5E-4D09-8E87-25D731C1CA53}" name="Wk 22 2026" dataDxfId="351"/>
+    <tableColumn id="58" xr3:uid="{D7916816-E553-4F2D-8AA1-8B73AE689CBE}" name="Wk 23 2026" dataDxfId="350"/>
+    <tableColumn id="59" xr3:uid="{FB91BBB5-D7BA-4F4C-87E9-19F8E811C8DF}" name="Wk 24 2026" dataDxfId="349"/>
+    <tableColumn id="60" xr3:uid="{160E7DB0-160A-4EEC-99A8-7099D5E36A98}" name="Wk 25 2026" dataDxfId="348"/>
+    <tableColumn id="61" xr3:uid="{1DF41442-370E-4036-BF10-C41DD3F86F8D}" name="Wk 26 2026" dataDxfId="347"/>
+    <tableColumn id="62" xr3:uid="{777383E0-737E-41ED-990E-AA49E980420D}" name="Wk 27 2026" dataDxfId="346"/>
+    <tableColumn id="63" xr3:uid="{118EE8B6-61F5-4F11-862F-4F5A9A3F209D}" name="Wk 28 2026" dataDxfId="345"/>
+    <tableColumn id="64" xr3:uid="{92636CCD-AE3A-4C24-8EF7-40B16C39CE29}" name="Wk 29 2026" dataDxfId="344"/>
+    <tableColumn id="65" xr3:uid="{CA7D1538-48D0-45B3-92D4-EB88707FBC0E}" name="Wk 30 2026" dataDxfId="343"/>
+    <tableColumn id="66" xr3:uid="{80C36D3A-590C-4889-B412-79A1060EF41C}" name="Wk 31 2026" dataDxfId="342"/>
+    <tableColumn id="67" xr3:uid="{A229E8B6-C900-4967-89CD-263ED049DDEE}" name="Wk 32 2026" dataDxfId="341"/>
+    <tableColumn id="68" xr3:uid="{CC75C4AF-50E9-4F08-8A63-B1CD63F7A456}" name="Wk 33 2026" dataDxfId="340"/>
+    <tableColumn id="69" xr3:uid="{E00D699B-3BF1-4B96-A41F-1C7D94B04B54}" name="Wk 34 2026" dataDxfId="339"/>
+    <tableColumn id="70" xr3:uid="{F058CC15-5D67-4E65-829C-E0DFA3D6E472}" name="Wk 35 2026" dataDxfId="338"/>
+    <tableColumn id="71" xr3:uid="{B60EB0D0-64FC-4EE6-BDA5-7E4108469F12}" name="Wk 36 2026" dataDxfId="337"/>
+    <tableColumn id="72" xr3:uid="{E526BAC9-2190-4412-BE67-E9CF22014CA4}" name="Wk 37 2026" dataDxfId="336"/>
+    <tableColumn id="73" xr3:uid="{E83D517C-3CBB-41DE-B9E7-EBA588A6CAEE}" name="Wk 38 2026" dataDxfId="335"/>
+    <tableColumn id="74" xr3:uid="{55BFABC1-4178-45DD-A896-27C068139EA8}" name="Wk 39 2026" dataDxfId="334"/>
+    <tableColumn id="75" xr3:uid="{D7BB7615-FEC1-46C1-84B9-FB3F73AAC80C}" name="Wk 40 2026" dataDxfId="333"/>
+    <tableColumn id="76" xr3:uid="{D3945D6B-0E4C-47F2-AAC8-94EB6A31D77E}" name="Wk 41 2026" dataDxfId="332"/>
+    <tableColumn id="77" xr3:uid="{DCCE0153-DE92-424D-9C05-74F3CE412ACD}" name="Wk 42 2026" dataDxfId="331"/>
+    <tableColumn id="78" xr3:uid="{87223B2A-8EA0-4CD9-889D-26364DF683BB}" name="Wk 43 2026" dataDxfId="330"/>
+    <tableColumn id="79" xr3:uid="{C65EA61A-42A5-415F-8BF5-0BC0C4933507}" name="Wk 44 2026" dataDxfId="329"/>
+    <tableColumn id="80" xr3:uid="{35112091-BE1C-49BC-BBCF-DBB6539B0A6A}" name="Wk 45 2026" dataDxfId="328"/>
+    <tableColumn id="81" xr3:uid="{15480499-A158-493A-83DA-04E36B34A71A}" name="Wk 46 2026" dataDxfId="327"/>
+    <tableColumn id="82" xr3:uid="{03BCFECB-C4EA-4501-9287-8B5E353A4403}" name="Wk 47 2026" dataDxfId="326"/>
+    <tableColumn id="83" xr3:uid="{1843CFBA-F680-4990-8FE2-F2A7528747EF}" name="Wk 48 2026" dataDxfId="325"/>
+    <tableColumn id="84" xr3:uid="{26FF27B0-45AE-4D7B-80A7-128DF6F466EC}" name="Wk 49 2026" dataDxfId="324"/>
+    <tableColumn id="85" xr3:uid="{FBBCBBBC-332F-42C9-9FFC-3FE52724F052}" name="Wk 50 2026" dataDxfId="323"/>
+    <tableColumn id="86" xr3:uid="{92BECC55-7534-4C9C-AE28-829D72A18D5F}" name="Wk 51 2026" dataDxfId="322"/>
+    <tableColumn id="87" xr3:uid="{FA9411C3-37F9-40EE-A5DA-00EB785FEBFB}" name="Wk 52 2026" dataDxfId="321"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C223AE24-6038-4184-8476-A5B39BC0DE2B}" name="tblForecastTransits25" displayName="tblForecastTransits25" ref="B14:CJ20" totalsRowShown="0" headerRowDxfId="324" dataDxfId="322" headerRowBorderDxfId="323" tableBorderDxfId="321">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C223AE24-6038-4184-8476-A5B39BC0DE2B}" name="tblForecastTransits25" displayName="tblForecastTransits25" ref="B14:CJ20" totalsRowShown="0" headerRowDxfId="320" dataDxfId="318" headerRowBorderDxfId="319" tableBorderDxfId="317">
   <autoFilter ref="B14:CJ20" xr:uid="{22990427-97D6-4128-B413-6C553148C612}"/>
   <tableColumns count="87">
     <tableColumn id="1" xr3:uid="{90AF7D69-5FE9-4D3F-A8AB-B34F1E615FA7}" name="MP"/>
-    <tableColumn id="2" xr3:uid="{C2CE772C-B148-4D1F-99A4-E4B9B5D7C5B1}" name="Wk19 2025" dataDxfId="320"/>
-    <tableColumn id="3" xr3:uid="{A0DD27EA-24C9-4735-8521-C1BFE274BE0E}" name="Wk20 2025" dataDxfId="319"/>
-    <tableColumn id="4" xr3:uid="{4483A63E-2841-499A-8F6F-04265F3B4950}" name="Wk21 2025" dataDxfId="318"/>
-    <tableColumn id="5" xr3:uid="{4EF77BC7-8819-4D13-86DF-856DB47A9715}" name="Wk22 2025" dataDxfId="317"/>
-    <tableColumn id="6" xr3:uid="{2F2C0467-26DF-407B-99A5-8D2F93FFD54D}" name="Wk23 2025" dataDxfId="316"/>
-    <tableColumn id="7" xr3:uid="{F520AFFE-1894-48D5-9D25-3A0DC5D76E82}" name="Wk24 2025" dataDxfId="315"/>
-    <tableColumn id="8" xr3:uid="{A229F7FD-0149-49DA-87D3-5DD9C91931E6}" name="Wk25 2025" dataDxfId="314"/>
-    <tableColumn id="9" xr3:uid="{21BFCA83-1B04-4B60-A9B6-B9E8883C604F}" name="Wk26 2025" dataDxfId="313"/>
-    <tableColumn id="10" xr3:uid="{CCA99270-0564-44F1-B8A9-B10867174574}" name="Wk27 2025" dataDxfId="312"/>
-    <tableColumn id="11" xr3:uid="{CB04338F-4AC3-4FB9-9523-D03C9AC04CFA}" name="Wk28 2025" dataDxfId="311"/>
-    <tableColumn id="12" xr3:uid="{168D703C-6431-481A-8487-7E8368E366BC}" name="Wk29 2025" dataDxfId="310"/>
-    <tableColumn id="13" xr3:uid="{FDB41DB1-6F6B-4916-B572-38394BE66B1F}" name="Wk30 2025" dataDxfId="309"/>
-    <tableColumn id="14" xr3:uid="{0778B44C-DBF4-4080-A78B-648661D9426C}" name="Wk31 2025" dataDxfId="308"/>
-    <tableColumn id="15" xr3:uid="{BC7FB12D-725E-462E-9C0B-97CE889859A6}" name="Wk32 2025" dataDxfId="307"/>
-    <tableColumn id="16" xr3:uid="{FE953FAB-8873-440D-BE48-EBDFFBBADC0C}" name="Wk33 2025" dataDxfId="306"/>
-    <tableColumn id="17" xr3:uid="{0A4E75BB-3909-4A92-A8DA-A871FC7E3BAA}" name="Wk34 2025" dataDxfId="305"/>
-    <tableColumn id="18" xr3:uid="{D0723E92-F800-4D68-A58A-1B66CFA31C51}" name="Wk35 2025" dataDxfId="304"/>
-    <tableColumn id="19" xr3:uid="{2918C770-1CC1-4371-AC1B-01806A1CE446}" name="Wk36 2025" dataDxfId="303"/>
-    <tableColumn id="20" xr3:uid="{7941FE6E-EA83-4CDC-AD2A-06132476A42F}" name="Wk37 2025" dataDxfId="302"/>
-    <tableColumn id="21" xr3:uid="{55E82EB0-84EE-45B6-8BEE-D9FFCA630F6F}" name="Wk38 2025" dataDxfId="301"/>
-    <tableColumn id="22" xr3:uid="{0F0514F0-00F0-493C-ACED-298BE578B94B}" name="Wk39 2025" dataDxfId="300"/>
-    <tableColumn id="23" xr3:uid="{EE422636-D01A-49ED-BEC6-E94D6602FEA4}" name="Wk40 2025" dataDxfId="299"/>
-    <tableColumn id="24" xr3:uid="{7C96F367-6EEF-4D2F-A12C-9FA19C9B3D5F}" name="Wk41 2025" dataDxfId="298"/>
-    <tableColumn id="25" xr3:uid="{7C86F617-5706-4579-9F0D-62B11B689E95}" name="Wk42 2025" dataDxfId="297"/>
-    <tableColumn id="26" xr3:uid="{9605EE82-61E2-429C-B07E-6EDD0989F2E5}" name="Wk43 2025" dataDxfId="296"/>
-    <tableColumn id="27" xr3:uid="{8448055E-FBE4-458F-A852-2061A0876458}" name="Wk44 2025" dataDxfId="295"/>
-    <tableColumn id="28" xr3:uid="{6E71A468-4C0A-4173-B213-FEE8AE4214F8}" name="Wk45 2025" dataDxfId="294"/>
-    <tableColumn id="29" xr3:uid="{C28CFFE0-0AE5-40CA-B043-10C1F8CEA429}" name="Wk46 2025" dataDxfId="293"/>
-    <tableColumn id="30" xr3:uid="{7DB27D58-5B61-4A1E-8C66-D7EDFD58C08F}" name="Wk47 2025" dataDxfId="292"/>
-    <tableColumn id="31" xr3:uid="{551232DA-E355-4153-A68D-1C12EE07407A}" name="Wk48 2025" dataDxfId="291"/>
-    <tableColumn id="32" xr3:uid="{290C8FF1-1A55-4657-B36C-90C662AB1A17}" name="Wk49 2025" dataDxfId="290"/>
-    <tableColumn id="33" xr3:uid="{80E1EB9E-D171-4C0F-906A-21652CA22175}" name="Wk50 2025" dataDxfId="289"/>
-    <tableColumn id="34" xr3:uid="{439313A2-30FA-4F2B-A161-6D67E80A6287}" name="Wk51 2025" dataDxfId="288"/>
-    <tableColumn id="35" xr3:uid="{70D90196-AEB3-45F6-BB30-1A09F881B512}" name="Wk52 2025" dataDxfId="287"/>
-    <tableColumn id="36" xr3:uid="{406BBDD2-445E-4FDF-9C9D-E868BC5B42A0}" name="Wk 1 2026" dataDxfId="286"/>
-    <tableColumn id="37" xr3:uid="{90CC7935-24F1-40BA-BC51-2B594B5867C7}" name="Wk 2 2026" dataDxfId="285"/>
-    <tableColumn id="38" xr3:uid="{4925818B-A192-485F-ADE0-76413A1C2E2B}" name="Wk 3 2026" dataDxfId="284"/>
-    <tableColumn id="39" xr3:uid="{22F195C3-EA30-463B-9725-404EB437FD93}" name="Wk 4 2026" dataDxfId="283"/>
-    <tableColumn id="40" xr3:uid="{46318D25-00B3-4564-89E1-B9732A5202E3}" name="Wk 5 2026" dataDxfId="282"/>
-    <tableColumn id="41" xr3:uid="{7C7D4D36-F88B-498C-8101-CAA47E6CE383}" name="Wk 6 2026" dataDxfId="281"/>
-    <tableColumn id="42" xr3:uid="{DDF48BA8-DFA4-447D-B5FB-76E9A9EA5B8A}" name="Wk 7 2026" dataDxfId="280"/>
-    <tableColumn id="43" xr3:uid="{9A9726D5-4EBF-4EF9-B335-99C249FC43D8}" name="Wk 8 2026" dataDxfId="279"/>
-    <tableColumn id="44" xr3:uid="{C9413AAF-02E5-4136-99E5-A85640D38BF6}" name="Wk 9 2026" dataDxfId="278"/>
-    <tableColumn id="45" xr3:uid="{801C2224-8D3B-4149-B940-59E352E8FEB1}" name="Wk 10 2026" dataDxfId="277"/>
-    <tableColumn id="46" xr3:uid="{449AD6DE-0D47-410A-B25B-B408ED93F299}" name="Wk 11 2026" dataDxfId="276"/>
-    <tableColumn id="47" xr3:uid="{465AD38B-86F5-4A59-96DA-6968BE07E826}" name="Wk 12 2026" dataDxfId="275"/>
-    <tableColumn id="48" xr3:uid="{71695512-FC8C-46C8-A340-CC6972781435}" name="Wk 13 2026" dataDxfId="274"/>
-    <tableColumn id="49" xr3:uid="{46488E34-662F-490E-AFC3-A2B73363CB16}" name="Wk 14 2026" dataDxfId="273"/>
-    <tableColumn id="50" xr3:uid="{6B9C4F73-EE41-4207-B7C3-326AEAE82D6C}" name="Wk 15 2026" dataDxfId="272"/>
-    <tableColumn id="51" xr3:uid="{CB795A69-D494-48E6-B94F-730F618D2DB3}" name="Wk 16 2026" dataDxfId="271"/>
-    <tableColumn id="52" xr3:uid="{D4B307B7-FFF2-4846-9E1B-F84EE8118CFB}" name="Wk 17 2026" dataDxfId="270"/>
-    <tableColumn id="53" xr3:uid="{3C609ADA-5E16-4958-9C3E-D01F85BA6B76}" name="Wk 18 2026" dataDxfId="269"/>
-    <tableColumn id="54" xr3:uid="{7319B7BA-31F7-4D99-8B17-0ED4906E4EF4}" name="Wk 19 2026" dataDxfId="268"/>
-    <tableColumn id="55" xr3:uid="{91ACBED5-E173-4D69-84C4-A82B47621937}" name="Wk 20 2026" dataDxfId="267"/>
-    <tableColumn id="56" xr3:uid="{7E4863D4-3183-47E0-B05A-60319AB4C59A}" name="Wk 21 2026" dataDxfId="266"/>
-    <tableColumn id="57" xr3:uid="{2BFF8CF2-1C85-4094-9F60-2A59FD5E1095}" name="Wk 22 2026" dataDxfId="265"/>
-    <tableColumn id="58" xr3:uid="{5D198BA4-E324-49E3-8BE7-6A3B9B8E7E96}" name="Wk 23 2026" dataDxfId="264"/>
-    <tableColumn id="59" xr3:uid="{EAF42B2C-2C00-44F9-A35A-6CC91B62E182}" name="Wk 24 2026" dataDxfId="263"/>
-    <tableColumn id="60" xr3:uid="{B7B56993-506F-4044-99B7-68ADE63D7D7F}" name="Wk 25 2026" dataDxfId="262"/>
-    <tableColumn id="61" xr3:uid="{3525D9D8-F0A1-4B9D-BD41-C5AF41F667AD}" name="Wk 26 2026" dataDxfId="261"/>
-    <tableColumn id="62" xr3:uid="{7E567130-D108-49D2-9FED-02795BCBC159}" name="Wk 27 2026" dataDxfId="260"/>
-    <tableColumn id="63" xr3:uid="{228AC1EB-C6D5-40F2-83EF-4C2A42678A80}" name="Wk 28 2026" dataDxfId="259"/>
-    <tableColumn id="64" xr3:uid="{D307FBAF-E420-4D3E-A1CA-B1BCAFF9BC21}" name="Wk 29 2026" dataDxfId="258"/>
-    <tableColumn id="65" xr3:uid="{ED124B6E-396F-426B-803C-09FA55D63265}" name="Wk 30 2026" dataDxfId="257"/>
-    <tableColumn id="66" xr3:uid="{552A1633-3764-45A0-A6BE-EB10E5D3EE2A}" name="Wk 31 2026" dataDxfId="256"/>
-    <tableColumn id="67" xr3:uid="{20B829D7-CE26-47FE-A68C-782AD2405E45}" name="Wk 32 2026" dataDxfId="255"/>
-    <tableColumn id="68" xr3:uid="{094157AB-A526-4480-8D0F-6FF1416ECB5A}" name="Wk 33 2026" dataDxfId="254"/>
-    <tableColumn id="69" xr3:uid="{B40298A5-625D-4FF3-8CA6-A8C054E7D2BE}" name="Wk 34 2026" dataDxfId="253"/>
-    <tableColumn id="70" xr3:uid="{2288879E-142C-4BEE-B86A-AD54EB2B1DBB}" name="Wk 35 2026" dataDxfId="252"/>
-    <tableColumn id="71" xr3:uid="{B639EECA-0F34-491E-9923-96684065B5CC}" name="Wk 36 2026" dataDxfId="251"/>
-    <tableColumn id="72" xr3:uid="{20DB7AA9-253C-4673-B174-AC7609F1D183}" name="Wk 37 2026" dataDxfId="250"/>
-    <tableColumn id="73" xr3:uid="{8629C5E0-1573-498A-8F5B-99B6E6A74F5E}" name="Wk 38 2026" dataDxfId="249"/>
-    <tableColumn id="74" xr3:uid="{DBC53E68-797B-4408-8A78-59A872D576AC}" name="Wk 39 2026" dataDxfId="248"/>
-    <tableColumn id="75" xr3:uid="{2E5E4B64-1837-4A81-98B3-355113834168}" name="Wk 40 2026" dataDxfId="247"/>
-    <tableColumn id="76" xr3:uid="{903F1D00-C23F-4028-AE8E-28388781BFC8}" name="Wk 41 2026" dataDxfId="246"/>
-    <tableColumn id="77" xr3:uid="{D1A3DF15-DAE8-41ED-A2DC-BFC1F3679CE2}" name="Wk 42 2026" dataDxfId="245"/>
-    <tableColumn id="78" xr3:uid="{4A57ADAE-62BD-46E8-A048-172EADCF66CF}" name="Wk 43 2026" dataDxfId="244"/>
-    <tableColumn id="79" xr3:uid="{BD7B15E9-F25C-4522-8675-D4CED683E419}" name="Wk 44 2026" dataDxfId="243"/>
-    <tableColumn id="80" xr3:uid="{BEBA2E4B-4F5F-454B-8DEC-350007AD1A05}" name="Wk 45 2026" dataDxfId="242"/>
-    <tableColumn id="81" xr3:uid="{25E6C9C6-112C-4731-AA28-CF416D89698B}" name="Wk 46 2026" dataDxfId="241"/>
-    <tableColumn id="82" xr3:uid="{1672F750-5907-4B0D-82DC-722C1AB7D7EE}" name="Wk 47 2026" dataDxfId="240"/>
-    <tableColumn id="83" xr3:uid="{8CCFC408-290D-4730-930F-DE6E8D9A4415}" name="Wk 48 2026" dataDxfId="239"/>
-    <tableColumn id="84" xr3:uid="{9B0242EE-08B0-45EE-8ECB-49A04C9A6C27}" name="Wk 49 2026" dataDxfId="238"/>
-    <tableColumn id="85" xr3:uid="{8F4B4399-02CA-40AA-8688-ABDB0B15BE96}" name="Wk 50 2026" dataDxfId="237"/>
-    <tableColumn id="86" xr3:uid="{5FF095FA-D85E-4885-BB91-093A77DB66D6}" name="Wk 51 2026" dataDxfId="236"/>
-    <tableColumn id="87" xr3:uid="{F196C26A-5A23-477D-9B39-A0524030CCB7}" name="Wk 52 2026" dataDxfId="235"/>
+    <tableColumn id="2" xr3:uid="{C2CE772C-B148-4D1F-99A4-E4B9B5D7C5B1}" name="Wk19 2025" dataDxfId="316"/>
+    <tableColumn id="3" xr3:uid="{A0DD27EA-24C9-4735-8521-C1BFE274BE0E}" name="Wk20 2025" dataDxfId="315"/>
+    <tableColumn id="4" xr3:uid="{4483A63E-2841-499A-8F6F-04265F3B4950}" name="Wk21 2025" dataDxfId="314"/>
+    <tableColumn id="5" xr3:uid="{4EF77BC7-8819-4D13-86DF-856DB47A9715}" name="Wk22 2025" dataDxfId="313"/>
+    <tableColumn id="6" xr3:uid="{2F2C0467-26DF-407B-99A5-8D2F93FFD54D}" name="Wk23 2025" dataDxfId="312"/>
+    <tableColumn id="7" xr3:uid="{F520AFFE-1894-48D5-9D25-3A0DC5D76E82}" name="Wk24 2025" dataDxfId="311"/>
+    <tableColumn id="8" xr3:uid="{A229F7FD-0149-49DA-87D3-5DD9C91931E6}" name="Wk25 2025" dataDxfId="310"/>
+    <tableColumn id="9" xr3:uid="{21BFCA83-1B04-4B60-A9B6-B9E8883C604F}" name="Wk26 2025" dataDxfId="309"/>
+    <tableColumn id="10" xr3:uid="{CCA99270-0564-44F1-B8A9-B10867174574}" name="Wk27 2025" dataDxfId="308"/>
+    <tableColumn id="11" xr3:uid="{CB04338F-4AC3-4FB9-9523-D03C9AC04CFA}" name="Wk28 2025" dataDxfId="307"/>
+    <tableColumn id="12" xr3:uid="{168D703C-6431-481A-8487-7E8368E366BC}" name="Wk29 2025" dataDxfId="306"/>
+    <tableColumn id="13" xr3:uid="{FDB41DB1-6F6B-4916-B572-38394BE66B1F}" name="Wk30 2025" dataDxfId="305"/>
+    <tableColumn id="14" xr3:uid="{0778B44C-DBF4-4080-A78B-648661D9426C}" name="Wk31 2025" dataDxfId="304"/>
+    <tableColumn id="15" xr3:uid="{BC7FB12D-725E-462E-9C0B-97CE889859A6}" name="Wk32 2025" dataDxfId="303"/>
+    <tableColumn id="16" xr3:uid="{FE953FAB-8873-440D-BE48-EBDFFBBADC0C}" name="Wk33 2025" dataDxfId="302"/>
+    <tableColumn id="17" xr3:uid="{0A4E75BB-3909-4A92-A8DA-A871FC7E3BAA}" name="Wk34 2025" dataDxfId="301"/>
+    <tableColumn id="18" xr3:uid="{D0723E92-F800-4D68-A58A-1B66CFA31C51}" name="Wk35 2025" dataDxfId="300"/>
+    <tableColumn id="19" xr3:uid="{2918C770-1CC1-4371-AC1B-01806A1CE446}" name="Wk36 2025" dataDxfId="299"/>
+    <tableColumn id="20" xr3:uid="{7941FE6E-EA83-4CDC-AD2A-06132476A42F}" name="Wk37 2025" dataDxfId="298"/>
+    <tableColumn id="21" xr3:uid="{55E82EB0-84EE-45B6-8BEE-D9FFCA630F6F}" name="Wk38 2025" dataDxfId="297"/>
+    <tableColumn id="22" xr3:uid="{0F0514F0-00F0-493C-ACED-298BE578B94B}" name="Wk39 2025" dataDxfId="296"/>
+    <tableColumn id="23" xr3:uid="{EE422636-D01A-49ED-BEC6-E94D6602FEA4}" name="Wk40 2025" dataDxfId="295"/>
+    <tableColumn id="24" xr3:uid="{7C96F367-6EEF-4D2F-A12C-9FA19C9B3D5F}" name="Wk41 2025" dataDxfId="294"/>
+    <tableColumn id="25" xr3:uid="{7C86F617-5706-4579-9F0D-62B11B689E95}" name="Wk42 2025" dataDxfId="293"/>
+    <tableColumn id="26" xr3:uid="{9605EE82-61E2-429C-B07E-6EDD0989F2E5}" name="Wk43 2025" dataDxfId="292"/>
+    <tableColumn id="27" xr3:uid="{8448055E-FBE4-458F-A852-2061A0876458}" name="Wk44 2025" dataDxfId="291"/>
+    <tableColumn id="28" xr3:uid="{6E71A468-4C0A-4173-B213-FEE8AE4214F8}" name="Wk45 2025" dataDxfId="290"/>
+    <tableColumn id="29" xr3:uid="{C28CFFE0-0AE5-40CA-B043-10C1F8CEA429}" name="Wk46 2025" dataDxfId="289"/>
+    <tableColumn id="30" xr3:uid="{7DB27D58-5B61-4A1E-8C66-D7EDFD58C08F}" name="Wk47 2025" dataDxfId="288"/>
+    <tableColumn id="31" xr3:uid="{551232DA-E355-4153-A68D-1C12EE07407A}" name="Wk48 2025" dataDxfId="287"/>
+    <tableColumn id="32" xr3:uid="{290C8FF1-1A55-4657-B36C-90C662AB1A17}" name="Wk49 2025" dataDxfId="286"/>
+    <tableColumn id="33" xr3:uid="{80E1EB9E-D171-4C0F-906A-21652CA22175}" name="Wk50 2025" dataDxfId="285"/>
+    <tableColumn id="34" xr3:uid="{439313A2-30FA-4F2B-A161-6D67E80A6287}" name="Wk51 2025" dataDxfId="284"/>
+    <tableColumn id="35" xr3:uid="{70D90196-AEB3-45F6-BB30-1A09F881B512}" name="Wk52 2025" dataDxfId="283"/>
+    <tableColumn id="36" xr3:uid="{406BBDD2-445E-4FDF-9C9D-E868BC5B42A0}" name="Wk 1 2026" dataDxfId="282"/>
+    <tableColumn id="37" xr3:uid="{90CC7935-24F1-40BA-BC51-2B594B5867C7}" name="Wk 2 2026" dataDxfId="281"/>
+    <tableColumn id="38" xr3:uid="{4925818B-A192-485F-ADE0-76413A1C2E2B}" name="Wk 3 2026" dataDxfId="280"/>
+    <tableColumn id="39" xr3:uid="{22F195C3-EA30-463B-9725-404EB437FD93}" name="Wk 4 2026" dataDxfId="279"/>
+    <tableColumn id="40" xr3:uid="{46318D25-00B3-4564-89E1-B9732A5202E3}" name="Wk 5 2026" dataDxfId="278"/>
+    <tableColumn id="41" xr3:uid="{7C7D4D36-F88B-498C-8101-CAA47E6CE383}" name="Wk 6 2026" dataDxfId="277"/>
+    <tableColumn id="42" xr3:uid="{DDF48BA8-DFA4-447D-B5FB-76E9A9EA5B8A}" name="Wk 7 2026" dataDxfId="276"/>
+    <tableColumn id="43" xr3:uid="{9A9726D5-4EBF-4EF9-B335-99C249FC43D8}" name="Wk 8 2026" dataDxfId="275"/>
+    <tableColumn id="44" xr3:uid="{C9413AAF-02E5-4136-99E5-A85640D38BF6}" name="Wk 9 2026" dataDxfId="274"/>
+    <tableColumn id="45" xr3:uid="{801C2224-8D3B-4149-B940-59E352E8FEB1}" name="Wk 10 2026" dataDxfId="273"/>
+    <tableColumn id="46" xr3:uid="{449AD6DE-0D47-410A-B25B-B408ED93F299}" name="Wk 11 2026" dataDxfId="272"/>
+    <tableColumn id="47" xr3:uid="{465AD38B-86F5-4A59-96DA-6968BE07E826}" name="Wk 12 2026" dataDxfId="271"/>
+    <tableColumn id="48" xr3:uid="{71695512-FC8C-46C8-A340-CC6972781435}" name="Wk 13 2026" dataDxfId="270"/>
+    <tableColumn id="49" xr3:uid="{46488E34-662F-490E-AFC3-A2B73363CB16}" name="Wk 14 2026" dataDxfId="269"/>
+    <tableColumn id="50" xr3:uid="{6B9C4F73-EE41-4207-B7C3-326AEAE82D6C}" name="Wk 15 2026" dataDxfId="268"/>
+    <tableColumn id="51" xr3:uid="{CB795A69-D494-48E6-B94F-730F618D2DB3}" name="Wk 16 2026" dataDxfId="267"/>
+    <tableColumn id="52" xr3:uid="{D4B307B7-FFF2-4846-9E1B-F84EE8118CFB}" name="Wk 17 2026" dataDxfId="266"/>
+    <tableColumn id="53" xr3:uid="{3C609ADA-5E16-4958-9C3E-D01F85BA6B76}" name="Wk 18 2026" dataDxfId="265"/>
+    <tableColumn id="54" xr3:uid="{7319B7BA-31F7-4D99-8B17-0ED4906E4EF4}" name="Wk 19 2026" dataDxfId="264"/>
+    <tableColumn id="55" xr3:uid="{91ACBED5-E173-4D69-84C4-A82B47621937}" name="Wk 20 2026" dataDxfId="263"/>
+    <tableColumn id="56" xr3:uid="{7E4863D4-3183-47E0-B05A-60319AB4C59A}" name="Wk 21 2026" dataDxfId="262"/>
+    <tableColumn id="57" xr3:uid="{2BFF8CF2-1C85-4094-9F60-2A59FD5E1095}" name="Wk 22 2026" dataDxfId="261"/>
+    <tableColumn id="58" xr3:uid="{5D198BA4-E324-49E3-8BE7-6A3B9B8E7E96}" name="Wk 23 2026" dataDxfId="260"/>
+    <tableColumn id="59" xr3:uid="{EAF42B2C-2C00-44F9-A35A-6CC91B62E182}" name="Wk 24 2026" dataDxfId="259"/>
+    <tableColumn id="60" xr3:uid="{B7B56993-506F-4044-99B7-68ADE63D7D7F}" name="Wk 25 2026" dataDxfId="258"/>
+    <tableColumn id="61" xr3:uid="{3525D9D8-F0A1-4B9D-BD41-C5AF41F667AD}" name="Wk 26 2026" dataDxfId="257"/>
+    <tableColumn id="62" xr3:uid="{7E567130-D108-49D2-9FED-02795BCBC159}" name="Wk 27 2026" dataDxfId="256"/>
+    <tableColumn id="63" xr3:uid="{228AC1EB-C6D5-40F2-83EF-4C2A42678A80}" name="Wk 28 2026" dataDxfId="255"/>
+    <tableColumn id="64" xr3:uid="{D307FBAF-E420-4D3E-A1CA-B1BCAFF9BC21}" name="Wk 29 2026" dataDxfId="254"/>
+    <tableColumn id="65" xr3:uid="{ED124B6E-396F-426B-803C-09FA55D63265}" name="Wk 30 2026" dataDxfId="253"/>
+    <tableColumn id="66" xr3:uid="{552A1633-3764-45A0-A6BE-EB10E5D3EE2A}" name="Wk 31 2026" dataDxfId="252"/>
+    <tableColumn id="67" xr3:uid="{20B829D7-CE26-47FE-A68C-782AD2405E45}" name="Wk 32 2026" dataDxfId="251"/>
+    <tableColumn id="68" xr3:uid="{094157AB-A526-4480-8D0F-6FF1416ECB5A}" name="Wk 33 2026" dataDxfId="250"/>
+    <tableColumn id="69" xr3:uid="{B40298A5-625D-4FF3-8CA6-A8C054E7D2BE}" name="Wk 34 2026" dataDxfId="249"/>
+    <tableColumn id="70" xr3:uid="{2288879E-142C-4BEE-B86A-AD54EB2B1DBB}" name="Wk 35 2026" dataDxfId="248"/>
+    <tableColumn id="71" xr3:uid="{B639EECA-0F34-491E-9923-96684065B5CC}" name="Wk 36 2026" dataDxfId="247"/>
+    <tableColumn id="72" xr3:uid="{20DB7AA9-253C-4673-B174-AC7609F1D183}" name="Wk 37 2026" dataDxfId="246"/>
+    <tableColumn id="73" xr3:uid="{8629C5E0-1573-498A-8F5B-99B6E6A74F5E}" name="Wk 38 2026" dataDxfId="245"/>
+    <tableColumn id="74" xr3:uid="{DBC53E68-797B-4408-8A78-59A872D576AC}" name="Wk 39 2026" dataDxfId="244"/>
+    <tableColumn id="75" xr3:uid="{2E5E4B64-1837-4A81-98B3-355113834168}" name="Wk 40 2026" dataDxfId="243"/>
+    <tableColumn id="76" xr3:uid="{903F1D00-C23F-4028-AE8E-28388781BFC8}" name="Wk 41 2026" dataDxfId="242"/>
+    <tableColumn id="77" xr3:uid="{D1A3DF15-DAE8-41ED-A2DC-BFC1F3679CE2}" name="Wk 42 2026" dataDxfId="241"/>
+    <tableColumn id="78" xr3:uid="{4A57ADAE-62BD-46E8-A048-172EADCF66CF}" name="Wk 43 2026" dataDxfId="240"/>
+    <tableColumn id="79" xr3:uid="{BD7B15E9-F25C-4522-8675-D4CED683E419}" name="Wk 44 2026" dataDxfId="239"/>
+    <tableColumn id="80" xr3:uid="{BEBA2E4B-4F5F-454B-8DEC-350007AD1A05}" name="Wk 45 2026" dataDxfId="238"/>
+    <tableColumn id="81" xr3:uid="{25E6C9C6-112C-4731-AA28-CF416D89698B}" name="Wk 46 2026" dataDxfId="237"/>
+    <tableColumn id="82" xr3:uid="{1672F750-5907-4B0D-82DC-722C1AB7D7EE}" name="Wk 47 2026" dataDxfId="236"/>
+    <tableColumn id="83" xr3:uid="{8CCFC408-290D-4730-930F-DE6E8D9A4415}" name="Wk 48 2026" dataDxfId="235"/>
+    <tableColumn id="84" xr3:uid="{9B0242EE-08B0-45EE-8ECB-49A04C9A6C27}" name="Wk 49 2026" dataDxfId="234"/>
+    <tableColumn id="85" xr3:uid="{8F4B4399-02CA-40AA-8688-ABDB0B15BE96}" name="Wk 50 2026" dataDxfId="233"/>
+    <tableColumn id="86" xr3:uid="{5FF095FA-D85E-4885-BB91-093A77DB66D6}" name="Wk 51 2026" dataDxfId="232"/>
+    <tableColumn id="87" xr3:uid="{F196C26A-5A23-477D-9B39-A0524030CCB7}" name="Wk 52 2026" dataDxfId="231"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F9880D93-3E9B-4BB8-8F9F-3210FFA8DEBE}" name="tblForecastConversion26" displayName="tblForecastConversion26" ref="B25:CJ31" totalsRowShown="0" headerRowDxfId="234" headerRowBorderDxfId="233" tableBorderDxfId="232">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F9880D93-3E9B-4BB8-8F9F-3210FFA8DEBE}" name="tblForecastConversion26" displayName="tblForecastConversion26" ref="B25:CJ31" totalsRowShown="0" headerRowDxfId="230" headerRowBorderDxfId="229" tableBorderDxfId="228">
   <autoFilter ref="B25:CJ31" xr:uid="{A3DDD57D-4EA3-4820-AB76-FC029A3E1E93}"/>
   <tableColumns count="87">
     <tableColumn id="1" xr3:uid="{19709AAB-A454-4CDD-8042-E660E6539FDB}" name="MP"/>
-    <tableColumn id="2" xr3:uid="{251A9C41-3B84-4933-8227-8CF5BF418024}" name="Wk19 2025" dataDxfId="231"/>
-    <tableColumn id="3" xr3:uid="{F10B1F4B-B8C5-43CF-B2A2-620D07E4CADC}" name="Wk20 2025" dataDxfId="230"/>
-    <tableColumn id="4" xr3:uid="{57C50167-E989-4A5E-B79D-46FB7418988B}" name="Wk21 2025" dataDxfId="229"/>
-    <tableColumn id="5" xr3:uid="{73D7C84C-2F32-4EF4-BD24-E83F543EB035}" name="Wk22 2025" dataDxfId="228"/>
-    <tableColumn id="6" xr3:uid="{ED8EF779-8372-4AA0-ADF8-00FD7FBF7099}" name="Wk23 2025" dataDxfId="227"/>
-    <tableColumn id="7" xr3:uid="{BB99AAEA-DAD8-4C1D-82B1-404493760F91}" name="Wk24 2025" dataDxfId="226"/>
-    <tableColumn id="8" xr3:uid="{60C84499-2BC4-47CC-A1A3-93D84D3C1F6B}" name="Wk25 2025" dataDxfId="225"/>
-    <tableColumn id="9" xr3:uid="{10916351-2A88-4C13-8AA5-451BAF476748}" name="Wk26 2025" dataDxfId="224"/>
-    <tableColumn id="10" xr3:uid="{10893799-E298-4F5B-96BD-431CB346D0B2}" name="Wk27 2025" dataDxfId="223"/>
-    <tableColumn id="11" xr3:uid="{2431BF64-6EFD-4E36-89F3-4E6C80D18BAB}" name="Wk28 2025" dataDxfId="222"/>
-    <tableColumn id="12" xr3:uid="{9CC7ACFB-9C6E-47E7-9AAC-35F635827979}" name="Wk29 2025" dataDxfId="221"/>
-    <tableColumn id="13" xr3:uid="{67AC7F80-32AC-43E5-87BE-1B79F81917D4}" name="Wk30 2025" dataDxfId="220"/>
-    <tableColumn id="14" xr3:uid="{6277956A-BDE5-40D6-9EA2-726755ED7694}" name="Wk31 2025" dataDxfId="219"/>
-    <tableColumn id="15" xr3:uid="{4A4F3B36-9124-4463-9553-6207D7F9B6A5}" name="Wk32 2025" dataDxfId="218"/>
-    <tableColumn id="16" xr3:uid="{427FB6BC-4E70-41A6-AE77-53C2EDF704BD}" name="Wk33 2025" dataDxfId="217"/>
-    <tableColumn id="17" xr3:uid="{4144B392-27FA-4687-B013-11028BD56AE7}" name="Wk34 2025" dataDxfId="216"/>
-    <tableColumn id="18" xr3:uid="{67FF2B25-6FF4-4B88-8995-3DB633E49BFE}" name="Wk35 2025" dataDxfId="215"/>
-    <tableColumn id="19" xr3:uid="{ADDC8232-E4E0-4CAB-82E6-E25A0453AEB4}" name="Wk36 2025" dataDxfId="214"/>
-    <tableColumn id="20" xr3:uid="{2F5A67E8-1A48-4D22-8E40-E5DFEF914106}" name="Wk37 2025" dataDxfId="213"/>
-    <tableColumn id="21" xr3:uid="{0365B1EB-5F00-4430-80DE-8185E796B733}" name="Wk38 2025" dataDxfId="212"/>
-    <tableColumn id="22" xr3:uid="{CB7F21C9-397D-4D10-88A8-311BEB3153AF}" name="Wk39 2025" dataDxfId="211"/>
-    <tableColumn id="23" xr3:uid="{785CFE1E-0F7D-4A16-AAB8-FEF970029AEE}" name="Wk40 2025" dataDxfId="210"/>
-    <tableColumn id="24" xr3:uid="{3F5A290C-DE40-4BA2-ACD1-48B1D35751C2}" name="Wk41 2025" dataDxfId="209"/>
-    <tableColumn id="25" xr3:uid="{D025795C-544E-4C9F-BD99-53A55DE058C4}" name="Wk42 2025" dataDxfId="208"/>
-    <tableColumn id="26" xr3:uid="{00786A22-6936-4965-B42A-ECEB13DA9305}" name="Wk43 2025" dataDxfId="207"/>
-    <tableColumn id="27" xr3:uid="{8FB0E2F7-F1B8-488D-8D6F-4F5966783BD4}" name="Wk44 2025" dataDxfId="206"/>
-    <tableColumn id="28" xr3:uid="{236C8E7F-C751-4C06-BEAA-6A8FD02B14E2}" name="Wk45 2025" dataDxfId="205"/>
-    <tableColumn id="29" xr3:uid="{B10855DD-6B23-47EC-BF28-4C19C93EBB7B}" name="Wk46 2025" dataDxfId="204"/>
-    <tableColumn id="30" xr3:uid="{0F99B47A-ED9A-4487-A63F-ABC2A910F590}" name="Wk47 2025" dataDxfId="203"/>
-    <tableColumn id="31" xr3:uid="{522DDE35-F449-4AD7-89A0-0ED56B293919}" name="Wk48 2025" dataDxfId="202"/>
-    <tableColumn id="32" xr3:uid="{6917E470-1827-487A-9572-74E9DA22819F}" name="Wk49 2025" dataDxfId="201"/>
-    <tableColumn id="33" xr3:uid="{5704AB2D-B913-446C-852F-BD81C74614C7}" name="Wk50 2025" dataDxfId="200"/>
-    <tableColumn id="34" xr3:uid="{F3C2A90B-FBAC-4A65-9961-E2293897679A}" name="Wk51 2025" dataDxfId="199"/>
-    <tableColumn id="35" xr3:uid="{4F4995B6-4011-45F4-8331-97C880A5122E}" name="Wk52 2025" dataDxfId="198"/>
-    <tableColumn id="36" xr3:uid="{21BD62B3-ACC7-4844-B5DA-2962BEA9926F}" name="Wk 1 2026" dataDxfId="197"/>
-    <tableColumn id="37" xr3:uid="{2E9C2235-253E-48D0-BF48-4AAD7EF79292}" name="Wk 2 2026" dataDxfId="196"/>
-    <tableColumn id="38" xr3:uid="{68374603-71A9-42E5-AF82-2BBBFBAC9B36}" name="Wk 3 2026" dataDxfId="195"/>
-    <tableColumn id="39" xr3:uid="{F0DB1902-2942-4F44-B3ED-A57B46C74896}" name="Wk 4 2026" dataDxfId="194"/>
-    <tableColumn id="40" xr3:uid="{EDD81630-FFD0-40F4-BD97-D12144F95FFD}" name="Wk 5 2026" dataDxfId="193"/>
-    <tableColumn id="41" xr3:uid="{A2D9B204-3120-4FAE-A1FD-F334B9C080FC}" name="Wk 6 2026" dataDxfId="192"/>
-    <tableColumn id="42" xr3:uid="{017D52ED-1A22-4E63-B81F-3FC372A81285}" name="Wk 7 2026" dataDxfId="191"/>
-    <tableColumn id="43" xr3:uid="{15099DB2-F5B8-4210-BEDD-3FEE44708FDC}" name="Wk 8 2026" dataDxfId="190"/>
-    <tableColumn id="44" xr3:uid="{53DDB2C3-B621-42AC-9858-59FA91F20C71}" name="Wk 9 2026" dataDxfId="189"/>
-    <tableColumn id="45" xr3:uid="{CFBCA57F-D256-4E28-9D3A-D8AF20CD8E0C}" name="Wk 10 2026" dataDxfId="188"/>
-    <tableColumn id="46" xr3:uid="{A8AEAD12-2A04-400E-825A-82CD5596C732}" name="Wk 11 2026" dataDxfId="187"/>
-    <tableColumn id="47" xr3:uid="{107966B7-887B-42C6-8646-70A3AC43E553}" name="Wk 12 2026" dataDxfId="186"/>
-    <tableColumn id="48" xr3:uid="{394B57A4-D3F2-49EB-B5A3-5D1732EC6B2C}" name="Wk 13 2026" dataDxfId="185"/>
-    <tableColumn id="49" xr3:uid="{750D9CAD-F514-47DF-9E6A-0A50EDA8D48D}" name="Wk 14 2026" dataDxfId="184"/>
-    <tableColumn id="50" xr3:uid="{9D41C67A-86C7-4BE9-86EE-7B2E99FE95BF}" name="Wk 15 2026" dataDxfId="183"/>
-    <tableColumn id="51" xr3:uid="{5DA457BC-2164-4F1C-9F51-9D19FA3685AD}" name="Wk 16 2026" dataDxfId="182"/>
-    <tableColumn id="52" xr3:uid="{593F0E6B-3F47-4FA4-B3C5-028425E81FDF}" name="Wk 17 2026" dataDxfId="181"/>
-    <tableColumn id="53" xr3:uid="{34B7F7FC-C0E7-4F4B-91E2-F45F36B280E0}" name="Wk 18 2026" dataDxfId="180"/>
-    <tableColumn id="54" xr3:uid="{140D5B8A-A261-4622-B3F1-EC75701E505B}" name="Wk 19 2026" dataDxfId="179"/>
-    <tableColumn id="55" xr3:uid="{EB17F7F4-D539-4189-AE83-527959D19C79}" name="Wk 20 2026" dataDxfId="178"/>
-    <tableColumn id="56" xr3:uid="{7717CBFD-85B0-4A90-95E8-52794597607D}" name="Wk 21 2026" dataDxfId="177"/>
-    <tableColumn id="57" xr3:uid="{406ECD6F-0F9E-4DC7-BA51-8898E53B55B9}" name="Wk 22 2026" dataDxfId="176"/>
-    <tableColumn id="58" xr3:uid="{D228D428-6196-47C9-9AEC-F1862BACDD91}" name="Wk 23 2026" dataDxfId="175"/>
-    <tableColumn id="59" xr3:uid="{6D9A04A0-9F46-4B04-8056-61B10E2EE7E4}" name="Wk 24 2026" dataDxfId="174"/>
-    <tableColumn id="60" xr3:uid="{2FB1EEAA-91BA-42AA-97B1-7E0F55B91038}" name="Wk 25 2026" dataDxfId="173"/>
-    <tableColumn id="61" xr3:uid="{82BDB344-CF7D-47C7-AFE3-28840AE5F550}" name="Wk 26 2026" dataDxfId="172"/>
-    <tableColumn id="62" xr3:uid="{83ACCEFA-A6CA-4A98-8F0F-2866384750F5}" name="Wk 27 2026" dataDxfId="171"/>
-    <tableColumn id="63" xr3:uid="{CA6BDFF2-9FE4-4DC3-95D4-32AF8D649152}" name="Wk 28 2026" dataDxfId="170"/>
-    <tableColumn id="64" xr3:uid="{C76C25C6-B4BF-4F2B-B7AD-CDD402C1E654}" name="Wk 29 2026" dataDxfId="169"/>
-    <tableColumn id="65" xr3:uid="{AACB71CE-2090-43F0-99B5-9FCDD8A03F2E}" name="Wk 30 2026" dataDxfId="168"/>
-    <tableColumn id="66" xr3:uid="{BADF505C-ED78-4CD0-A338-A013008F2697}" name="Wk 31 2026" dataDxfId="167"/>
-    <tableColumn id="67" xr3:uid="{3E22C4D8-CDFD-45AA-9821-EB1D8EFE6930}" name="Wk 32 2026" dataDxfId="166"/>
-    <tableColumn id="68" xr3:uid="{18D3F6C6-8EB0-4FFB-AE28-D34B0B4503EC}" name="Wk 33 2026" dataDxfId="165"/>
-    <tableColumn id="69" xr3:uid="{13B6243E-7D13-4FB6-828E-ACCBBCCAC3E2}" name="Wk 34 2026" dataDxfId="164"/>
-    <tableColumn id="70" xr3:uid="{758FD66C-4C4B-459E-ADB0-D45789CD0191}" name="Wk 35 2026" dataDxfId="163"/>
-    <tableColumn id="71" xr3:uid="{1B031FFD-CB8B-4E27-9A52-912776C2BD39}" name="Wk 36 2026" dataDxfId="162"/>
-    <tableColumn id="72" xr3:uid="{EAD84479-C984-4017-8D5C-F8B65AA95747}" name="Wk 37 2026" dataDxfId="161"/>
-    <tableColumn id="73" xr3:uid="{548D01E8-D822-4B76-A4FD-527D06F1F841}" name="Wk 38 2026" dataDxfId="160"/>
-    <tableColumn id="74" xr3:uid="{2CCDCB83-4578-412E-BDBE-B1759394F807}" name="Wk 39 2026" dataDxfId="159"/>
-    <tableColumn id="75" xr3:uid="{A2B47FAA-DF88-47C7-8FFF-9B3B5C8A6DD2}" name="Wk 40 2026" dataDxfId="158"/>
-    <tableColumn id="76" xr3:uid="{0015EEB1-F974-42C1-845C-EBE7BA1ADE35}" name="Wk 41 2026" dataDxfId="157"/>
-    <tableColumn id="77" xr3:uid="{2A5AF859-384F-4A7E-BAD8-E8E8FE921B91}" name="Wk 42 2026" dataDxfId="156"/>
-    <tableColumn id="78" xr3:uid="{FB1942F9-837A-45B2-9E28-A87BFEA05A3C}" name="Wk 43 2026" dataDxfId="155"/>
-    <tableColumn id="79" xr3:uid="{97F7C186-8FA9-4AC0-BF05-F1A72BA571C2}" name="Wk 44 2026" dataDxfId="154"/>
-    <tableColumn id="80" xr3:uid="{94110167-94FE-44E3-80F3-C0E28D9B947F}" name="Wk 45 2026" dataDxfId="153"/>
-    <tableColumn id="81" xr3:uid="{B54E2646-EF1B-470A-B500-CE3297E09990}" name="Wk 46 2026" dataDxfId="152"/>
-    <tableColumn id="82" xr3:uid="{A1347978-F005-4A77-A89F-3C9D020591C1}" name="Wk 47 2026" dataDxfId="151"/>
-    <tableColumn id="83" xr3:uid="{6392E998-6A9E-4474-8BB0-5D7C9C7A4B5E}" name="Wk 48 2026" dataDxfId="150"/>
-    <tableColumn id="84" xr3:uid="{6F788E70-5322-4E09-B880-57F7282FBDE6}" name="Wk 49 2026" dataDxfId="149"/>
-    <tableColumn id="85" xr3:uid="{32D9ACF4-883C-4011-989B-133EB02E36E5}" name="Wk 50 2026" dataDxfId="148"/>
-    <tableColumn id="86" xr3:uid="{A32BCA83-FCDB-4ECC-865D-6028DCBB9A1F}" name="Wk 51 2026" dataDxfId="147"/>
-    <tableColumn id="87" xr3:uid="{BEB0D13A-C664-4E08-ABD1-A8CDA2297D56}" name="Wk 52 2026" dataDxfId="146"/>
+    <tableColumn id="2" xr3:uid="{251A9C41-3B84-4933-8227-8CF5BF418024}" name="Wk19 2025" dataDxfId="227"/>
+    <tableColumn id="3" xr3:uid="{F10B1F4B-B8C5-43CF-B2A2-620D07E4CADC}" name="Wk20 2025" dataDxfId="226"/>
+    <tableColumn id="4" xr3:uid="{57C50167-E989-4A5E-B79D-46FB7418988B}" name="Wk21 2025" dataDxfId="225"/>
+    <tableColumn id="5" xr3:uid="{73D7C84C-2F32-4EF4-BD24-E83F543EB035}" name="Wk22 2025" dataDxfId="224"/>
+    <tableColumn id="6" xr3:uid="{ED8EF779-8372-4AA0-ADF8-00FD7FBF7099}" name="Wk23 2025" dataDxfId="223"/>
+    <tableColumn id="7" xr3:uid="{BB99AAEA-DAD8-4C1D-82B1-404493760F91}" name="Wk24 2025" dataDxfId="222"/>
+    <tableColumn id="8" xr3:uid="{60C84499-2BC4-47CC-A1A3-93D84D3C1F6B}" name="Wk25 2025" dataDxfId="221"/>
+    <tableColumn id="9" xr3:uid="{10916351-2A88-4C13-8AA5-451BAF476748}" name="Wk26 2025" dataDxfId="220"/>
+    <tableColumn id="10" xr3:uid="{10893799-E298-4F5B-96BD-431CB346D0B2}" name="Wk27 2025" dataDxfId="219"/>
+    <tableColumn id="11" xr3:uid="{2431BF64-6EFD-4E36-89F3-4E6C80D18BAB}" name="Wk28 2025" dataDxfId="218"/>
+    <tableColumn id="12" xr3:uid="{9CC7ACFB-9C6E-47E7-9AAC-35F635827979}" name="Wk29 2025" dataDxfId="217"/>
+    <tableColumn id="13" xr3:uid="{67AC7F80-32AC-43E5-87BE-1B79F81917D4}" name="Wk30 2025" dataDxfId="216"/>
+    <tableColumn id="14" xr3:uid="{6277956A-BDE5-40D6-9EA2-726755ED7694}" name="Wk31 2025" dataDxfId="215"/>
+    <tableColumn id="15" xr3:uid="{4A4F3B36-9124-4463-9553-6207D7F9B6A5}" name="Wk32 2025" dataDxfId="214"/>
+    <tableColumn id="16" xr3:uid="{427FB6BC-4E70-41A6-AE77-53C2EDF704BD}" name="Wk33 2025" dataDxfId="213"/>
+    <tableColumn id="17" xr3:uid="{4144B392-27FA-4687-B013-11028BD56AE7}" name="Wk34 2025" dataDxfId="212"/>
+    <tableColumn id="18" xr3:uid="{67FF2B25-6FF4-4B88-8995-3DB633E49BFE}" name="Wk35 2025" dataDxfId="211"/>
+    <tableColumn id="19" xr3:uid="{ADDC8232-E4E0-4CAB-82E6-E25A0453AEB4}" name="Wk36 2025" dataDxfId="210"/>
+    <tableColumn id="20" xr3:uid="{2F5A67E8-1A48-4D22-8E40-E5DFEF914106}" name="Wk37 2025" dataDxfId="209"/>
+    <tableColumn id="21" xr3:uid="{0365B1EB-5F00-4430-80DE-8185E796B733}" name="Wk38 2025" dataDxfId="208"/>
+    <tableColumn id="22" xr3:uid="{CB7F21C9-397D-4D10-88A8-311BEB3153AF}" name="Wk39 2025" dataDxfId="207"/>
+    <tableColumn id="23" xr3:uid="{785CFE1E-0F7D-4A16-AAB8-FEF970029AEE}" name="Wk40 2025" dataDxfId="206"/>
+    <tableColumn id="24" xr3:uid="{3F5A290C-DE40-4BA2-ACD1-48B1D35751C2}" name="Wk41 2025" dataDxfId="205"/>
+    <tableColumn id="25" xr3:uid="{D025795C-544E-4C9F-BD99-53A55DE058C4}" name="Wk42 2025" dataDxfId="204"/>
+    <tableColumn id="26" xr3:uid="{00786A22-6936-4965-B42A-ECEB13DA9305}" name="Wk43 2025" dataDxfId="203"/>
+    <tableColumn id="27" xr3:uid="{8FB0E2F7-F1B8-488D-8D6F-4F5966783BD4}" name="Wk44 2025" dataDxfId="202"/>
+    <tableColumn id="28" xr3:uid="{236C8E7F-C751-4C06-BEAA-6A8FD02B14E2}" name="Wk45 2025" dataDxfId="201"/>
+    <tableColumn id="29" xr3:uid="{B10855DD-6B23-47EC-BF28-4C19C93EBB7B}" name="Wk46 2025" dataDxfId="200"/>
+    <tableColumn id="30" xr3:uid="{0F99B47A-ED9A-4487-A63F-ABC2A910F590}" name="Wk47 2025" dataDxfId="199"/>
+    <tableColumn id="31" xr3:uid="{522DDE35-F449-4AD7-89A0-0ED56B293919}" name="Wk48 2025" dataDxfId="198"/>
+    <tableColumn id="32" xr3:uid="{6917E470-1827-487A-9572-74E9DA22819F}" name="Wk49 2025" dataDxfId="197"/>
+    <tableColumn id="33" xr3:uid="{5704AB2D-B913-446C-852F-BD81C74614C7}" name="Wk50 2025" dataDxfId="196"/>
+    <tableColumn id="34" xr3:uid="{F3C2A90B-FBAC-4A65-9961-E2293897679A}" name="Wk51 2025" dataDxfId="195"/>
+    <tableColumn id="35" xr3:uid="{4F4995B6-4011-45F4-8331-97C880A5122E}" name="Wk52 2025" dataDxfId="194"/>
+    <tableColumn id="36" xr3:uid="{21BD62B3-ACC7-4844-B5DA-2962BEA9926F}" name="Wk 1 2026" dataDxfId="193"/>
+    <tableColumn id="37" xr3:uid="{2E9C2235-253E-48D0-BF48-4AAD7EF79292}" name="Wk 2 2026" dataDxfId="192"/>
+    <tableColumn id="38" xr3:uid="{68374603-71A9-42E5-AF82-2BBBFBAC9B36}" name="Wk 3 2026" dataDxfId="191"/>
+    <tableColumn id="39" xr3:uid="{F0DB1902-2942-4F44-B3ED-A57B46C74896}" name="Wk 4 2026" dataDxfId="190"/>
+    <tableColumn id="40" xr3:uid="{EDD81630-FFD0-40F4-BD97-D12144F95FFD}" name="Wk 5 2026" dataDxfId="189"/>
+    <tableColumn id="41" xr3:uid="{A2D9B204-3120-4FAE-A1FD-F334B9C080FC}" name="Wk 6 2026" dataDxfId="188"/>
+    <tableColumn id="42" xr3:uid="{017D52ED-1A22-4E63-B81F-3FC372A81285}" name="Wk 7 2026" dataDxfId="187"/>
+    <tableColumn id="43" xr3:uid="{15099DB2-F5B8-4210-BEDD-3FEE44708FDC}" name="Wk 8 2026" dataDxfId="186"/>
+    <tableColumn id="44" xr3:uid="{53DDB2C3-B621-42AC-9858-59FA91F20C71}" name="Wk 9 2026" dataDxfId="185"/>
+    <tableColumn id="45" xr3:uid="{CFBCA57F-D256-4E28-9D3A-D8AF20CD8E0C}" name="Wk 10 2026" dataDxfId="184"/>
+    <tableColumn id="46" xr3:uid="{A8AEAD12-2A04-400E-825A-82CD5596C732}" name="Wk 11 2026" dataDxfId="183"/>
+    <tableColumn id="47" xr3:uid="{107966B7-887B-42C6-8646-70A3AC43E553}" name="Wk 12 2026" dataDxfId="182"/>
+    <tableColumn id="48" xr3:uid="{394B57A4-D3F2-49EB-B5A3-5D1732EC6B2C}" name="Wk 13 2026" dataDxfId="181"/>
+    <tableColumn id="49" xr3:uid="{750D9CAD-F514-47DF-9E6A-0A50EDA8D48D}" name="Wk 14 2026" dataDxfId="180"/>
+    <tableColumn id="50" xr3:uid="{9D41C67A-86C7-4BE9-86EE-7B2E99FE95BF}" name="Wk 15 2026" dataDxfId="179"/>
+    <tableColumn id="51" xr3:uid="{5DA457BC-2164-4F1C-9F51-9D19FA3685AD}" name="Wk 16 2026" dataDxfId="178"/>
+    <tableColumn id="52" xr3:uid="{593F0E6B-3F47-4FA4-B3C5-028425E81FDF}" name="Wk 17 2026" dataDxfId="177"/>
+    <tableColumn id="53" xr3:uid="{34B7F7FC-C0E7-4F4B-91E2-F45F36B280E0}" name="Wk 18 2026" dataDxfId="176"/>
+    <tableColumn id="54" xr3:uid="{140D5B8A-A261-4622-B3F1-EC75701E505B}" name="Wk 19 2026" dataDxfId="175"/>
+    <tableColumn id="55" xr3:uid="{EB17F7F4-D539-4189-AE83-527959D19C79}" name="Wk 20 2026" dataDxfId="174"/>
+    <tableColumn id="56" xr3:uid="{7717CBFD-85B0-4A90-95E8-52794597607D}" name="Wk 21 2026" dataDxfId="173"/>
+    <tableColumn id="57" xr3:uid="{406ECD6F-0F9E-4DC7-BA51-8898E53B55B9}" name="Wk 22 2026" dataDxfId="172"/>
+    <tableColumn id="58" xr3:uid="{D228D428-6196-47C9-9AEC-F1862BACDD91}" name="Wk 23 2026" dataDxfId="171"/>
+    <tableColumn id="59" xr3:uid="{6D9A04A0-9F46-4B04-8056-61B10E2EE7E4}" name="Wk 24 2026" dataDxfId="170"/>
+    <tableColumn id="60" xr3:uid="{2FB1EEAA-91BA-42AA-97B1-7E0F55B91038}" name="Wk 25 2026" dataDxfId="169"/>
+    <tableColumn id="61" xr3:uid="{82BDB344-CF7D-47C7-AFE3-28840AE5F550}" name="Wk 26 2026" dataDxfId="168"/>
+    <tableColumn id="62" xr3:uid="{83ACCEFA-A6CA-4A98-8F0F-2866384750F5}" name="Wk 27 2026" dataDxfId="167"/>
+    <tableColumn id="63" xr3:uid="{CA6BDFF2-9FE4-4DC3-95D4-32AF8D649152}" name="Wk 28 2026" dataDxfId="166"/>
+    <tableColumn id="64" xr3:uid="{C76C25C6-B4BF-4F2B-B7AD-CDD402C1E654}" name="Wk 29 2026" dataDxfId="165"/>
+    <tableColumn id="65" xr3:uid="{AACB71CE-2090-43F0-99B5-9FCDD8A03F2E}" name="Wk 30 2026" dataDxfId="164"/>
+    <tableColumn id="66" xr3:uid="{BADF505C-ED78-4CD0-A338-A013008F2697}" name="Wk 31 2026" dataDxfId="163"/>
+    <tableColumn id="67" xr3:uid="{3E22C4D8-CDFD-45AA-9821-EB1D8EFE6930}" name="Wk 32 2026" dataDxfId="162"/>
+    <tableColumn id="68" xr3:uid="{18D3F6C6-8EB0-4FFB-AE28-D34B0B4503EC}" name="Wk 33 2026" dataDxfId="161"/>
+    <tableColumn id="69" xr3:uid="{13B6243E-7D13-4FB6-828E-ACCBBCCAC3E2}" name="Wk 34 2026" dataDxfId="160"/>
+    <tableColumn id="70" xr3:uid="{758FD66C-4C4B-459E-ADB0-D45789CD0191}" name="Wk 35 2026" dataDxfId="159"/>
+    <tableColumn id="71" xr3:uid="{1B031FFD-CB8B-4E27-9A52-912776C2BD39}" name="Wk 36 2026" dataDxfId="158"/>
+    <tableColumn id="72" xr3:uid="{EAD84479-C984-4017-8D5C-F8B65AA95747}" name="Wk 37 2026" dataDxfId="157"/>
+    <tableColumn id="73" xr3:uid="{548D01E8-D822-4B76-A4FD-527D06F1F841}" name="Wk 38 2026" dataDxfId="156"/>
+    <tableColumn id="74" xr3:uid="{2CCDCB83-4578-412E-BDBE-B1759394F807}" name="Wk 39 2026" dataDxfId="155"/>
+    <tableColumn id="75" xr3:uid="{A2B47FAA-DF88-47C7-8FFF-9B3B5C8A6DD2}" name="Wk 40 2026" dataDxfId="154"/>
+    <tableColumn id="76" xr3:uid="{0015EEB1-F974-42C1-845C-EBE7BA1ADE35}" name="Wk 41 2026" dataDxfId="153"/>
+    <tableColumn id="77" xr3:uid="{2A5AF859-384F-4A7E-BAD8-E8E8FE921B91}" name="Wk 42 2026" dataDxfId="152"/>
+    <tableColumn id="78" xr3:uid="{FB1942F9-837A-45B2-9E28-A87BFEA05A3C}" name="Wk 43 2026" dataDxfId="151"/>
+    <tableColumn id="79" xr3:uid="{97F7C186-8FA9-4AC0-BF05-F1A72BA571C2}" name="Wk 44 2026" dataDxfId="150"/>
+    <tableColumn id="80" xr3:uid="{94110167-94FE-44E3-80F3-C0E28D9B947F}" name="Wk 45 2026" dataDxfId="149"/>
+    <tableColumn id="81" xr3:uid="{B54E2646-EF1B-470A-B500-CE3297E09990}" name="Wk 46 2026" dataDxfId="148"/>
+    <tableColumn id="82" xr3:uid="{A1347978-F005-4A77-A89F-3C9D020591C1}" name="Wk 47 2026" dataDxfId="147"/>
+    <tableColumn id="83" xr3:uid="{6392E998-6A9E-4474-8BB0-5D7C9C7A4B5E}" name="Wk 48 2026" dataDxfId="146"/>
+    <tableColumn id="84" xr3:uid="{6F788E70-5322-4E09-B880-57F7282FBDE6}" name="Wk 49 2026" dataDxfId="145"/>
+    <tableColumn id="85" xr3:uid="{32D9ACF4-883C-4011-989B-133EB02E36E5}" name="Wk 50 2026" dataDxfId="144"/>
+    <tableColumn id="86" xr3:uid="{A32BCA83-FCDB-4ECC-865D-6028DCBB9A1F}" name="Wk 51 2026" dataDxfId="143"/>
+    <tableColumn id="87" xr3:uid="{BEB0D13A-C664-4E08-ABD1-A8CDA2297D56}" name="Wk 52 2026" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1BBD732E-DC21-4DAE-B276-9E6E2FB65295}" name="TblForecastUPO27" displayName="TblForecastUPO27" ref="B36:CJ42" totalsRowShown="0" headerRowDxfId="145" headerRowBorderDxfId="144" tableBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1BBD732E-DC21-4DAE-B276-9E6E2FB65295}" name="TblForecastUPO27" displayName="TblForecastUPO27" ref="B36:CJ42" totalsRowShown="0" headerRowDxfId="141" headerRowBorderDxfId="140" tableBorderDxfId="139">
   <autoFilter ref="B36:CJ42" xr:uid="{3A99EC39-3902-44BE-97E1-A361C84F19E1}"/>
   <tableColumns count="87">
     <tableColumn id="1" xr3:uid="{144B814F-58E6-4B6C-8C0E-65FD554AF3CB}" name="MP"/>
-    <tableColumn id="2" xr3:uid="{4821364A-661B-47EE-B5F6-A68B20A89CA5}" name="Wk19 2025" dataDxfId="142"/>
-    <tableColumn id="3" xr3:uid="{AA422AEB-6573-4DD7-A176-42B7EBEA4F3C}" name="Wk20 2025" dataDxfId="141"/>
-    <tableColumn id="4" xr3:uid="{DB4E66E9-AB40-42C5-ACBA-67189F08D127}" name="Wk21 2025" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{4821364A-661B-47EE-B5F6-A68B20A89CA5}" name="Wk19 2025" dataDxfId="138"/>
+    <tableColumn id="3" xr3:uid="{AA422AEB-6573-4DD7-A176-42B7EBEA4F3C}" name="Wk20 2025" dataDxfId="137"/>
+    <tableColumn id="4" xr3:uid="{DB4E66E9-AB40-42C5-ACBA-67189F08D127}" name="Wk21 2025" dataDxfId="136"/>
     <tableColumn id="5" xr3:uid="{C3427049-0A80-48EB-80E4-C1B2CE551F1D}" name="Wk22 2025"/>
     <tableColumn id="6" xr3:uid="{0CCF3FBD-B589-45F3-8E82-0C3BD9D995D1}" name="Wk23 2025"/>
     <tableColumn id="7" xr3:uid="{E9FF8575-D9FB-4AB3-A479-CFA6862F7E1B}" name="Wk24 2025"/>
     <tableColumn id="8" xr3:uid="{D9FB4E1F-C4DF-479B-8E31-724FDBBE748D}" name="Wk25 2025"/>
     <tableColumn id="9" xr3:uid="{AEB335AF-596C-4178-86E8-3D3FA64766EF}" name="Wk26 2025"/>
     <tableColumn id="10" xr3:uid="{75E445E1-E5B2-4C79-B91F-56CB0ACEFBE8}" name="Wk27 2025"/>
-    <tableColumn id="11" xr3:uid="{2EC4CB03-A7E3-4DFA-AE11-E2FE05AECCC4}" name="Wk28 2025" dataDxfId="139"/>
-    <tableColumn id="12" xr3:uid="{EE81FC78-3E72-4FFD-9972-9DAADEFECB78}" name="Wk29 2025" dataDxfId="138"/>
+    <tableColumn id="11" xr3:uid="{2EC4CB03-A7E3-4DFA-AE11-E2FE05AECCC4}" name="Wk28 2025" dataDxfId="135"/>
+    <tableColumn id="12" xr3:uid="{EE81FC78-3E72-4FFD-9972-9DAADEFECB78}" name="Wk29 2025" dataDxfId="134"/>
     <tableColumn id="13" xr3:uid="{5F388E32-2F1C-4FC2-9C8D-5FB53B9283F8}" name="Wk30 2025"/>
     <tableColumn id="14" xr3:uid="{9394B147-A24D-41D6-9926-65BF91B62BA3}" name="Wk31 2025"/>
     <tableColumn id="15" xr3:uid="{79C44F6B-E7D0-4F2D-99F2-5944A9CFC1BE}" name="Wk32 2025"/>
@@ -25015,69 +25043,69 @@
     <tableColumn id="22" xr3:uid="{CE7B393B-23A5-4838-B192-CD32BBED1139}" name="Wk39 2025"/>
     <tableColumn id="23" xr3:uid="{647C4F5D-13D9-466D-ABC0-88483CD9D40F}" name="Wk40 2025"/>
     <tableColumn id="24" xr3:uid="{BA7F7DDE-D3A4-4F1E-8BFA-484C4E401E9E}" name="Wk41 2025"/>
-    <tableColumn id="25" xr3:uid="{1854A1B5-2922-45CE-B9F2-9D5F6250BF3D}" name="Wk42 2025" dataDxfId="137"/>
-    <tableColumn id="26" xr3:uid="{FBE2AC7C-5E90-4CBA-98DD-14A1FD292B48}" name="Wk43 2025" dataDxfId="136"/>
-    <tableColumn id="27" xr3:uid="{D5EE5B13-6A8E-4939-A39D-F492CE1C9BF0}" name="Wk44 2025" dataDxfId="135"/>
-    <tableColumn id="28" xr3:uid="{293528AD-1E49-4618-97BF-BEF268D9E321}" name="Wk45 2025" dataDxfId="134"/>
-    <tableColumn id="29" xr3:uid="{D3CA8AE8-8C9B-4A11-8E42-FA2BF14BE63A}" name="Wk46 2025" dataDxfId="133"/>
-    <tableColumn id="30" xr3:uid="{F40CE1AB-E55D-4E39-AAA6-F52C8C4BE884}" name="Wk47 2025" dataDxfId="132"/>
-    <tableColumn id="31" xr3:uid="{B42EE7D8-0F7A-4D08-8A18-81DB208939D5}" name="Wk48 2025" dataDxfId="131"/>
-    <tableColumn id="32" xr3:uid="{64F3055F-6E9B-4B35-932E-45D6566C92CF}" name="Wk49 2025" dataDxfId="130"/>
-    <tableColumn id="33" xr3:uid="{57E31240-4114-4D66-996E-3D8B43656BAF}" name="Wk50 2025" dataDxfId="129"/>
-    <tableColumn id="34" xr3:uid="{E57E5CE8-5555-43D8-8093-A9FC4DC46882}" name="Wk51 2025" dataDxfId="128"/>
-    <tableColumn id="35" xr3:uid="{EC272B9B-F125-4C95-BA8D-86231342D144}" name="Wk52 2025" dataDxfId="127"/>
-    <tableColumn id="36" xr3:uid="{6007C119-962E-4928-8A17-17694012642E}" name="Wk 1 2026" dataDxfId="126"/>
-    <tableColumn id="37" xr3:uid="{455E8279-829F-4144-8053-74AA8C05019E}" name="Wk 2 2026" dataDxfId="125"/>
-    <tableColumn id="38" xr3:uid="{F904B546-0724-4DA7-9B94-C54B518A8AE1}" name="Wk 3 2026" dataDxfId="124"/>
-    <tableColumn id="39" xr3:uid="{D6E39830-E9D4-4B4C-8641-82772B345A66}" name="Wk 4 2026" dataDxfId="123"/>
-    <tableColumn id="40" xr3:uid="{CD445D52-13B4-4645-AD8B-00038CCB386E}" name="Wk 5 2026" dataDxfId="122"/>
-    <tableColumn id="41" xr3:uid="{58ADA5F3-F94B-4487-A688-FDE8FB7DE8D5}" name="Wk 6 2026" dataDxfId="121"/>
-    <tableColumn id="42" xr3:uid="{5A752ADD-30F0-4894-837B-E233993181F2}" name="Wk 7 2026" dataDxfId="120"/>
-    <tableColumn id="43" xr3:uid="{373206F0-749D-44F4-8274-D5AC2BED8876}" name="Wk 8 2026" dataDxfId="119"/>
-    <tableColumn id="44" xr3:uid="{4B130792-C308-40E9-B2FD-5D68DDBCDE27}" name="Wk 9 2026" dataDxfId="118"/>
-    <tableColumn id="45" xr3:uid="{F1FCB6C7-CF31-406A-BCC0-E724EBF1D64B}" name="Wk 10 2026" dataDxfId="117"/>
-    <tableColumn id="46" xr3:uid="{6223F83F-90CA-499C-BAC6-A4229D05E71B}" name="Wk 11 2026" dataDxfId="116"/>
-    <tableColumn id="47" xr3:uid="{7F9BD2BD-A08D-450A-91C5-CA75C65DC2D9}" name="Wk 12 2026" dataDxfId="115"/>
-    <tableColumn id="48" xr3:uid="{7AFA6898-4679-4E25-9A5D-FC24A53FE7A9}" name="Wk 13 2026" dataDxfId="114"/>
-    <tableColumn id="49" xr3:uid="{728F4E64-78BF-499B-9136-44949CD9561B}" name="Wk 14 2026" dataDxfId="113"/>
-    <tableColumn id="50" xr3:uid="{F6276505-9D53-4E48-A2B3-3ECA9DA12FA4}" name="Wk 15 2026" dataDxfId="112"/>
-    <tableColumn id="51" xr3:uid="{A00C0348-8289-4D85-AA9B-303FAE4E2546}" name="Wk 16 2026" dataDxfId="111"/>
-    <tableColumn id="52" xr3:uid="{0F9B23F2-E653-4606-A6C8-39487731B568}" name="Wk 17 2026" dataDxfId="110"/>
-    <tableColumn id="53" xr3:uid="{0F767FE0-808A-4ED7-9115-D724908FC1D2}" name="Wk 18 2026" dataDxfId="109"/>
-    <tableColumn id="54" xr3:uid="{0F4D6570-1791-46DF-9B33-119588CB9EB2}" name="Wk 19 2026" dataDxfId="108"/>
-    <tableColumn id="55" xr3:uid="{C858FD0E-4BB0-46AA-A65B-A19A8653F41F}" name="Wk 20 2026" dataDxfId="107"/>
-    <tableColumn id="56" xr3:uid="{F65EE8AE-F415-4A2A-8D22-F1ECE3AB4DBC}" name="Wk 21 2026" dataDxfId="106"/>
-    <tableColumn id="57" xr3:uid="{9646CDF0-DE4F-40D0-A641-19862007288B}" name="Wk 22 2026" dataDxfId="105"/>
-    <tableColumn id="58" xr3:uid="{BE9E1FF7-EBCD-4416-86F0-F2A0599EC19F}" name="Wk 23 2026" dataDxfId="104"/>
-    <tableColumn id="59" xr3:uid="{7482E9B2-65E2-4EB3-A160-A44356DFB2CD}" name="Wk 24 2026" dataDxfId="103"/>
-    <tableColumn id="60" xr3:uid="{E3F0CC41-44DF-43D7-9596-E04A034B4EA6}" name="Wk 25 2026" dataDxfId="102"/>
-    <tableColumn id="61" xr3:uid="{0E86C126-F221-4117-9410-F2821E0E6D7F}" name="Wk 26 2026" dataDxfId="101"/>
-    <tableColumn id="62" xr3:uid="{30503B81-5288-4CCA-8DA8-C0285DBB9342}" name="Wk 27 2026" dataDxfId="100"/>
-    <tableColumn id="63" xr3:uid="{AD0D1E9D-6BDD-4468-9053-59250BA106FD}" name="Wk 28 2026" dataDxfId="99"/>
-    <tableColumn id="64" xr3:uid="{B13C5F96-DB89-455C-AF68-C6C4A228919C}" name="Wk 29 2026" dataDxfId="98"/>
-    <tableColumn id="65" xr3:uid="{DA58387C-DC06-43E7-82EF-605FAAC8A3E2}" name="Wk 30 2026" dataDxfId="97"/>
-    <tableColumn id="66" xr3:uid="{F342D305-8893-4CF7-A7F6-88CDAF43690F}" name="Wk 31 2026" dataDxfId="96"/>
-    <tableColumn id="67" xr3:uid="{34AE6431-103B-4338-A2A3-136AD20DE849}" name="Wk 32 2026" dataDxfId="95"/>
-    <tableColumn id="68" xr3:uid="{5D3B4F7A-C5F6-4B49-9B69-E73E176D0520}" name="Wk 33 2026" dataDxfId="94"/>
-    <tableColumn id="69" xr3:uid="{DB4EE644-D449-479D-90A1-F4D66F33FC6B}" name="Wk 34 2026" dataDxfId="93"/>
-    <tableColumn id="70" xr3:uid="{2B425192-6C70-4903-BAD9-35863103B509}" name="Wk 35 2026" dataDxfId="92"/>
-    <tableColumn id="71" xr3:uid="{D6807F3C-65B9-4E6E-A832-2D8EC13B39CA}" name="Wk 36 2026" dataDxfId="91"/>
-    <tableColumn id="72" xr3:uid="{DB4D976D-CE01-4308-BD50-E1FFD41361F1}" name="Wk 37 2026" dataDxfId="90"/>
-    <tableColumn id="73" xr3:uid="{5806AF63-DFD0-4135-A433-537DC5995EC1}" name="Wk 38 2026" dataDxfId="89"/>
-    <tableColumn id="74" xr3:uid="{113620FF-812E-45A4-8516-DA80EC60C8A6}" name="Wk 39 2026" dataDxfId="88"/>
-    <tableColumn id="75" xr3:uid="{F0AF6534-FEB4-4CAF-BF99-601AA6B7282A}" name="Wk 40 2026" dataDxfId="87"/>
-    <tableColumn id="76" xr3:uid="{6C690B7D-5214-4843-A5A6-CACCD48FDCA5}" name="Wk 41 2026" dataDxfId="86"/>
-    <tableColumn id="77" xr3:uid="{83592EED-48D6-4493-BBAE-36FE797D8C1A}" name="Wk 42 2026" dataDxfId="85"/>
-    <tableColumn id="78" xr3:uid="{11F380BC-4093-4B73-AE5E-FB9007F6C7D9}" name="Wk 43 2026" dataDxfId="84"/>
-    <tableColumn id="79" xr3:uid="{9F4C4B0C-C8B2-4B07-B9CC-5CF91C9E7AE3}" name="Wk 44 2026" dataDxfId="83"/>
-    <tableColumn id="80" xr3:uid="{B7B92490-A4D8-4D80-AB83-5B73CF274AE5}" name="Wk 45 2026" dataDxfId="82"/>
-    <tableColumn id="81" xr3:uid="{55B0865E-7C34-417B-99E8-4FCDB6C776DF}" name="Wk 46 2026" dataDxfId="81"/>
-    <tableColumn id="82" xr3:uid="{736CC5E9-9551-4CFC-B000-407898AB376C}" name="Wk 47 2026" dataDxfId="80"/>
-    <tableColumn id="83" xr3:uid="{DA3184FA-8AAF-487B-914C-C931ECC77EFC}" name="Wk 48 2026" dataDxfId="79"/>
-    <tableColumn id="84" xr3:uid="{2A8641FD-6F9C-4B59-91BD-B501CB6A852A}" name="Wk 49 2026" dataDxfId="78"/>
-    <tableColumn id="85" xr3:uid="{F826EE3C-BDE2-4A31-94A9-B843213F843C}" name="Wk 50 2026" dataDxfId="77"/>
-    <tableColumn id="86" xr3:uid="{9307F62C-CF1F-46DA-A5EA-11F34CD9D784}" name="Wk 51 2026" dataDxfId="76"/>
-    <tableColumn id="87" xr3:uid="{6423CA9E-D1EF-4A7E-A9D6-7E05F827907D}" name="Wk 52 2026" dataDxfId="75"/>
+    <tableColumn id="25" xr3:uid="{1854A1B5-2922-45CE-B9F2-9D5F6250BF3D}" name="Wk42 2025" dataDxfId="133"/>
+    <tableColumn id="26" xr3:uid="{FBE2AC7C-5E90-4CBA-98DD-14A1FD292B48}" name="Wk43 2025" dataDxfId="132"/>
+    <tableColumn id="27" xr3:uid="{D5EE5B13-6A8E-4939-A39D-F492CE1C9BF0}" name="Wk44 2025" dataDxfId="131"/>
+    <tableColumn id="28" xr3:uid="{293528AD-1E49-4618-97BF-BEF268D9E321}" name="Wk45 2025" dataDxfId="130"/>
+    <tableColumn id="29" xr3:uid="{D3CA8AE8-8C9B-4A11-8E42-FA2BF14BE63A}" name="Wk46 2025" dataDxfId="129"/>
+    <tableColumn id="30" xr3:uid="{F40CE1AB-E55D-4E39-AAA6-F52C8C4BE884}" name="Wk47 2025" dataDxfId="128"/>
+    <tableColumn id="31" xr3:uid="{B42EE7D8-0F7A-4D08-8A18-81DB208939D5}" name="Wk48 2025" dataDxfId="127"/>
+    <tableColumn id="32" xr3:uid="{64F3055F-6E9B-4B35-932E-45D6566C92CF}" name="Wk49 2025" dataDxfId="126"/>
+    <tableColumn id="33" xr3:uid="{57E31240-4114-4D66-996E-3D8B43656BAF}" name="Wk50 2025" dataDxfId="125"/>
+    <tableColumn id="34" xr3:uid="{E57E5CE8-5555-43D8-8093-A9FC4DC46882}" name="Wk51 2025" dataDxfId="124"/>
+    <tableColumn id="35" xr3:uid="{EC272B9B-F125-4C95-BA8D-86231342D144}" name="Wk52 2025" dataDxfId="123"/>
+    <tableColumn id="36" xr3:uid="{6007C119-962E-4928-8A17-17694012642E}" name="Wk 1 2026" dataDxfId="122"/>
+    <tableColumn id="37" xr3:uid="{455E8279-829F-4144-8053-74AA8C05019E}" name="Wk 2 2026" dataDxfId="121"/>
+    <tableColumn id="38" xr3:uid="{F904B546-0724-4DA7-9B94-C54B518A8AE1}" name="Wk 3 2026" dataDxfId="120"/>
+    <tableColumn id="39" xr3:uid="{D6E39830-E9D4-4B4C-8641-82772B345A66}" name="Wk 4 2026" dataDxfId="119"/>
+    <tableColumn id="40" xr3:uid="{CD445D52-13B4-4645-AD8B-00038CCB386E}" name="Wk 5 2026" dataDxfId="118"/>
+    <tableColumn id="41" xr3:uid="{58ADA5F3-F94B-4487-A688-FDE8FB7DE8D5}" name="Wk 6 2026" dataDxfId="117"/>
+    <tableColumn id="42" xr3:uid="{5A752ADD-30F0-4894-837B-E233993181F2}" name="Wk 7 2026" dataDxfId="116"/>
+    <tableColumn id="43" xr3:uid="{373206F0-749D-44F4-8274-D5AC2BED8876}" name="Wk 8 2026" dataDxfId="115"/>
+    <tableColumn id="44" xr3:uid="{4B130792-C308-40E9-B2FD-5D68DDBCDE27}" name="Wk 9 2026" dataDxfId="114"/>
+    <tableColumn id="45" xr3:uid="{F1FCB6C7-CF31-406A-BCC0-E724EBF1D64B}" name="Wk 10 2026" dataDxfId="113"/>
+    <tableColumn id="46" xr3:uid="{6223F83F-90CA-499C-BAC6-A4229D05E71B}" name="Wk 11 2026" dataDxfId="112"/>
+    <tableColumn id="47" xr3:uid="{7F9BD2BD-A08D-450A-91C5-CA75C65DC2D9}" name="Wk 12 2026" dataDxfId="111"/>
+    <tableColumn id="48" xr3:uid="{7AFA6898-4679-4E25-9A5D-FC24A53FE7A9}" name="Wk 13 2026" dataDxfId="110"/>
+    <tableColumn id="49" xr3:uid="{728F4E64-78BF-499B-9136-44949CD9561B}" name="Wk 14 2026" dataDxfId="109"/>
+    <tableColumn id="50" xr3:uid="{F6276505-9D53-4E48-A2B3-3ECA9DA12FA4}" name="Wk 15 2026" dataDxfId="108"/>
+    <tableColumn id="51" xr3:uid="{A00C0348-8289-4D85-AA9B-303FAE4E2546}" name="Wk 16 2026" dataDxfId="107"/>
+    <tableColumn id="52" xr3:uid="{0F9B23F2-E653-4606-A6C8-39487731B568}" name="Wk 17 2026" dataDxfId="106"/>
+    <tableColumn id="53" xr3:uid="{0F767FE0-808A-4ED7-9115-D724908FC1D2}" name="Wk 18 2026" dataDxfId="105"/>
+    <tableColumn id="54" xr3:uid="{0F4D6570-1791-46DF-9B33-119588CB9EB2}" name="Wk 19 2026" dataDxfId="104"/>
+    <tableColumn id="55" xr3:uid="{C858FD0E-4BB0-46AA-A65B-A19A8653F41F}" name="Wk 20 2026" dataDxfId="103"/>
+    <tableColumn id="56" xr3:uid="{F65EE8AE-F415-4A2A-8D22-F1ECE3AB4DBC}" name="Wk 21 2026" dataDxfId="102"/>
+    <tableColumn id="57" xr3:uid="{9646CDF0-DE4F-40D0-A641-19862007288B}" name="Wk 22 2026" dataDxfId="101"/>
+    <tableColumn id="58" xr3:uid="{BE9E1FF7-EBCD-4416-86F0-F2A0599EC19F}" name="Wk 23 2026" dataDxfId="100"/>
+    <tableColumn id="59" xr3:uid="{7482E9B2-65E2-4EB3-A160-A44356DFB2CD}" name="Wk 24 2026" dataDxfId="99"/>
+    <tableColumn id="60" xr3:uid="{E3F0CC41-44DF-43D7-9596-E04A034B4EA6}" name="Wk 25 2026" dataDxfId="98"/>
+    <tableColumn id="61" xr3:uid="{0E86C126-F221-4117-9410-F2821E0E6D7F}" name="Wk 26 2026" dataDxfId="97"/>
+    <tableColumn id="62" xr3:uid="{30503B81-5288-4CCA-8DA8-C0285DBB9342}" name="Wk 27 2026" dataDxfId="96"/>
+    <tableColumn id="63" xr3:uid="{AD0D1E9D-6BDD-4468-9053-59250BA106FD}" name="Wk 28 2026" dataDxfId="95"/>
+    <tableColumn id="64" xr3:uid="{B13C5F96-DB89-455C-AF68-C6C4A228919C}" name="Wk 29 2026" dataDxfId="94"/>
+    <tableColumn id="65" xr3:uid="{DA58387C-DC06-43E7-82EF-605FAAC8A3E2}" name="Wk 30 2026" dataDxfId="93"/>
+    <tableColumn id="66" xr3:uid="{F342D305-8893-4CF7-A7F6-88CDAF43690F}" name="Wk 31 2026" dataDxfId="92"/>
+    <tableColumn id="67" xr3:uid="{34AE6431-103B-4338-A2A3-136AD20DE849}" name="Wk 32 2026" dataDxfId="91"/>
+    <tableColumn id="68" xr3:uid="{5D3B4F7A-C5F6-4B49-9B69-E73E176D0520}" name="Wk 33 2026" dataDxfId="90"/>
+    <tableColumn id="69" xr3:uid="{DB4EE644-D449-479D-90A1-F4D66F33FC6B}" name="Wk 34 2026" dataDxfId="89"/>
+    <tableColumn id="70" xr3:uid="{2B425192-6C70-4903-BAD9-35863103B509}" name="Wk 35 2026" dataDxfId="88"/>
+    <tableColumn id="71" xr3:uid="{D6807F3C-65B9-4E6E-A832-2D8EC13B39CA}" name="Wk 36 2026" dataDxfId="87"/>
+    <tableColumn id="72" xr3:uid="{DB4D976D-CE01-4308-BD50-E1FFD41361F1}" name="Wk 37 2026" dataDxfId="86"/>
+    <tableColumn id="73" xr3:uid="{5806AF63-DFD0-4135-A433-537DC5995EC1}" name="Wk 38 2026" dataDxfId="85"/>
+    <tableColumn id="74" xr3:uid="{113620FF-812E-45A4-8516-DA80EC60C8A6}" name="Wk 39 2026" dataDxfId="84"/>
+    <tableColumn id="75" xr3:uid="{F0AF6534-FEB4-4CAF-BF99-601AA6B7282A}" name="Wk 40 2026" dataDxfId="83"/>
+    <tableColumn id="76" xr3:uid="{6C690B7D-5214-4843-A5A6-CACCD48FDCA5}" name="Wk 41 2026" dataDxfId="82"/>
+    <tableColumn id="77" xr3:uid="{83592EED-48D6-4493-BBAE-36FE797D8C1A}" name="Wk 42 2026" dataDxfId="81"/>
+    <tableColumn id="78" xr3:uid="{11F380BC-4093-4B73-AE5E-FB9007F6C7D9}" name="Wk 43 2026" dataDxfId="80"/>
+    <tableColumn id="79" xr3:uid="{9F4C4B0C-C8B2-4B07-B9CC-5CF91C9E7AE3}" name="Wk 44 2026" dataDxfId="79"/>
+    <tableColumn id="80" xr3:uid="{B7B92490-A4D8-4D80-AB83-5B73CF274AE5}" name="Wk 45 2026" dataDxfId="78"/>
+    <tableColumn id="81" xr3:uid="{55B0865E-7C34-417B-99E8-4FCDB6C776DF}" name="Wk 46 2026" dataDxfId="77"/>
+    <tableColumn id="82" xr3:uid="{736CC5E9-9551-4CFC-B000-407898AB376C}" name="Wk 47 2026" dataDxfId="76"/>
+    <tableColumn id="83" xr3:uid="{DA3184FA-8AAF-487B-914C-C931ECC77EFC}" name="Wk 48 2026" dataDxfId="75"/>
+    <tableColumn id="84" xr3:uid="{2A8641FD-6F9C-4B59-91BD-B501CB6A852A}" name="Wk 49 2026" dataDxfId="74"/>
+    <tableColumn id="85" xr3:uid="{F826EE3C-BDE2-4A31-94A9-B843213F843C}" name="Wk 50 2026" dataDxfId="73"/>
+    <tableColumn id="86" xr3:uid="{9307F62C-CF1F-46DA-A5EA-11F34CD9D784}" name="Wk 51 2026" dataDxfId="72"/>
+    <tableColumn id="87" xr3:uid="{6423CA9E-D1EF-4A7E-A9D6-7E05F827907D}" name="Wk 52 2026" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -25091,50 +25119,50 @@
   </sortState>
   <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{E49512D2-A8B2-4D5E-8CE5-731DE6803917}" name="MP"/>
-    <tableColumn id="2" xr3:uid="{A3AF106A-9088-4179-8152-EAACC8115F39}" name="Wk19" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{C2064F86-6B3D-4EE3-BAB8-B1A11C272908}" name="Wk20" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{A8C41D82-8C9F-4D49-A92D-0EBC0E5BD61F}" name="Wk21" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{1700678B-1DAB-4FF1-B586-2D741AC23049}" name="Wk22" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{D3787CAF-3418-499B-8BE2-10F031EA56B6}" name="Wk23" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{D827C4CD-3095-4C0F-97CD-F0E5E494FEB2}" name="Wk24" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{843F4658-7D91-4BB8-98B7-1FE910314525}" name="Wk25" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{A5028661-1DAA-40C8-9B13-3BE2DBF7E1CE}" name="Wk26" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{E3924AA5-E1A5-40CE-BD1F-25B4AD0B9200}" name="Wk27" dataDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{24AED37B-4073-4E2E-A921-9E2C057EB600}" name="Wk28" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{E784281E-FFFF-4F4E-939C-7F817CD71C3E}" name="Wk29" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{541035CF-EA5F-4322-8338-3721D1A7DAEA}" name="Wk30" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{2BDB5858-0CEA-43AB-859F-2BA6C154D49F}" name="Wk31" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{7F135EFC-1D1A-40E3-9EA8-2F2B957530F7}" name="Wk32" dataDxfId="53"/>
-    <tableColumn id="16" xr3:uid="{4C6678E5-A3AB-45A8-87FC-AA9E65F49D5B}" name="Wk33" dataDxfId="52"/>
-    <tableColumn id="17" xr3:uid="{8920ED02-A4FF-442E-BB87-9297AE969734}" name="Wk34" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{9299C561-AB63-4538-8868-80B0F3C5D362}" name="Wk35" dataDxfId="50"/>
-    <tableColumn id="19" xr3:uid="{B8D15A49-5955-4F54-8C85-E9733F42B5B2}" name="Wk36" dataDxfId="49"/>
-    <tableColumn id="20" xr3:uid="{E1652891-6F55-462E-8D7C-97788370AF60}" name="Wk37" dataDxfId="48"/>
-    <tableColumn id="21" xr3:uid="{D5FD520C-D51D-4FEF-928F-F6E74C63E578}" name="Wk38" dataDxfId="47"/>
-    <tableColumn id="22" xr3:uid="{D203BB7C-46B4-4E39-9B99-B2A4B233F99F}" name="Wk39" dataDxfId="46"/>
-    <tableColumn id="23" xr3:uid="{2F306056-94BE-4AB8-85D9-A1B87C27ED9B}" name="Wk40" dataDxfId="45"/>
-    <tableColumn id="24" xr3:uid="{5EC10564-ED11-4002-A834-3D122E7084C2}" name="Wk41" dataDxfId="44"/>
-    <tableColumn id="25" xr3:uid="{682F16F4-8AF7-48C2-A81C-69FA8B41245E}" name="Wk42" dataDxfId="43"/>
-    <tableColumn id="26" xr3:uid="{AC5C7FAE-41EB-45BE-9752-1A44D5354E60}" name="Wk43" dataDxfId="42"/>
-    <tableColumn id="27" xr3:uid="{CC71102B-A022-477E-8B2C-1D851D255511}" name="Wk44" dataDxfId="41"/>
-    <tableColumn id="28" xr3:uid="{A3E132DE-DBF2-4F41-9D6A-19172A8D76BA}" name="Wk45" dataDxfId="40"/>
-    <tableColumn id="29" xr3:uid="{083CCE35-C91E-4374-8FAC-74E5EBE9BEFC}" name="Wk46" dataDxfId="39"/>
-    <tableColumn id="30" xr3:uid="{4609462C-7FBC-4465-97CB-497205BC409C}" name="Wk47" dataDxfId="38"/>
-    <tableColumn id="31" xr3:uid="{1313040F-8C54-4F3C-B344-CF2579424DA2}" name="Wk48" dataDxfId="37"/>
-    <tableColumn id="32" xr3:uid="{F0610F8D-BBCD-4DD1-87A7-225DDFD43F96}" name="Wk49" dataDxfId="36"/>
-    <tableColumn id="33" xr3:uid="{4F200981-4999-4C21-AFEC-190FD0690988}" name="Wk50" dataDxfId="35"/>
-    <tableColumn id="34" xr3:uid="{78B2FB42-BA1F-4B56-8C3A-E53988EE1C11}" name="Wk51" dataDxfId="34"/>
-    <tableColumn id="35" xr3:uid="{766F3B04-E54A-4063-8FD7-F8CBB459411A}" name="Wk52" dataDxfId="33"/>
-    <tableColumn id="36" xr3:uid="{F5EB77F4-2229-4A64-8F4A-C2F2B5DFD5F0}" name="2026 wk1" dataDxfId="32"/>
-    <tableColumn id="37" xr3:uid="{EC183AEE-CACD-4AE3-AFFE-06D97ABFC8C4}" name="2026 wk2" dataDxfId="31"/>
-    <tableColumn id="38" xr3:uid="{2DF1513B-ECDC-4D72-B5EE-242303CB63D7}" name="2026 wk3" dataDxfId="30"/>
-    <tableColumn id="39" xr3:uid="{1385AF38-78CD-426E-A74C-0F2A6DA9B748}" name="2026 wk4" dataDxfId="29"/>
-    <tableColumn id="40" xr3:uid="{1998FD27-0F28-4CE4-8951-AC19629DE58B}" name="2026 wk5" dataDxfId="28"/>
-    <tableColumn id="41" xr3:uid="{C4FB3DD7-8D68-4E96-B064-14932193950A}" name="2026 wk6" dataDxfId="27"/>
-    <tableColumn id="42" xr3:uid="{6E152B1E-A2D2-4028-A95A-1A1E3DF84797}" name="2026 wk7" dataDxfId="26"/>
-    <tableColumn id="43" xr3:uid="{C5BCEF20-F957-4BFD-8081-B1653E3A857D}" name="2026 wk8" dataDxfId="25"/>
-    <tableColumn id="44" xr3:uid="{65E6812A-4A84-4CC1-B18F-0048E5E61844}" name="2026 wk64" dataDxfId="24"/>
-    <tableColumn id="45" xr3:uid="{AB2BFD8E-2DD5-4571-A901-8D17BA517312}" name="2026 wk9" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{A3AF106A-9088-4179-8152-EAACC8115F39}" name="Wk19" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{C2064F86-6B3D-4EE3-BAB8-B1A11C272908}" name="Wk20" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{A8C41D82-8C9F-4D49-A92D-0EBC0E5BD61F}" name="Wk21" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{1700678B-1DAB-4FF1-B586-2D741AC23049}" name="Wk22" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{D3787CAF-3418-499B-8BE2-10F031EA56B6}" name="Wk23" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{D827C4CD-3095-4C0F-97CD-F0E5E494FEB2}" name="Wk24" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{843F4658-7D91-4BB8-98B7-1FE910314525}" name="Wk25" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{A5028661-1DAA-40C8-9B13-3BE2DBF7E1CE}" name="Wk26" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{E3924AA5-E1A5-40CE-BD1F-25B4AD0B9200}" name="Wk27" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{24AED37B-4073-4E2E-A921-9E2C057EB600}" name="Wk28" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{E784281E-FFFF-4F4E-939C-7F817CD71C3E}" name="Wk29" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{541035CF-EA5F-4322-8338-3721D1A7DAEA}" name="Wk30" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{2BDB5858-0CEA-43AB-859F-2BA6C154D49F}" name="Wk31" dataDxfId="58"/>
+    <tableColumn id="15" xr3:uid="{7F135EFC-1D1A-40E3-9EA8-2F2B957530F7}" name="Wk32" dataDxfId="57"/>
+    <tableColumn id="16" xr3:uid="{4C6678E5-A3AB-45A8-87FC-AA9E65F49D5B}" name="Wk33" dataDxfId="56"/>
+    <tableColumn id="17" xr3:uid="{8920ED02-A4FF-442E-BB87-9297AE969734}" name="Wk34" dataDxfId="55"/>
+    <tableColumn id="18" xr3:uid="{9299C561-AB63-4538-8868-80B0F3C5D362}" name="Wk35" dataDxfId="54"/>
+    <tableColumn id="19" xr3:uid="{B8D15A49-5955-4F54-8C85-E9733F42B5B2}" name="Wk36" dataDxfId="53"/>
+    <tableColumn id="20" xr3:uid="{E1652891-6F55-462E-8D7C-97788370AF60}" name="Wk37" dataDxfId="52"/>
+    <tableColumn id="21" xr3:uid="{D5FD520C-D51D-4FEF-928F-F6E74C63E578}" name="Wk38" dataDxfId="51"/>
+    <tableColumn id="22" xr3:uid="{D203BB7C-46B4-4E39-9B99-B2A4B233F99F}" name="Wk39" dataDxfId="50"/>
+    <tableColumn id="23" xr3:uid="{2F306056-94BE-4AB8-85D9-A1B87C27ED9B}" name="Wk40" dataDxfId="49"/>
+    <tableColumn id="24" xr3:uid="{5EC10564-ED11-4002-A834-3D122E7084C2}" name="Wk41" dataDxfId="48"/>
+    <tableColumn id="25" xr3:uid="{682F16F4-8AF7-48C2-A81C-69FA8B41245E}" name="Wk42" dataDxfId="47"/>
+    <tableColumn id="26" xr3:uid="{AC5C7FAE-41EB-45BE-9752-1A44D5354E60}" name="Wk43" dataDxfId="46"/>
+    <tableColumn id="27" xr3:uid="{CC71102B-A022-477E-8B2C-1D851D255511}" name="Wk44" dataDxfId="45"/>
+    <tableColumn id="28" xr3:uid="{A3E132DE-DBF2-4F41-9D6A-19172A8D76BA}" name="Wk45" dataDxfId="44"/>
+    <tableColumn id="29" xr3:uid="{083CCE35-C91E-4374-8FAC-74E5EBE9BEFC}" name="Wk46" dataDxfId="43"/>
+    <tableColumn id="30" xr3:uid="{4609462C-7FBC-4465-97CB-497205BC409C}" name="Wk47" dataDxfId="42"/>
+    <tableColumn id="31" xr3:uid="{1313040F-8C54-4F3C-B344-CF2579424DA2}" name="Wk48" dataDxfId="41"/>
+    <tableColumn id="32" xr3:uid="{F0610F8D-BBCD-4DD1-87A7-225DDFD43F96}" name="Wk49" dataDxfId="40"/>
+    <tableColumn id="33" xr3:uid="{4F200981-4999-4C21-AFEC-190FD0690988}" name="Wk50" dataDxfId="39"/>
+    <tableColumn id="34" xr3:uid="{78B2FB42-BA1F-4B56-8C3A-E53988EE1C11}" name="Wk51" dataDxfId="38"/>
+    <tableColumn id="35" xr3:uid="{766F3B04-E54A-4063-8FD7-F8CBB459411A}" name="Wk52" dataDxfId="37"/>
+    <tableColumn id="36" xr3:uid="{F5EB77F4-2229-4A64-8F4A-C2F2B5DFD5F0}" name="2026 wk1" dataDxfId="36"/>
+    <tableColumn id="37" xr3:uid="{EC183AEE-CACD-4AE3-AFFE-06D97ABFC8C4}" name="2026 wk2" dataDxfId="35"/>
+    <tableColumn id="38" xr3:uid="{2DF1513B-ECDC-4D72-B5EE-242303CB63D7}" name="2026 wk3" dataDxfId="34"/>
+    <tableColumn id="39" xr3:uid="{1385AF38-78CD-426E-A74C-0F2A6DA9B748}" name="2026 wk4" dataDxfId="33"/>
+    <tableColumn id="40" xr3:uid="{1998FD27-0F28-4CE4-8951-AC19629DE58B}" name="2026 wk5" dataDxfId="32"/>
+    <tableColumn id="41" xr3:uid="{C4FB3DD7-8D68-4E96-B064-14932193950A}" name="2026 wk6" dataDxfId="31"/>
+    <tableColumn id="42" xr3:uid="{6E152B1E-A2D2-4028-A95A-1A1E3DF84797}" name="2026 wk7" dataDxfId="30"/>
+    <tableColumn id="43" xr3:uid="{C5BCEF20-F957-4BFD-8081-B1653E3A857D}" name="2026 wk8" dataDxfId="29"/>
+    <tableColumn id="44" xr3:uid="{65E6812A-4A84-4CC1-B18F-0048E5E61844}" name="2026 wk64" dataDxfId="28"/>
+    <tableColumn id="45" xr3:uid="{AB2BFD8E-2DD5-4571-A901-8D17BA517312}" name="2026 wk9" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -25459,8 +25487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D77377D-25FF-4950-B779-72A32825D78E}">
   <dimension ref="B1:CJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AO31" sqref="AO31:AO37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25473,6 +25501,9 @@
     <col min="20" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="37" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:88" x14ac:dyDescent="0.25">
@@ -25852,10 +25883,18 @@
       <c r="AK3" s="1">
         <v>288997</v>
       </c>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
+      <c r="AL3" s="1">
+        <v>349629</v>
+      </c>
+      <c r="AM3" s="1">
+        <v>323142</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>232295</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>250690</v>
+      </c>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
@@ -26005,10 +26044,18 @@
       <c r="AK4" s="1">
         <v>64727</v>
       </c>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
+      <c r="AL4" s="1">
+        <v>85630</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>77429</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>51933</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>61256</v>
+      </c>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
@@ -26124,10 +26171,18 @@
       <c r="AK5" s="1">
         <v>13343</v>
       </c>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
+      <c r="AL5" s="1">
+        <v>21818</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>18797</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>12059</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>12187</v>
+      </c>
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
       <c r="AR5" s="1"/>
@@ -26243,10 +26298,18 @@
       <c r="AK6" s="1">
         <v>116045</v>
       </c>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
-      <c r="AN6" s="1"/>
-      <c r="AO6" s="1"/>
+      <c r="AL6" s="1">
+        <v>159911</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>157746</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>122343</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>110625</v>
+      </c>
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
       <c r="AR6" s="1"/>
@@ -26362,10 +26425,18 @@
       <c r="AK7" s="1">
         <v>100603</v>
       </c>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
-      <c r="AN7" s="1"/>
-      <c r="AO7" s="1"/>
+      <c r="AL7" s="1">
+        <v>258311</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>175888</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>92729</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>97704</v>
+      </c>
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
@@ -26558,10 +26629,18 @@
         <f t="shared" si="1"/>
         <v>583715</v>
       </c>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
+      <c r="AL8" s="2">
+        <v>875299</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>753002</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>511359</v>
+      </c>
+      <c r="AO8" s="2">
+        <v>532462</v>
+      </c>
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2"/>
       <c r="AR8" s="2"/>
@@ -26987,10 +27066,18 @@
       <c r="AK13" s="1">
         <v>1611180</v>
       </c>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="2"/>
+      <c r="AL13" s="1">
+        <v>1439414</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>1389172</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>1107351</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>1194077</v>
+      </c>
       <c r="AP13" s="2"/>
       <c r="AQ13" s="1"/>
       <c r="AR13" s="1"/>
@@ -27140,10 +27227,18 @@
       <c r="AK14" s="1">
         <v>1367559</v>
       </c>
-      <c r="AL14" s="1"/>
-      <c r="AM14" s="1"/>
-      <c r="AN14" s="1"/>
-      <c r="AO14" s="1"/>
+      <c r="AL14" s="1">
+        <v>1277012</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>1261399</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>1066204</v>
+      </c>
+      <c r="AO14" s="1">
+        <v>1970459</v>
+      </c>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
@@ -27259,10 +27354,18 @@
       <c r="AK15" s="1">
         <v>513048</v>
       </c>
-      <c r="AL15" s="1"/>
-      <c r="AM15" s="1"/>
-      <c r="AN15" s="1"/>
-      <c r="AO15" s="1"/>
+      <c r="AL15" s="1">
+        <v>412666</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>397887</v>
+      </c>
+      <c r="AN15" s="1">
+        <v>399012</v>
+      </c>
+      <c r="AO15" s="1">
+        <v>478066</v>
+      </c>
       <c r="AP15" s="1"/>
       <c r="AQ15" s="1"/>
       <c r="AR15" s="1"/>
@@ -27378,10 +27481,18 @@
       <c r="AK16" s="1">
         <v>1028000</v>
       </c>
-      <c r="AL16" s="1"/>
-      <c r="AM16" s="1"/>
-      <c r="AN16" s="1"/>
-      <c r="AO16" s="1"/>
+      <c r="AL16" s="1">
+        <v>981826</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>1047291</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>990397</v>
+      </c>
+      <c r="AO16" s="1">
+        <v>1502666</v>
+      </c>
       <c r="AP16" s="1"/>
       <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
@@ -27497,10 +27608,18 @@
       <c r="AK17" s="1">
         <v>901152</v>
       </c>
-      <c r="AL17" s="1"/>
-      <c r="AM17" s="1"/>
-      <c r="AN17" s="1"/>
-      <c r="AO17" s="1"/>
+      <c r="AL17" s="1">
+        <v>1376576</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>1010795</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>815749</v>
+      </c>
+      <c r="AO17" s="1">
+        <v>1345573</v>
+      </c>
       <c r="AP17" s="1"/>
       <c r="AQ17" s="1"/>
       <c r="AR17" s="1"/>
@@ -27674,7 +27793,7 @@
         <v>6606556</v>
       </c>
       <c r="AG18" s="2">
-        <f t="shared" ref="AG18:AK18" si="3">SUBTOTAL(109,AG13:AG17)</f>
+        <f t="shared" ref="AG18:AL18" si="3">SUBTOTAL(109,AG13:AG17)</f>
         <v>8126363</v>
       </c>
       <c r="AH18" s="2">
@@ -27693,10 +27812,19 @@
         <f t="shared" si="3"/>
         <v>5420939</v>
       </c>
-      <c r="AL18" s="1"/>
-      <c r="AM18" s="1"/>
-      <c r="AN18" s="1"/>
-      <c r="AO18" s="2"/>
+      <c r="AL18" s="2">
+        <f t="shared" si="3"/>
+        <v>5487494</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>5106544</v>
+      </c>
+      <c r="AN18" s="1">
+        <v>4378713</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>6490841</v>
+      </c>
       <c r="AP18" s="2"/>
       <c r="AQ18" s="2"/>
       <c r="AR18" s="1"/>
@@ -28122,10 +28250,18 @@
       <c r="AK22" s="19">
         <v>2.6019423973527661E-2</v>
       </c>
-      <c r="AL22" s="19"/>
-      <c r="AM22" s="19"/>
-      <c r="AN22" s="19"/>
-      <c r="AO22" s="20"/>
+      <c r="AL22" s="19">
+        <v>3.2348181750670606E-2</v>
+      </c>
+      <c r="AM22" s="19">
+        <v>3.1531012718367488E-2</v>
+      </c>
+      <c r="AN22" s="19">
+        <v>3.0523293878815302E-2</v>
+      </c>
+      <c r="AO22" s="20">
+        <v>2.9993040649807338E-2</v>
+      </c>
       <c r="AP22" s="20"/>
       <c r="AQ22" s="19"/>
       <c r="AR22" s="19"/>
@@ -28275,10 +28411,18 @@
       <c r="AK23" s="19">
         <v>1.2607112092128185E-2</v>
       </c>
-      <c r="AL23" s="19"/>
-      <c r="AM23" s="19"/>
-      <c r="AN23" s="19"/>
-      <c r="AO23" s="19"/>
+      <c r="AL23" s="19">
+        <v>1.6195939760128258E-2</v>
+      </c>
+      <c r="AM23" s="19">
+        <v>1.5642948821110531E-2</v>
+      </c>
+      <c r="AN23" s="19">
+        <v>1.349085165690618E-2</v>
+      </c>
+      <c r="AO23" s="19">
+        <v>8.3797734436494246E-3</v>
+      </c>
       <c r="AP23" s="19"/>
       <c r="AQ23" s="19"/>
       <c r="AR23" s="19"/>
@@ -28394,10 +28538,18 @@
       <c r="AK24" s="19">
         <v>6.9654199892106349E-3</v>
       </c>
-      <c r="AL24" s="19"/>
-      <c r="AM24" s="19"/>
-      <c r="AN24" s="19"/>
-      <c r="AO24" s="19"/>
+      <c r="AL24" s="19">
+        <v>1.21230628112458E-2</v>
+      </c>
+      <c r="AM24" s="19">
+        <v>1.133990303779716E-2</v>
+      </c>
+      <c r="AN24" s="19">
+        <v>7.7065351418002456E-3</v>
+      </c>
+      <c r="AO24" s="19">
+        <v>6.3087523480021583E-3</v>
+      </c>
       <c r="AP24" s="19"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
@@ -28513,10 +28665,18 @@
       <c r="AK25" s="19">
         <v>1.5529640306558382E-2</v>
       </c>
-      <c r="AL25" s="19"/>
-      <c r="AM25" s="19"/>
-      <c r="AN25" s="19"/>
-      <c r="AO25" s="19"/>
+      <c r="AL25" s="19">
+        <v>2.0757568960449811E-2</v>
+      </c>
+      <c r="AM25" s="19">
+        <v>1.994001667158412E-2</v>
+      </c>
+      <c r="AN25" s="19">
+        <v>1.6598394381243081E-2</v>
+      </c>
+      <c r="AO25" s="19">
+        <v>1.0038824329558259E-2</v>
+      </c>
       <c r="AP25" s="19"/>
       <c r="AQ25" s="19"/>
       <c r="AR25" s="19"/>
@@ -28632,10 +28792,18 @@
       <c r="AK26" s="19">
         <v>2.6749182009756033E-2</v>
       </c>
-      <c r="AL26" s="19"/>
-      <c r="AM26" s="19"/>
-      <c r="AN26" s="19"/>
-      <c r="AO26" s="19"/>
+      <c r="AL26" s="19">
+        <v>4.4559396288576962E-2</v>
+      </c>
+      <c r="AM26" s="19">
+        <v>3.6204175920933522E-2</v>
+      </c>
+      <c r="AN26" s="19">
+        <v>1.6129961544543731E-2</v>
+      </c>
+      <c r="AO26" s="19">
+        <v>1.040225985509519E-2</v>
+      </c>
       <c r="AP26" s="19"/>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="19"/>
@@ -28821,17 +28989,26 @@
         <v>1.5095419171480101E-2</v>
       </c>
       <c r="AJ27" s="20">
-        <f t="shared" ref="AJ27:AK27" si="5">(AJ22*AJ13+AJ23*AJ14+AJ24*AJ15+AJ25*AJ16+AJ26*AJ17)/AJ18</f>
+        <f t="shared" ref="AJ27:AL27" si="5">(AJ22*AJ13+AJ23*AJ14+AJ24*AJ15+AJ25*AJ16+AJ26*AJ17)/AJ18</f>
         <v>1.2852220290029056E-2</v>
       </c>
       <c r="AK27" s="20">
         <f t="shared" si="5"/>
         <v>1.8964627533991665E-2</v>
       </c>
-      <c r="AL27" s="19"/>
-      <c r="AM27" s="19"/>
-      <c r="AN27" s="19"/>
-      <c r="AO27" s="20"/>
+      <c r="AL27" s="20">
+        <f t="shared" si="5"/>
+        <v>2.8057857987087178E-2</v>
+      </c>
+      <c r="AM27" s="19">
+        <v>2.4581008212207711E-2</v>
+      </c>
+      <c r="AN27" s="19">
+        <v>1.846569985290198E-2</v>
+      </c>
+      <c r="AO27" s="20">
+        <v>1.3006635041591681E-2</v>
+      </c>
       <c r="AP27" s="20"/>
       <c r="AQ27" s="20"/>
       <c r="AR27" s="19"/>
@@ -29237,7 +29414,7 @@
         <v>5.22</v>
       </c>
       <c r="AE32" s="32">
-        <f>AE3/(AE13*AE22)</f>
+        <f t="shared" ref="AE32:AE37" si="6">AE3/(AE13*AE22)</f>
         <v>7.2872698157903244</v>
       </c>
       <c r="AF32" s="32">
@@ -29258,10 +29435,18 @@
       <c r="AK32" s="31">
         <v>6.8936875333606427</v>
       </c>
-      <c r="AL32" s="31"/>
-      <c r="AM32" s="31"/>
-      <c r="AN32" s="31"/>
-      <c r="AO32" s="32"/>
+      <c r="AL32" s="31">
+        <v>7.5088227223022699</v>
+      </c>
+      <c r="AM32" s="31">
+        <v>7.3773343682936856</v>
+      </c>
+      <c r="AN32" s="31">
+        <v>6.8726331360946746</v>
+      </c>
+      <c r="AO32" s="32">
+        <v>6.9997766236667216</v>
+      </c>
       <c r="AP32" s="32"/>
       <c r="AQ32" s="31"/>
       <c r="AR32" s="31"/>
@@ -29391,7 +29576,7 @@
         <v>3.46</v>
       </c>
       <c r="AE33" s="31">
-        <f>AE4/(AE14*AE23)</f>
+        <f t="shared" si="6"/>
         <v>3.9851282835805746</v>
       </c>
       <c r="AF33" s="31">
@@ -29412,10 +29597,18 @@
       <c r="AK33" s="31">
         <v>3.7511261817588859</v>
       </c>
-      <c r="AL33" s="31"/>
-      <c r="AM33" s="31"/>
-      <c r="AN33" s="31"/>
-      <c r="AO33" s="31"/>
+      <c r="AL33" s="31">
+        <v>4.1439271126661303</v>
+      </c>
+      <c r="AM33" s="31">
+        <v>3.924032029191161</v>
+      </c>
+      <c r="AN33" s="31">
+        <v>3.610469966629589</v>
+      </c>
+      <c r="AO33" s="31">
+        <v>3.7097868217054262</v>
+      </c>
       <c r="AP33" s="31"/>
       <c r="AQ33" s="31"/>
       <c r="AR33" s="31"/>
@@ -29511,7 +29704,7 @@
         <v>3.59</v>
       </c>
       <c r="AE34" s="31">
-        <f>AE5/(AE15*AE24)</f>
+        <f t="shared" si="6"/>
         <v>4.5367802899780338</v>
       </c>
       <c r="AF34" s="31">
@@ -29532,10 +29725,18 @@
       <c r="AK34" s="31">
         <v>3.7793612878327174</v>
       </c>
-      <c r="AL34" s="31"/>
-      <c r="AM34" s="31"/>
-      <c r="AN34" s="31"/>
-      <c r="AO34" s="31"/>
+      <c r="AL34" s="31">
+        <v>4.372684543916872</v>
+      </c>
+      <c r="AM34" s="31">
+        <v>4.1660017730496453</v>
+      </c>
+      <c r="AN34" s="31">
+        <v>3.9216260162601619</v>
+      </c>
+      <c r="AO34" s="31">
+        <v>4.0407824933687007</v>
+      </c>
       <c r="AP34" s="31"/>
       <c r="AQ34" s="31"/>
       <c r="AR34" s="31"/>
@@ -29631,7 +29832,7 @@
         <v>5.43</v>
       </c>
       <c r="AE35" s="31">
-        <f>AE6/(AE16*AE25)</f>
+        <f t="shared" si="6"/>
         <v>8.8527477187512389</v>
       </c>
       <c r="AF35" s="31">
@@ -29652,10 +29853,18 @@
       <c r="AK35" s="31">
         <v>7.2713226750972764</v>
       </c>
-      <c r="AL35" s="31"/>
-      <c r="AM35" s="31"/>
-      <c r="AN35" s="31"/>
-      <c r="AO35" s="31"/>
+      <c r="AL35" s="31">
+        <v>7.8463155284133856</v>
+      </c>
+      <c r="AM35" s="31">
+        <v>7.553799741416463</v>
+      </c>
+      <c r="AN35" s="31">
+        <v>7.4422410122270213</v>
+      </c>
+      <c r="AO35" s="31">
+        <v>7.3334438183626123</v>
+      </c>
       <c r="AP35" s="31"/>
       <c r="AQ35" s="31"/>
       <c r="AR35" s="31"/>
@@ -29751,7 +29960,7 @@
         <v>4.71</v>
       </c>
       <c r="AE36" s="31">
-        <f>AE7/(AE17*AE26)</f>
+        <f t="shared" si="6"/>
         <v>7.8620323518980246</v>
       </c>
       <c r="AF36" s="31">
@@ -29772,10 +29981,18 @@
       <c r="AK36" s="31">
         <v>4.1782483643158983</v>
       </c>
-      <c r="AL36" s="31"/>
-      <c r="AM36" s="31"/>
-      <c r="AN36" s="31"/>
-      <c r="AO36" s="31"/>
+      <c r="AL36" s="31">
+        <v>4.2057741890022777</v>
+      </c>
+      <c r="AM36" s="31">
+        <v>4.806339663888509</v>
+      </c>
+      <c r="AN36" s="31">
+        <v>7.0473476212190302</v>
+      </c>
+      <c r="AO36" s="31">
+        <v>6.9803529327713081</v>
+      </c>
       <c r="AP36" s="31"/>
       <c r="AQ36" s="31"/>
       <c r="AR36" s="31"/>
@@ -29833,115 +30050,115 @@
         <v>5.2996453900709222</v>
       </c>
       <c r="D37" s="33">
-        <f t="shared" ref="D37:AD37" si="6">SUMPRODUCT(D13:D17,D32:D36)/D18</f>
+        <f t="shared" ref="D37:AD37" si="7">SUMPRODUCT(D13:D17,D32:D36)/D18</f>
         <v>4.9864864864864868</v>
       </c>
       <c r="E37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.2931034482758621</v>
+      </c>
+      <c r="F37" s="33">
+        <f t="shared" si="7"/>
+        <v>7.8047161572052399</v>
+      </c>
+      <c r="G37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.785372694218931</v>
+      </c>
+      <c r="H37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.1401174136807404</v>
+      </c>
+      <c r="I37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.0885035158810723</v>
+      </c>
+      <c r="J37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.1332727156860702</v>
+      </c>
+      <c r="K37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.3527178058107499</v>
+      </c>
+      <c r="L37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.3715120535473675</v>
+      </c>
+      <c r="M37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.3454260658850261</v>
+      </c>
+      <c r="N37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.0900548171145878</v>
+      </c>
+      <c r="O37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.2132403748014164</v>
+      </c>
+      <c r="P37" s="33">
+        <f t="shared" si="7"/>
+        <v>10.440902831521161</v>
+      </c>
+      <c r="Q37" s="33">
+        <f t="shared" si="7"/>
+        <v>11.945442814068828</v>
+      </c>
+      <c r="R37" s="33">
+        <f t="shared" si="7"/>
+        <v>9.7718517340139197</v>
+      </c>
+      <c r="S37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.8755449198898626</v>
+      </c>
+      <c r="T37" s="33">
+        <f t="shared" si="7"/>
+        <v>12.04925528199515</v>
+      </c>
+      <c r="U37" s="33">
+        <f t="shared" si="7"/>
+        <v>9.9651604906189704</v>
+      </c>
+      <c r="V37" s="33">
+        <f t="shared" si="7"/>
+        <v>5.8805883107385553</v>
+      </c>
+      <c r="W37" s="33">
+        <f t="shared" si="7"/>
+        <v>6.3826186546372208</v>
+      </c>
+      <c r="X37" s="31">
+        <f t="shared" si="7"/>
+        <v>7.044358563498994</v>
+      </c>
+      <c r="Y37" s="31">
+        <f t="shared" si="7"/>
+        <v>9.9001804000889742</v>
+      </c>
+      <c r="Z37" s="31">
+        <f t="shared" si="7"/>
+        <v>5.4015650086011213</v>
+      </c>
+      <c r="AA37" s="31">
+        <f t="shared" si="7"/>
+        <v>7.1811385053926404</v>
+      </c>
+      <c r="AB37" s="31">
+        <f t="shared" si="7"/>
+        <v>7.1262405492748346</v>
+      </c>
+      <c r="AC37" s="31">
+        <f t="shared" si="7"/>
+        <v>4.3708967835770531</v>
+      </c>
+      <c r="AD37" s="31">
+        <f t="shared" si="7"/>
+        <v>4.6490813281782613</v>
+      </c>
+      <c r="AE37" s="32">
         <f t="shared" si="6"/>
-        <v>5.2931034482758621</v>
-      </c>
-      <c r="F37" s="33">
-        <f t="shared" si="6"/>
-        <v>7.8047161572052399</v>
-      </c>
-      <c r="G37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.785372694218931</v>
-      </c>
-      <c r="H37" s="33">
-        <f t="shared" si="6"/>
-        <v>5.1401174136807404</v>
-      </c>
-      <c r="I37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.0885035158810723</v>
-      </c>
-      <c r="J37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.1332727156860702</v>
-      </c>
-      <c r="K37" s="33">
-        <f t="shared" si="6"/>
-        <v>5.3527178058107499</v>
-      </c>
-      <c r="L37" s="33">
-        <f t="shared" si="6"/>
-        <v>5.3715120535473675</v>
-      </c>
-      <c r="M37" s="33">
-        <f t="shared" si="6"/>
-        <v>5.3454260658850261</v>
-      </c>
-      <c r="N37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.0900548171145878</v>
-      </c>
-      <c r="O37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.2132403748014164</v>
-      </c>
-      <c r="P37" s="33">
-        <f t="shared" si="6"/>
-        <v>10.440902831521161</v>
-      </c>
-      <c r="Q37" s="33">
-        <f t="shared" si="6"/>
-        <v>11.945442814068828</v>
-      </c>
-      <c r="R37" s="33">
-        <f t="shared" si="6"/>
-        <v>9.7718517340139197</v>
-      </c>
-      <c r="S37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.8755449198898626</v>
-      </c>
-      <c r="T37" s="33">
-        <f t="shared" si="6"/>
-        <v>12.04925528199515</v>
-      </c>
-      <c r="U37" s="33">
-        <f t="shared" si="6"/>
-        <v>9.9651604906189704</v>
-      </c>
-      <c r="V37" s="33">
-        <f t="shared" si="6"/>
-        <v>5.8805883107385553</v>
-      </c>
-      <c r="W37" s="33">
-        <f t="shared" si="6"/>
-        <v>6.3826186546372208</v>
-      </c>
-      <c r="X37" s="31">
-        <f t="shared" si="6"/>
-        <v>7.044358563498994</v>
-      </c>
-      <c r="Y37" s="31">
-        <f t="shared" si="6"/>
-        <v>9.9001804000889742</v>
-      </c>
-      <c r="Z37" s="31">
-        <f t="shared" si="6"/>
-        <v>5.4015650086011213</v>
-      </c>
-      <c r="AA37" s="31">
-        <f t="shared" si="6"/>
-        <v>7.1811385053926404</v>
-      </c>
-      <c r="AB37" s="31">
-        <f t="shared" si="6"/>
-        <v>7.1262405492748346</v>
-      </c>
-      <c r="AC37" s="31">
-        <f t="shared" si="6"/>
-        <v>4.3708967835770531</v>
-      </c>
-      <c r="AD37" s="31">
-        <f t="shared" si="6"/>
-        <v>4.6490813281782613</v>
-      </c>
-      <c r="AE37" s="32">
-        <f>AE8/(AE18*AE27)</f>
         <v>6.8861378307008607</v>
       </c>
       <c r="AF37" s="32">
@@ -29961,17 +30178,26 @@
         <v>5.3840713053707816</v>
       </c>
       <c r="AJ37" s="32">
-        <f t="shared" ref="AJ37:AK37" si="7">AJ8/(AJ18*AJ27)</f>
+        <f t="shared" ref="AJ37:AL37" si="8">AJ8/(AJ18*AJ27)</f>
         <v>5.7777013235698229</v>
       </c>
       <c r="AK37" s="32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.6778251713217447</v>
       </c>
-      <c r="AL37" s="31"/>
-      <c r="AM37" s="31"/>
-      <c r="AN37" s="31"/>
-      <c r="AO37" s="32"/>
+      <c r="AL37" s="32">
+        <f t="shared" si="8"/>
+        <v>5.6849658627281823</v>
+      </c>
+      <c r="AM37" s="31">
+        <v>5.9988687422325624</v>
+      </c>
+      <c r="AN37" s="31">
+        <v>6.3243173048382308</v>
+      </c>
+      <c r="AO37" s="32">
+        <v>6.3069980100445369</v>
+      </c>
       <c r="AP37" s="32"/>
       <c r="AQ37" s="32"/>
       <c r="AR37" s="31"/>
@@ -30036,7 +30262,7 @@
   <dimension ref="B2:CJ48"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS8" sqref="AS7:AS8"/>
+      <selection activeCell="AN26" sqref="AN26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -30409,35 +30635,35 @@
       </c>
       <c r="AM4" s="1">
         <f t="shared" si="0"/>
-        <v>345716.49836058979</v>
+        <v>376965.56405024382</v>
       </c>
       <c r="AN4" s="1">
         <f t="shared" si="0"/>
-        <v>383923.45720675745</v>
+        <v>346112.08772227605</v>
       </c>
       <c r="AO4" s="1">
         <f t="shared" si="0"/>
-        <v>329772.58443574834</v>
+        <v>266743.74347369029</v>
       </c>
       <c r="AP4" s="1">
         <f t="shared" si="0"/>
-        <v>468057.19613424112</v>
+        <v>326718.30161780695</v>
       </c>
       <c r="AQ4" s="1">
         <f t="shared" si="0"/>
-        <v>334072.57428473874</v>
+        <v>269327.2313336985</v>
       </c>
       <c r="AR4" s="1">
         <f t="shared" si="0"/>
-        <v>468093.11928652745</v>
+        <v>383901.28867961897</v>
       </c>
       <c r="AS4" s="1">
         <f t="shared" si="0"/>
-        <v>336434.20032053057</v>
+        <v>265183.04636620876</v>
       </c>
       <c r="AT4" s="1">
         <f t="shared" si="0"/>
-        <v>401078.76609983662</v>
+        <v>331822.58462427661</v>
       </c>
       <c r="AU4" s="52"/>
       <c r="AV4" s="52"/>
@@ -30563,35 +30789,35 @@
       </c>
       <c r="AM5" s="1">
         <f t="shared" si="1"/>
-        <v>159314.26727549787</v>
+        <v>170577.05021267934</v>
       </c>
       <c r="AN5" s="1">
         <f t="shared" si="1"/>
-        <v>199066.87149461216</v>
+        <v>185438.90414062259</v>
       </c>
       <c r="AO5" s="1">
         <f t="shared" si="1"/>
-        <v>139743.42978945273</v>
+        <v>97830.551727729951</v>
       </c>
       <c r="AP5" s="1">
         <f t="shared" si="1"/>
-        <v>196494.73865113588</v>
+        <v>121850.25496240622</v>
       </c>
       <c r="AQ5" s="1">
         <f t="shared" si="1"/>
-        <v>154230.61665064641</v>
+        <v>90592.280004826433</v>
       </c>
       <c r="AR5" s="1">
         <f t="shared" si="1"/>
-        <v>209973.10900717246</v>
+        <v>141987.82915273451</v>
       </c>
       <c r="AS5" s="1">
         <f t="shared" si="1"/>
-        <v>169068.11086875523</v>
+        <v>102515.03102087478</v>
       </c>
       <c r="AT5" s="1">
         <f t="shared" si="1"/>
-        <v>191115.74182663031</v>
+        <v>128102.31679247828</v>
       </c>
       <c r="AU5" s="2"/>
       <c r="AV5" s="2"/>
@@ -30713,39 +30939,39 @@
       </c>
       <c r="AL6" s="1">
         <f t="shared" si="2"/>
-        <v>51945.908867743368</v>
+        <v>50506.493998128055</v>
       </c>
       <c r="AM6" s="1">
         <f t="shared" si="2"/>
-        <v>37769.209607723489</v>
+        <v>38831.530311740891</v>
       </c>
       <c r="AN6" s="1">
         <f t="shared" si="2"/>
-        <v>59979.419679618484</v>
+        <v>55815.181888526815</v>
       </c>
       <c r="AO6" s="1">
         <f t="shared" si="2"/>
-        <v>43938.66951000072</v>
+        <v>31906.460200202462</v>
       </c>
       <c r="AP6" s="1">
         <f t="shared" si="2"/>
-        <v>48381.843695825773</v>
+        <v>43162.590532843053</v>
       </c>
       <c r="AQ6" s="1">
         <f t="shared" si="2"/>
-        <v>49844.663533292187</v>
+        <v>34654.494275728415</v>
       </c>
       <c r="AR6" s="1">
         <f t="shared" si="2"/>
-        <v>58895.086653424049</v>
+        <v>52618.157885084343</v>
       </c>
       <c r="AS6" s="1">
         <f t="shared" si="2"/>
-        <v>42789.790695761774</v>
+        <v>39680.887413488483</v>
       </c>
       <c r="AT6" s="1">
         <f t="shared" si="2"/>
-        <v>62809.811537882197</v>
+        <v>64711.901031597794</v>
       </c>
       <c r="AU6" s="2"/>
       <c r="AV6" s="2"/>
@@ -30867,39 +31093,39 @@
       </c>
       <c r="AL7" s="1">
         <f t="shared" si="3"/>
-        <v>153446.95602198329</v>
+        <v>149946.66445756797</v>
       </c>
       <c r="AM7" s="1">
         <f t="shared" si="3"/>
-        <v>124388.64387352044</v>
+        <v>126785.07850143504</v>
       </c>
       <c r="AN7" s="1">
         <f t="shared" si="3"/>
-        <v>156056.97171710638</v>
+        <v>146156.702688499</v>
       </c>
       <c r="AO7" s="1">
         <f t="shared" si="3"/>
-        <v>147677.51031349486</v>
+        <v>81227.270028582047</v>
       </c>
       <c r="AP7" s="1">
         <f t="shared" si="3"/>
-        <v>169690.0796554733</v>
+        <v>114454.05356902246</v>
       </c>
       <c r="AQ7" s="1">
         <f t="shared" si="3"/>
-        <v>141367.7577345575</v>
+        <v>86334.776298790617</v>
       </c>
       <c r="AR7" s="1">
         <f t="shared" si="3"/>
-        <v>180486.62483531493</v>
+        <v>133417.61251746674</v>
       </c>
       <c r="AS7" s="1">
         <f t="shared" si="3"/>
-        <v>149719.16342925839</v>
+        <v>97916.117131298917</v>
       </c>
       <c r="AT7" s="1">
         <f t="shared" si="3"/>
-        <v>169777.89816659209</v>
+        <v>138707.27898055239</v>
       </c>
       <c r="AU7" s="2"/>
       <c r="AV7" s="2"/>
@@ -31021,39 +31247,39 @@
       </c>
       <c r="AL8" s="1">
         <f t="shared" si="4"/>
-        <v>137706.65936582102</v>
+        <v>134887.04283281852</v>
       </c>
       <c r="AM8" s="1">
         <f t="shared" si="4"/>
-        <v>72105.832850847102</v>
+        <v>73156.121651249297</v>
       </c>
       <c r="AN8" s="1">
         <f t="shared" si="4"/>
-        <v>140534.99976318842</v>
+        <v>133061.99526745611</v>
       </c>
       <c r="AO8" s="1">
         <f t="shared" si="4"/>
-        <v>71234.175203151797</v>
+        <v>48331.821625707351</v>
       </c>
       <c r="AP8" s="1">
         <f t="shared" si="4"/>
-        <v>144663.80478419227</v>
+        <v>105199.71962597249</v>
       </c>
       <c r="AQ8" s="1">
         <f t="shared" si="4"/>
-        <v>75409.602415202622</v>
+        <v>50831.342193191733</v>
       </c>
       <c r="AR8" s="1">
         <f t="shared" si="4"/>
-        <v>152007.83918318711</v>
+        <v>117649.23865260642</v>
       </c>
       <c r="AS8" s="1">
         <f t="shared" si="4"/>
-        <v>76420.198903411088</v>
+        <v>54227.654056660402</v>
       </c>
       <c r="AT8" s="1">
         <f t="shared" si="4"/>
-        <v>148914.59188794837</v>
+        <v>120678.20308585466</v>
       </c>
       <c r="AU8" s="2"/>
       <c r="AV8" s="2"/>
@@ -31175,39 +31401,39 @@
       </c>
       <c r="AL9" s="1">
         <f t="shared" si="5"/>
-        <v>878599.84133559407</v>
+        <v>870840.51836856105</v>
       </c>
       <c r="AM9" s="1">
         <f t="shared" si="5"/>
-        <v>739294.45196817862</v>
+        <v>786315.3447273483</v>
       </c>
       <c r="AN9" s="1">
         <f t="shared" si="5"/>
-        <v>939561.71986128285</v>
+        <v>866584.87170738052</v>
       </c>
       <c r="AO9" s="1">
         <f t="shared" si="5"/>
-        <v>732366.36925184843</v>
+        <v>526039.84705591213</v>
       </c>
       <c r="AP9" s="1">
         <f t="shared" si="5"/>
-        <v>1027287.6629208683</v>
+        <v>711384.92030805117</v>
       </c>
       <c r="AQ9" s="1">
         <f t="shared" si="5"/>
-        <v>754925.21461843757</v>
+        <v>531740.12410623569</v>
       </c>
       <c r="AR9" s="1">
         <f t="shared" si="5"/>
-        <v>1069455.7789656259</v>
+        <v>829574.126887511</v>
       </c>
       <c r="AS9" s="1">
         <f t="shared" si="5"/>
-        <v>774431.46421771706</v>
+        <v>559522.73598853138</v>
       </c>
       <c r="AT9" s="1">
         <f t="shared" si="5"/>
-        <v>973696.80951888952</v>
+        <v>784022.28451475967</v>
       </c>
       <c r="AU9" s="51"/>
       <c r="AV9" s="51"/>
@@ -31286,6 +31512,18 @@
       <c r="AG11" s="1">
         <v>1071603</v>
       </c>
+      <c r="AJ11" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>225</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="13" spans="2:88" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -31622,28 +31860,28 @@
         <v>1291804.5555555555</v>
       </c>
       <c r="AM15" s="1">
-        <v>1540409.4222222222</v>
+        <v>1679645.9222222222</v>
       </c>
       <c r="AN15" s="1">
-        <v>1413758.8555555556</v>
+        <v>1274522.3555555556</v>
       </c>
       <c r="AO15" s="1">
-        <v>1469368.1055555556</v>
+        <v>1188530.4222222222</v>
       </c>
       <c r="AP15" s="1">
-        <v>1723572.7422222223</v>
+        <v>1203106.7222222222</v>
       </c>
       <c r="AQ15" s="1">
-        <v>1488527.5755555555</v>
+        <v>1200041.6722222222</v>
       </c>
       <c r="AR15" s="1">
-        <v>1723705.0255555557</v>
+        <v>1413677.2222222222</v>
       </c>
       <c r="AS15" s="2">
-        <v>1499050.2755555557</v>
+        <v>1181576.4222222222</v>
       </c>
       <c r="AT15" s="2">
-        <v>1476931.5255555557</v>
+        <v>1221902.7222222222</v>
       </c>
       <c r="AU15" s="50"/>
       <c r="AV15" s="50"/>
@@ -31755,28 +31993,28 @@
         <v>1629741.0944444444</v>
       </c>
       <c r="AM16" s="1">
-        <v>1700996.5444444446</v>
+        <v>1821249.1444444444</v>
       </c>
       <c r="AN16" s="1">
-        <v>1756557.5444444444</v>
+        <v>1636304.9444444445</v>
       </c>
       <c r="AO16" s="1">
-        <v>1492038.9444444445</v>
+        <v>1044535.6418844444</v>
       </c>
       <c r="AP16" s="1">
-        <v>1733861.1544444445</v>
+        <v>1075201.4287444446</v>
       </c>
       <c r="AQ16" s="1">
-        <v>1646718.4669444445</v>
+        <v>967252.70044444443</v>
       </c>
       <c r="AR16" s="1">
-        <v>1852793.7169444445</v>
+        <v>1252894.5205444444</v>
       </c>
       <c r="AS16" s="1">
-        <v>1805138.2169444445</v>
+        <v>1094551.7718044445</v>
       </c>
       <c r="AT16" s="1">
-        <v>1686397.1169444444</v>
+        <v>1130369.3544444446</v>
       </c>
       <c r="AU16" s="49"/>
       <c r="AV16" s="49"/>
@@ -31885,31 +32123,31 @@
         <v>514037.93403995328</v>
       </c>
       <c r="AL17" s="1">
-        <v>640953.13403995335</v>
+        <v>623192.4</v>
       </c>
       <c r="AM17" s="1">
-        <v>563894.93403995328</v>
+        <v>579755.4</v>
       </c>
       <c r="AN17" s="1">
-        <v>740077.47403995332</v>
+        <v>688695.54</v>
       </c>
       <c r="AO17" s="1">
-        <v>656005.0740399533</v>
+        <v>476363.98687999998</v>
       </c>
       <c r="AP17" s="1">
-        <v>596976.64403995336</v>
+        <v>532577.0263399533</v>
       </c>
       <c r="AQ17" s="1">
-        <v>744181.66403995338</v>
+        <v>517392.18179995328</v>
       </c>
       <c r="AR17" s="1">
-        <v>726698.04403995327</v>
+        <v>649247.91843995336</v>
       </c>
       <c r="AS17" s="1">
-        <v>638852.29403995327</v>
+        <v>592436.3157999533</v>
       </c>
       <c r="AT17" s="1">
-        <v>775001.27403995325</v>
+        <v>798470.88403995335</v>
       </c>
       <c r="AU17" s="49"/>
       <c r="AV17" s="49"/>
@@ -32018,31 +32256,31 @@
         <v>1336375.9907409865</v>
       </c>
       <c r="AL18" s="1">
-        <v>1327642.1240743198</v>
+        <v>1297357.1666666667</v>
       </c>
       <c r="AM18" s="1">
-        <v>1302233.4574076533</v>
+        <v>1327321.8999999999</v>
       </c>
       <c r="AN18" s="1">
-        <v>1350224.30407432</v>
+        <v>1264565.9466666668</v>
       </c>
       <c r="AO18" s="1">
-        <v>1546046.2374076531</v>
+        <v>850374.00032000011</v>
       </c>
       <c r="AP18" s="1">
-        <v>1468179.6474076533</v>
+        <v>990270.68850765319</v>
       </c>
       <c r="AQ18" s="1">
-        <v>1479988.99407432</v>
+        <v>903844.84252765332</v>
       </c>
       <c r="AR18" s="1">
-        <v>1561592.6974076533</v>
+        <v>1154345.7561076533</v>
       </c>
       <c r="AS18" s="1">
-        <v>1567420.4474076533</v>
+        <v>1025090.7138876533</v>
       </c>
       <c r="AT18" s="1">
-        <v>1468939.4640743199</v>
+        <v>1200112.6074076532</v>
       </c>
       <c r="AU18" s="49"/>
       <c r="AV18" s="49"/>
@@ -32151,31 +32389,31 @@
         <v>825971.89056297007</v>
       </c>
       <c r="AL19" s="1">
-        <v>980242.89056297007</v>
+        <v>960171.9</v>
       </c>
       <c r="AM19" s="1">
-        <v>896160.14056297007</v>
+        <v>909213.55</v>
       </c>
       <c r="AN19" s="1">
-        <v>1000375.98056297</v>
+        <v>947180.59000000008</v>
       </c>
       <c r="AO19" s="1">
-        <v>885326.83056297014</v>
+        <v>600687.21696000011</v>
       </c>
       <c r="AP19" s="1">
-        <v>1029766.22056297</v>
+        <v>748847.42486297013</v>
       </c>
       <c r="AQ19" s="1">
-        <v>937220.71056297002</v>
+        <v>631752.25864297012</v>
       </c>
       <c r="AR19" s="1">
-        <v>1082043.5580629702</v>
+        <v>837467.34036297002</v>
       </c>
       <c r="AS19" s="1">
-        <v>949780.80806297006</v>
+        <v>673962.98136297008</v>
       </c>
       <c r="AT19" s="1">
-        <v>1060024.7705629701</v>
+        <v>859028.5405629701</v>
       </c>
       <c r="AU19" s="49"/>
       <c r="AV19" s="49"/>
@@ -32297,39 +32535,39 @@
       </c>
       <c r="AL20" s="1">
         <f t="shared" si="6"/>
-        <v>5870383.7986772433</v>
+        <v>5802267.1166666672</v>
       </c>
       <c r="AM20" s="1">
         <f t="shared" si="6"/>
-        <v>6003694.4986772435</v>
+        <v>6317185.916666666</v>
       </c>
       <c r="AN20" s="1">
         <f t="shared" si="6"/>
-        <v>6260994.1586772427</v>
+        <v>5811269.3766666669</v>
       </c>
       <c r="AO20" s="1">
         <f t="shared" si="6"/>
-        <v>6048785.1920105759</v>
+        <v>4160491.2682666667</v>
       </c>
       <c r="AP20" s="1">
         <f t="shared" si="6"/>
-        <v>6552356.4086772427</v>
+        <v>4550003.2906772438</v>
       </c>
       <c r="AQ20" s="1">
         <f t="shared" si="6"/>
-        <v>6296637.411177244</v>
+        <v>4220283.6556372438</v>
       </c>
       <c r="AR20" s="1">
         <f t="shared" si="6"/>
-        <v>6946833.0420105774</v>
+        <v>5307632.7576772431</v>
       </c>
       <c r="AS20" s="2">
         <f t="shared" si="6"/>
-        <v>6460242.0420105765</v>
+        <v>4567618.205077244</v>
       </c>
       <c r="AT20" s="2">
         <f t="shared" si="6"/>
-        <v>6467294.1511772433</v>
+        <v>5209884.1086772438</v>
       </c>
       <c r="AU20" s="48"/>
       <c r="AV20" s="48"/>
@@ -33384,39 +33622,39 @@
       </c>
       <c r="AL31" s="45">
         <f t="shared" si="7"/>
-        <v>1.7886643950743384E-2</v>
+        <v>1.7945292703201769E-2</v>
       </c>
       <c r="AM31" s="45">
         <f t="shared" si="7"/>
-        <v>1.6095656743944881E-2</v>
+        <v>1.6266333406931861E-2</v>
       </c>
       <c r="AN31" s="45">
         <f t="shared" si="7"/>
-        <v>1.7945530591252316E-2</v>
+        <v>1.7861524132220967E-2</v>
       </c>
       <c r="AO31" s="45">
         <f t="shared" si="7"/>
-        <v>1.5666173080232521E-2</v>
+        <v>1.6299729963241676E-2</v>
       </c>
       <c r="AP31" s="45">
         <f t="shared" si="7"/>
-        <v>1.8489783836860996E-2</v>
+        <v>1.8312949853171511E-2</v>
       </c>
       <c r="AQ31" s="45">
         <f t="shared" si="7"/>
-        <v>1.5633408925296598E-2</v>
+        <v>1.6138753755478991E-2</v>
       </c>
       <c r="AR31" s="45">
         <f t="shared" si="7"/>
-        <v>1.8229091052853162E-2</v>
+        <v>1.8301324051658102E-2</v>
       </c>
       <c r="AS31" s="45">
         <f t="shared" si="7"/>
-        <v>1.5709867022628953E-2</v>
+        <v>1.5812244489524521E-2</v>
       </c>
       <c r="AT31" s="45">
         <f t="shared" si="7"/>
-        <v>1.7879123781504903E-2</v>
+        <v>1.7639538124275805E-2</v>
       </c>
       <c r="AU31" s="44"/>
       <c r="AV31" s="44"/>
@@ -34363,39 +34601,39 @@
       </c>
       <c r="AL42" s="39">
         <f t="shared" si="8"/>
-        <v>8.3675008010355132</v>
+        <v>8.3635443233414062</v>
       </c>
       <c r="AM42" s="39">
         <f t="shared" si="8"/>
-        <v>7.6505060076706792</v>
+        <v>7.6521490852459415</v>
       </c>
       <c r="AN42" s="39">
         <f t="shared" si="8"/>
-        <v>8.3622993861916726</v>
+        <v>8.3487523970830857</v>
       </c>
       <c r="AO42" s="39">
         <f t="shared" si="8"/>
-        <v>7.7285373626158949</v>
+        <v>7.7569969094693567</v>
       </c>
       <c r="AP42" s="39">
         <f t="shared" si="8"/>
-        <v>8.4793532092894974</v>
+        <v>8.5375770868229814</v>
       </c>
       <c r="AQ42" s="39">
         <f t="shared" si="8"/>
-        <v>7.6690497976450427</v>
+        <v>7.8070650041718794</v>
       </c>
       <c r="AR42" s="39">
         <f t="shared" si="8"/>
-        <v>8.4452197773820252</v>
+        <v>8.5402743424211565</v>
       </c>
       <c r="AS42" s="39">
         <f t="shared" si="8"/>
-        <v>7.6306527565973568</v>
+        <v>7.7470154584602655</v>
       </c>
       <c r="AT42" s="39">
         <f t="shared" si="8"/>
-        <v>8.4208300310513202</v>
+        <v>8.531259157281621</v>
       </c>
       <c r="AU42" s="38"/>
       <c r="AV42" s="38"/>
@@ -34475,7 +34713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C64C10-4E6F-44D7-82F0-C0BD1E4B671D}">
   <dimension ref="B2:AT16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AJ3" sqref="AJ3:AJ8"/>
     </sheetView>
   </sheetViews>

</xml_diff>